<commit_message>
SNOW, JNJ, PFE updates
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77562CDE-809C-4BA1-A0D1-B0A981C37D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDB610-3763-4C7F-953B-ECC737BCA121}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12450" yWindow="0" windowWidth="16410" windowHeight="15000" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="10995" yWindow="1995" windowWidth="17760" windowHeight="13500" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="80">
   <si>
     <t>Main</t>
   </si>
@@ -222,6 +222,60 @@
   </si>
   <si>
     <t xml:space="preserve">  Electronics/General</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Inventories</t>
+  </si>
+  <si>
+    <t>PP&amp;E</t>
+  </si>
+  <si>
+    <t>Leases</t>
+  </si>
+  <si>
+    <t>Goodwill</t>
+  </si>
+  <si>
+    <t>OA</t>
+  </si>
+  <si>
+    <t>L+SE</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>OLTL</t>
+  </si>
+  <si>
+    <t>Net Cash</t>
+  </si>
+  <si>
+    <t>ROIC</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Terminal</t>
+  </si>
+  <si>
+    <t>NPV</t>
   </si>
 </sst>
 </file>
@@ -737,7 +791,7 @@
   <dimension ref="J2:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -802,9 +856,7 @@
         <f>K4-K5+K6</f>
         <v>1107384.3999999999</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="L7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -813,13 +865,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5282D4FF-6525-4291-9B79-B00D62C08099}">
-  <dimension ref="A1:BN66"/>
+  <dimension ref="A1:DN66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AL4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="AW16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ24" sqref="AQ24"/>
+      <selection pane="bottomRight" activeCell="BC44" sqref="BC44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1386,9 +1438,34 @@
       <c r="P10" s="4">
         <v>18441</v>
       </c>
-      <c r="Q10" s="4"/>
-      <c r="R10" s="4"/>
-      <c r="S10" s="4"/>
+      <c r="Q10" s="4">
+        <f>+M10*1.4</f>
+        <v>20732.599999999999</v>
+      </c>
+      <c r="R10" s="4">
+        <f t="shared" ref="R10:W10" si="3">+N10*1.4</f>
+        <v>22554</v>
+      </c>
+      <c r="S10" s="4">
+        <f t="shared" si="3"/>
+        <v>24892</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="3"/>
+        <v>25817.399999999998</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="3"/>
+        <v>29025.639999999996</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="3"/>
+        <v>31575.599999999999</v>
+      </c>
+      <c r="W10" s="4">
+        <f t="shared" si="3"/>
+        <v>34848.799999999996</v>
+      </c>
       <c r="AN10" s="17">
         <v>4644</v>
       </c>
@@ -1416,6 +1493,42 @@
         <f>SUM(L10:O10)</f>
         <v>62202</v>
       </c>
+      <c r="AV10" s="2">
+        <f>SUM(P10:S10)</f>
+        <v>86619.6</v>
+      </c>
+      <c r="AW10" s="2">
+        <f>SUM(T10:W10)</f>
+        <v>121267.43999999997</v>
+      </c>
+      <c r="AX10" s="2">
+        <f>+AW10*1.3</f>
+        <v>157647.67199999996</v>
+      </c>
+      <c r="AY10" s="2">
+        <f t="shared" ref="AY10:BA10" si="4">+AX10*1.3</f>
+        <v>204941.97359999997</v>
+      </c>
+      <c r="AZ10" s="2">
+        <f t="shared" si="4"/>
+        <v>266424.56567999994</v>
+      </c>
+      <c r="BA10" s="2">
+        <f t="shared" si="4"/>
+        <v>346351.93538399995</v>
+      </c>
+      <c r="BB10" s="2">
+        <f>+BA10*1.2</f>
+        <v>415622.32246079994</v>
+      </c>
+      <c r="BC10" s="2">
+        <f t="shared" ref="BC10:BD10" si="5">+BB10*1.2</f>
+        <v>498746.7869529599</v>
+      </c>
+      <c r="BD10" s="2">
+        <f t="shared" si="5"/>
+        <v>598496.14434355183</v>
+      </c>
     </row>
     <row r="12" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
@@ -1463,24 +1576,85 @@
       <c r="P12" s="4">
         <v>51129</v>
       </c>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="4"/>
-      <c r="S12" s="4"/>
+      <c r="Q12" s="4">
+        <f>+M12*1.1</f>
+        <v>58472.700000000004</v>
+      </c>
+      <c r="R12" s="4">
+        <f t="shared" ref="R12:W12" si="6">+N12*1.1</f>
+        <v>54936.200000000004</v>
+      </c>
+      <c r="S12" s="4">
+        <f t="shared" si="6"/>
+        <v>72682.5</v>
+      </c>
+      <c r="T12" s="4">
+        <f t="shared" si="6"/>
+        <v>56241.9</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="6"/>
+        <v>64319.970000000008</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="6"/>
+        <v>60429.820000000007</v>
+      </c>
+      <c r="W12" s="4">
+        <f t="shared" si="6"/>
+        <v>79950.75</v>
+      </c>
       <c r="AR12" s="2">
         <f>26939+27165+29061+39822</f>
         <v>122987</v>
       </c>
       <c r="AS12" s="2">
-        <f t="shared" ref="AS12:AS27" si="3">SUM(D12:G12)</f>
+        <f t="shared" ref="AS12:AS27" si="7">SUM(D12:G12)</f>
         <v>141247</v>
       </c>
       <c r="AT12" s="2">
-        <f t="shared" ref="AT12:AT17" si="4">SUM(H12:K12)</f>
+        <f t="shared" ref="AT12:AT17" si="8">SUM(H12:K12)</f>
         <v>197349</v>
       </c>
       <c r="AU12" s="2">
-        <f t="shared" ref="AU12:AU17" si="5">SUM(L12:O12)</f>
+        <f t="shared" ref="AU12:AU17" si="9">SUM(L12:O12)</f>
         <v>222075</v>
+      </c>
+      <c r="AV12" s="2">
+        <f>SUM(P12:S12)</f>
+        <v>237220.40000000002</v>
+      </c>
+      <c r="AW12" s="2">
+        <f>SUM(T12:W12)</f>
+        <v>260942.44</v>
+      </c>
+      <c r="AX12" s="2">
+        <f>+AW12*1.05</f>
+        <v>273989.56200000003</v>
+      </c>
+      <c r="AY12" s="2">
+        <f t="shared" ref="AY12:BD12" si="10">+AX12*1.05</f>
+        <v>287689.04010000004</v>
+      </c>
+      <c r="AZ12" s="2">
+        <f t="shared" si="10"/>
+        <v>302073.49210500007</v>
+      </c>
+      <c r="BA12" s="2">
+        <f t="shared" si="10"/>
+        <v>317177.16671025008</v>
+      </c>
+      <c r="BB12" s="2">
+        <f t="shared" si="10"/>
+        <v>333036.0250457626</v>
+      </c>
+      <c r="BC12" s="2">
+        <f t="shared" si="10"/>
+        <v>349687.82629805076</v>
+      </c>
+      <c r="BD12" s="2">
+        <f t="shared" si="10"/>
+        <v>367172.21761295333</v>
       </c>
     </row>
     <row r="13" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1529,24 +1703,85 @@
       <c r="P13" s="4">
         <v>4591</v>
       </c>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
-      <c r="S13" s="4"/>
+      <c r="Q13" s="4">
+        <f>+M13</f>
+        <v>4198</v>
+      </c>
+      <c r="R13" s="4">
+        <f>+N13</f>
+        <v>4269</v>
+      </c>
+      <c r="S13" s="4">
+        <f>+O13</f>
+        <v>4688</v>
+      </c>
+      <c r="T13" s="4">
+        <f>+P13</f>
+        <v>4591</v>
+      </c>
+      <c r="U13" s="4">
+        <f>+Q13</f>
+        <v>4198</v>
+      </c>
+      <c r="V13" s="4">
+        <f>+R13</f>
+        <v>4269</v>
+      </c>
+      <c r="W13" s="4">
+        <f>+S13</f>
+        <v>4688</v>
+      </c>
       <c r="AR13" s="2">
         <f>4263+4312+4248+4401</f>
         <v>17224</v>
       </c>
       <c r="AS13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>17192</v>
       </c>
       <c r="AT13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>16224</v>
       </c>
       <c r="AU13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>17075</v>
+      </c>
+      <c r="AV13" s="2">
+        <f>SUM(P13:S13)</f>
+        <v>17746</v>
+      </c>
+      <c r="AW13" s="2">
+        <f>SUM(T13:W13)</f>
+        <v>17746</v>
+      </c>
+      <c r="AX13" s="2">
+        <f t="shared" ref="AX13:BD13" si="11">+AW13*1.05</f>
+        <v>18633.3</v>
+      </c>
+      <c r="AY13" s="2">
+        <f t="shared" si="11"/>
+        <v>19564.965</v>
+      </c>
+      <c r="AZ13" s="2">
+        <f t="shared" si="11"/>
+        <v>20543.213250000001</v>
+      </c>
+      <c r="BA13" s="2">
+        <f t="shared" si="11"/>
+        <v>21570.373912500003</v>
+      </c>
+      <c r="BB13" s="2">
+        <f t="shared" si="11"/>
+        <v>22648.892608125003</v>
+      </c>
+      <c r="BC13" s="2">
+        <f t="shared" si="11"/>
+        <v>23781.337238531254</v>
+      </c>
+      <c r="BD13" s="2">
+        <f t="shared" si="11"/>
+        <v>24970.404100457818</v>
       </c>
     </row>
     <row r="14" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1595,24 +1830,85 @@
       <c r="P14" s="4">
         <v>25335</v>
       </c>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
+      <c r="Q14" s="4">
+        <f>+M14*1.2</f>
+        <v>30102</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" ref="R14:W14" si="12">+N14*1.2</f>
+        <v>29102.399999999998</v>
+      </c>
+      <c r="S14" s="4">
+        <f t="shared" si="12"/>
+        <v>36384</v>
+      </c>
+      <c r="T14" s="4">
+        <f t="shared" si="12"/>
+        <v>30402</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="12"/>
+        <v>36122.400000000001</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="12"/>
+        <v>34922.879999999997</v>
+      </c>
+      <c r="W14" s="4">
+        <f t="shared" si="12"/>
+        <v>43660.799999999996</v>
+      </c>
       <c r="AR14" s="2">
         <f>9265+9702+10395+13383</f>
         <v>42745</v>
       </c>
       <c r="AS14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>53761</v>
       </c>
       <c r="AT14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>80437</v>
       </c>
       <c r="AU14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>103366</v>
+      </c>
+      <c r="AV14" s="2">
+        <f>SUM(P14:S14)</f>
+        <v>120923.4</v>
+      </c>
+      <c r="AW14" s="2">
+        <f>SUM(T14:W14)</f>
+        <v>145108.07999999999</v>
+      </c>
+      <c r="AX14" s="2">
+        <f t="shared" ref="AX14:BD14" si="13">+AW14*1.05</f>
+        <v>152363.484</v>
+      </c>
+      <c r="AY14" s="2">
+        <f t="shared" si="13"/>
+        <v>159981.65820000001</v>
+      </c>
+      <c r="AZ14" s="2">
+        <f t="shared" si="13"/>
+        <v>167980.74111</v>
+      </c>
+      <c r="BA14" s="2">
+        <f t="shared" si="13"/>
+        <v>176379.7781655</v>
+      </c>
+      <c r="BB14" s="2">
+        <f t="shared" si="13"/>
+        <v>185198.767073775</v>
+      </c>
+      <c r="BC14" s="2">
+        <f t="shared" si="13"/>
+        <v>194458.70542746375</v>
+      </c>
+      <c r="BD14" s="2">
+        <f t="shared" si="13"/>
+        <v>204181.64069883694</v>
       </c>
     </row>
     <row r="15" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1661,24 +1957,85 @@
       <c r="P15" s="4">
         <v>8410</v>
       </c>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
-      <c r="S15" s="4"/>
+      <c r="Q15" s="4">
+        <f t="shared" ref="Q15:Q16" si="14">+M15*1.2</f>
+        <v>9500.4</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" ref="R15:R16" si="15">+N15*1.2</f>
+        <v>9777.6</v>
+      </c>
+      <c r="S15" s="4">
+        <f t="shared" ref="S15:S16" si="16">+O15*1.2</f>
+        <v>9747.6</v>
+      </c>
+      <c r="T15" s="4">
+        <f t="shared" ref="T15:T16" si="17">+P15*1.2</f>
+        <v>10092</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" ref="U15:U16" si="18">+Q15*1.2</f>
+        <v>11400.48</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" ref="V15:V16" si="19">+R15*1.2</f>
+        <v>11733.12</v>
+      </c>
+      <c r="W15" s="4">
+        <f t="shared" ref="W15:W16" si="20">+S15*1.2</f>
+        <v>11697.12</v>
+      </c>
       <c r="AR15" s="2">
         <f>3102+3408+3698+3959</f>
         <v>14167</v>
       </c>
       <c r="AS15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>19210</v>
       </c>
       <c r="AT15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>25207</v>
       </c>
       <c r="AU15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>31768</v>
+      </c>
+      <c r="AV15" s="2">
+        <f>SUM(P15:S15)</f>
+        <v>37435.599999999999</v>
+      </c>
+      <c r="AW15" s="2">
+        <f>SUM(T15:W15)</f>
+        <v>44922.720000000001</v>
+      </c>
+      <c r="AX15" s="2">
+        <f>+AW15*1.1</f>
+        <v>49414.992000000006</v>
+      </c>
+      <c r="AY15" s="2">
+        <f t="shared" ref="AY15:BA15" si="21">+AX15*1.1</f>
+        <v>54356.491200000011</v>
+      </c>
+      <c r="AZ15" s="2">
+        <f t="shared" si="21"/>
+        <v>59792.14032000002</v>
+      </c>
+      <c r="BA15" s="2">
+        <f t="shared" si="21"/>
+        <v>65771.354352000024</v>
+      </c>
+      <c r="BB15" s="2">
+        <f t="shared" ref="AX15:BD15" si="22">+BA15*1.05</f>
+        <v>69059.922069600027</v>
+      </c>
+      <c r="BC15" s="2">
+        <f t="shared" si="22"/>
+        <v>72512.918173080034</v>
+      </c>
+      <c r="BD15" s="2">
+        <f t="shared" si="22"/>
+        <v>76138.564081734032</v>
       </c>
     </row>
     <row r="16" spans="1:66" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1727,27 +2084,88 @@
       <c r="P16" s="4">
         <v>7877</v>
       </c>
-      <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
+      <c r="Q16" s="4">
+        <f t="shared" si="14"/>
+        <v>8941.1999999999989</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="15"/>
+        <v>9134.4</v>
+      </c>
+      <c r="S16" s="4">
+        <f t="shared" si="16"/>
+        <v>11659.199999999999</v>
+      </c>
+      <c r="T16" s="4">
+        <f t="shared" si="17"/>
+        <v>9452.4</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="18"/>
+        <v>10729.439999999999</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="19"/>
+        <v>10961.279999999999</v>
+      </c>
+      <c r="W16" s="4">
+        <f t="shared" si="20"/>
+        <v>13991.039999999999</v>
+      </c>
       <c r="AR16" s="2">
         <f>2031+2194+2495+3388</f>
         <v>10108</v>
       </c>
       <c r="AS16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>14086</v>
       </c>
       <c r="AT16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20875</v>
       </c>
       <c r="AU16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>31160</v>
       </c>
-    </row>
-    <row r="17" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV16" s="2">
+        <f>SUM(P16:S16)</f>
+        <v>37611.799999999996</v>
+      </c>
+      <c r="AW16" s="2">
+        <f>SUM(T16:W16)</f>
+        <v>45134.159999999996</v>
+      </c>
+      <c r="AX16" s="2">
+        <f t="shared" ref="AX16:BA16" si="23">+AW16*1.1</f>
+        <v>49647.576000000001</v>
+      </c>
+      <c r="AY16" s="2">
+        <f t="shared" si="23"/>
+        <v>54612.333600000005</v>
+      </c>
+      <c r="AZ16" s="2">
+        <f t="shared" si="23"/>
+        <v>60073.566960000011</v>
+      </c>
+      <c r="BA16" s="2">
+        <f t="shared" si="23"/>
+        <v>66080.923656000014</v>
+      </c>
+      <c r="BB16" s="2">
+        <f t="shared" ref="AX16:BD16" si="24">+BA16*1.05</f>
+        <v>69384.969838800011</v>
+      </c>
+      <c r="BC16" s="2">
+        <f t="shared" si="24"/>
+        <v>72854.218330740012</v>
+      </c>
+      <c r="BD16" s="2">
+        <f t="shared" si="24"/>
+        <v>76496.929247277018</v>
+      </c>
+    </row>
+    <row r="17" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
@@ -1791,23 +2209,88 @@
       <c r="P17" s="4">
         <v>661</v>
       </c>
-      <c r="Q17" s="4"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
+      <c r="Q17" s="4">
+        <f>+M17</f>
+        <v>463</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" ref="R17:W17" si="25">+N17</f>
+        <v>479</v>
+      </c>
+      <c r="S17" s="4">
+        <f t="shared" si="25"/>
+        <v>710</v>
+      </c>
+      <c r="T17" s="4">
+        <f t="shared" si="25"/>
+        <v>661</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="25"/>
+        <v>463</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="25"/>
+        <v>479</v>
+      </c>
+      <c r="W17" s="4">
+        <f t="shared" si="25"/>
+        <v>710</v>
+      </c>
       <c r="AS17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AT17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>602</v>
       </c>
       <c r="AU17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>2176</v>
       </c>
-    </row>
-    <row r="19" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV17" s="2">
+        <f>SUM(P17:S17)</f>
+        <v>2313</v>
+      </c>
+      <c r="AW17" s="2">
+        <f>SUM(T17:W17)</f>
+        <v>2313</v>
+      </c>
+      <c r="AX17" s="2">
+        <f t="shared" ref="AX17:BD17" si="26">+AW17*1.05</f>
+        <v>2428.65</v>
+      </c>
+      <c r="AY17" s="2">
+        <f t="shared" si="26"/>
+        <v>2550.0825</v>
+      </c>
+      <c r="AZ17" s="2">
+        <f t="shared" si="26"/>
+        <v>2677.5866249999999</v>
+      </c>
+      <c r="BA17" s="2">
+        <f t="shared" si="26"/>
+        <v>2811.4659562500001</v>
+      </c>
+      <c r="BB17" s="2">
+        <f t="shared" si="26"/>
+        <v>2952.0392540625003</v>
+      </c>
+      <c r="BC17" s="2">
+        <f t="shared" si="26"/>
+        <v>3099.6412167656254</v>
+      </c>
+      <c r="BD17" s="2">
+        <f t="shared" si="26"/>
+        <v>3254.6232776039069</v>
+      </c>
+    </row>
+    <row r="18" spans="2:56" x14ac:dyDescent="0.2">
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+    </row>
+    <row r="19" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
@@ -1863,7 +2346,7 @@
         <v>141915</v>
       </c>
       <c r="AS19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>160407</v>
       </c>
       <c r="AT19" s="2">
@@ -1871,11 +2354,11 @@
         <v>215915</v>
       </c>
       <c r="AU19" s="2">
-        <f t="shared" ref="AU19:AU27" si="6">SUM(L19:O19)</f>
+        <f t="shared" ref="AU19:AU27" si="27">SUM(L19:O19)</f>
         <v>241787</v>
       </c>
     </row>
-    <row r="20" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1931,72 +2414,72 @@
         <v>90972</v>
       </c>
       <c r="AS20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>120115</v>
       </c>
       <c r="AT20" s="2">
-        <f t="shared" ref="AT20:AT27" si="7">SUM(H20:K20)</f>
+        <f t="shared" ref="AT20:AT27" si="28">SUM(H20:K20)</f>
         <v>170149</v>
       </c>
       <c r="AU20" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>228035</v>
       </c>
     </row>
-    <row r="21" spans="2:47" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:56" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="6">
-        <f t="shared" ref="C21:D21" si="8">C19+C20</f>
+        <f t="shared" ref="C21" si="29">C19+C20</f>
         <v>72383</v>
       </c>
       <c r="D21" s="6">
-        <f t="shared" ref="D21:F21" si="9">D19+D20</f>
+        <f t="shared" ref="D21:F21" si="30">D19+D20</f>
         <v>59700</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" ref="E21:F21" si="10">E19+E20</f>
+        <f t="shared" ref="E21" si="31">E19+E20</f>
         <v>63404</v>
       </c>
       <c r="F21" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="30"/>
         <v>69981</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" ref="G21" si="11">G19+G20</f>
+        <f t="shared" ref="G21" si="32">G19+G20</f>
         <v>87437</v>
       </c>
       <c r="H21" s="6">
-        <f t="shared" ref="H21:I21" si="12">H19+H20</f>
+        <f t="shared" ref="H21" si="33">H19+H20</f>
         <v>75452</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" ref="I21:J21" si="13">I19+I20</f>
+        <f t="shared" ref="I21" si="34">I19+I20</f>
         <v>88912</v>
       </c>
       <c r="J21" s="6">
-        <f t="shared" ref="J21:O21" si="14">J19+J20</f>
+        <f t="shared" ref="J21:O21" si="35">J19+J20</f>
         <v>96145</v>
       </c>
       <c r="K21" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="35"/>
         <v>125555</v>
       </c>
       <c r="L21" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="35"/>
         <v>108518</v>
       </c>
       <c r="M21" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="35"/>
         <v>113080</v>
       </c>
       <c r="N21" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="35"/>
         <v>110812</v>
       </c>
       <c r="O21" s="6">
-        <f t="shared" si="14"/>
+        <f t="shared" si="35"/>
         <v>137412</v>
       </c>
       <c r="P21" s="6">
@@ -2004,32 +2487,32 @@
         <v>116444</v>
       </c>
       <c r="Q21" s="6">
-        <f t="shared" ref="Q21:S21" si="15">Q19+Q20</f>
-        <v>0</v>
+        <f>SUM(Q10:Q17)</f>
+        <v>132409.9</v>
       </c>
       <c r="R21" s="6">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" ref="R21:W21" si="36">SUM(R10:R17)</f>
+        <v>130252.6</v>
       </c>
       <c r="S21" s="6">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>160763.30000000002</v>
       </c>
       <c r="T21" s="6">
-        <f t="shared" ref="T21" si="16">T19+T20</f>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>137257.70000000001</v>
       </c>
       <c r="U21" s="6">
-        <f t="shared" ref="U21" si="17">U19+U20</f>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>156258.93000000002</v>
       </c>
       <c r="V21" s="6">
-        <f t="shared" ref="V21" si="18">V19+V20</f>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>154370.70000000001</v>
       </c>
       <c r="W21" s="6">
-        <f t="shared" ref="W21" si="19">W19+W20</f>
-        <v>0</v>
+        <f t="shared" si="36"/>
+        <v>189546.50999999998</v>
       </c>
       <c r="AL21" s="5">
         <v>61093</v>
@@ -2042,19 +2525,19 @@
         <v>88988</v>
       </c>
       <c r="AO21" s="5">
-        <f t="shared" ref="AO21:AP21" si="20">+AO4+AO7+AO10</f>
+        <f t="shared" ref="AO21:AP21" si="37">+AO4+AO7+AO10</f>
         <v>107006</v>
       </c>
       <c r="AP21" s="5">
-        <f t="shared" si="20"/>
+        <f t="shared" si="37"/>
         <v>135987</v>
       </c>
       <c r="AQ21" s="6">
-        <f t="shared" ref="AQ21" si="21">AQ19+AQ20</f>
+        <f t="shared" ref="AQ21" si="38">AQ19+AQ20</f>
         <v>177866</v>
       </c>
       <c r="AR21" s="6">
-        <f t="shared" ref="AR21" si="22">AR19+AR20</f>
+        <f t="shared" ref="AR21" si="39">AR19+AR20</f>
         <v>232887</v>
       </c>
       <c r="AS21" s="6">
@@ -2069,8 +2552,44 @@
         <f>AU19+AU20</f>
         <v>469822</v>
       </c>
-    </row>
-    <row r="22" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV21" s="5">
+        <f>SUM(AV10:AV17)</f>
+        <v>539869.80000000005</v>
+      </c>
+      <c r="AW21" s="5">
+        <f>SUM(AW10:AW17)</f>
+        <v>637433.84</v>
+      </c>
+      <c r="AX21" s="5">
+        <f t="shared" ref="AX21:BD21" si="40">SUM(AX10:AX17)</f>
+        <v>704125.23599999992</v>
+      </c>
+      <c r="AY21" s="5">
+        <f t="shared" si="40"/>
+        <v>783696.54420000012</v>
+      </c>
+      <c r="AZ21" s="5">
+        <f t="shared" si="40"/>
+        <v>879565.30605000001</v>
+      </c>
+      <c r="BA21" s="5">
+        <f t="shared" si="40"/>
+        <v>996142.99813650013</v>
+      </c>
+      <c r="BB21" s="5">
+        <f t="shared" si="40"/>
+        <v>1097902.938350925</v>
+      </c>
+      <c r="BC21" s="5">
+        <f t="shared" si="40"/>
+        <v>1215141.4336375913</v>
+      </c>
+      <c r="BD21" s="5">
+        <f t="shared" si="40"/>
+        <v>1350710.5233624149</v>
+      </c>
+    </row>
+    <row r="22" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
@@ -2116,9 +2635,34 @@
       <c r="P22" s="4">
         <v>66499</v>
       </c>
-      <c r="Q22" s="4"/>
-      <c r="R22" s="4"/>
-      <c r="S22" s="4"/>
+      <c r="Q22" s="4">
+        <f>SUM(Q12:Q14)*0.8+Q10*0.7</f>
+        <v>88730.98000000001</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" ref="R22:W22" si="41">SUM(R12:R14)*0.8+R10*0.7</f>
+        <v>86433.88</v>
+      </c>
+      <c r="S22" s="4">
+        <f t="shared" si="41"/>
+        <v>108428</v>
+      </c>
+      <c r="T22" s="4">
+        <f t="shared" si="41"/>
+        <v>91060.099999999991</v>
+      </c>
+      <c r="U22" s="4">
+        <f t="shared" si="41"/>
+        <v>104030.24400000001</v>
+      </c>
+      <c r="V22" s="4">
+        <f t="shared" si="41"/>
+        <v>101800.28000000001</v>
+      </c>
+      <c r="W22" s="4">
+        <f t="shared" si="41"/>
+        <v>127033.79999999999</v>
+      </c>
       <c r="AN22" s="2">
         <v>62752</v>
       </c>
@@ -2135,19 +2679,55 @@
         <v>139156</v>
       </c>
       <c r="AS22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>165536</v>
       </c>
       <c r="AT22" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="28"/>
         <v>233307</v>
       </c>
       <c r="AU22" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>272344</v>
       </c>
-    </row>
-    <row r="23" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV22" s="17">
+        <f>SUM(P22:S22)</f>
+        <v>350091.86</v>
+      </c>
+      <c r="AW22" s="17">
+        <f>SUM(T22:W22)</f>
+        <v>423924.424</v>
+      </c>
+      <c r="AX22" s="4">
+        <f t="shared" ref="AX22:BD22" si="42">SUM(AX12:AX14)*0.8+AX10*0.7</f>
+        <v>466342.4472</v>
+      </c>
+      <c r="AY22" s="4">
+        <f t="shared" si="42"/>
+        <v>517247.91216000007</v>
+      </c>
+      <c r="AZ22" s="4">
+        <f t="shared" si="42"/>
+        <v>578975.15314800001</v>
+      </c>
+      <c r="BA22" s="4">
+        <f t="shared" si="42"/>
+        <v>654548.20979940007</v>
+      </c>
+      <c r="BB22" s="4">
+        <f t="shared" si="42"/>
+        <v>723642.57350469008</v>
+      </c>
+      <c r="BC22" s="4">
+        <f t="shared" si="42"/>
+        <v>803465.04603830853</v>
+      </c>
+      <c r="BD22" s="4">
+        <f t="shared" si="42"/>
+        <v>896006.71097028488</v>
+      </c>
+    </row>
+    <row r="23" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
@@ -2193,9 +2773,34 @@
       <c r="P23" s="4">
         <v>20271</v>
       </c>
-      <c r="Q23" s="4"/>
-      <c r="R23" s="4"/>
-      <c r="S23" s="4"/>
+      <c r="Q23" s="4">
+        <f>(Q14+Q12)*0.1</f>
+        <v>8857.4700000000012</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" ref="R23:W23" si="43">(R14+R12)*0.1</f>
+        <v>8403.86</v>
+      </c>
+      <c r="S23" s="4">
+        <f t="shared" si="43"/>
+        <v>10906.650000000001</v>
+      </c>
+      <c r="T23" s="4">
+        <f t="shared" si="43"/>
+        <v>8664.39</v>
+      </c>
+      <c r="U23" s="4">
+        <f t="shared" si="43"/>
+        <v>10044.237000000001</v>
+      </c>
+      <c r="V23" s="4">
+        <f t="shared" si="43"/>
+        <v>9535.2700000000023</v>
+      </c>
+      <c r="W23" s="4">
+        <f t="shared" si="43"/>
+        <v>12361.154999999999</v>
+      </c>
       <c r="AN23" s="2">
         <v>10766</v>
       </c>
@@ -2212,24 +2817,60 @@
         <v>34027</v>
       </c>
       <c r="AS23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>40231</v>
       </c>
       <c r="AT23" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="28"/>
         <v>58516</v>
       </c>
       <c r="AU23" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>75111</v>
       </c>
-    </row>
-    <row r="24" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV23" s="17">
+        <f>SUM(P23:S23)</f>
+        <v>48438.98</v>
+      </c>
+      <c r="AW23" s="17">
+        <f>SUM(T23:W23)</f>
+        <v>40605.052000000003</v>
+      </c>
+      <c r="AX23" s="4">
+        <f t="shared" ref="AX23:BD23" si="44">(AX14+AX12)*0.1</f>
+        <v>42635.304600000003</v>
+      </c>
+      <c r="AY23" s="4">
+        <f t="shared" si="44"/>
+        <v>44767.069830000008</v>
+      </c>
+      <c r="AZ23" s="4">
+        <f t="shared" si="44"/>
+        <v>47005.423321500013</v>
+      </c>
+      <c r="BA23" s="4">
+        <f t="shared" si="44"/>
+        <v>49355.694487575012</v>
+      </c>
+      <c r="BB23" s="4">
+        <f t="shared" si="44"/>
+        <v>51823.47921195376</v>
+      </c>
+      <c r="BC23" s="4">
+        <f t="shared" si="44"/>
+        <v>54414.653172551451</v>
+      </c>
+      <c r="BD23" s="4">
+        <f t="shared" si="44"/>
+        <v>57135.385831179032</v>
+      </c>
+    </row>
+    <row r="24" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="4">
-        <f t="shared" ref="C24" si="23">C21-C22-C23</f>
+        <f t="shared" ref="C24" si="45">C21-C22-C23</f>
         <v>17569</v>
       </c>
       <c r="D24" s="4">
@@ -2237,7 +2878,7 @@
         <v>17179</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" ref="E24" si="24">E21-E22-E23</f>
+        <f t="shared" ref="E24" si="46">E21-E22-E23</f>
         <v>17796</v>
       </c>
       <c r="F24" s="4">
@@ -2245,15 +2886,15 @@
         <v>18512</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" ref="G24" si="25">G21-G22-G23</f>
+        <f t="shared" ref="G24" si="47">G21-G22-G23</f>
         <v>21268</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" ref="H24" si="26">H21-H22-H23</f>
+        <f t="shared" ref="H24" si="48">H21-H22-H23</f>
         <v>19664</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" ref="I24" si="27">I21-I22-I23</f>
+        <f t="shared" ref="I24" si="49">I21-I22-I23</f>
         <v>22446</v>
       </c>
       <c r="J24" s="4">
@@ -2261,7 +2902,7 @@
         <v>24334</v>
       </c>
       <c r="K24" s="4">
-        <f t="shared" ref="K24" si="28">K21-K22-K23</f>
+        <f t="shared" ref="K24" si="50">K21-K22-K23</f>
         <v>27797</v>
       </c>
       <c r="L24" s="4">
@@ -2269,58 +2910,119 @@
         <v>29585</v>
       </c>
       <c r="M24" s="4">
-        <f t="shared" ref="M24:P24" si="29">M21-M22-M23</f>
+        <f t="shared" ref="M24:W24" si="51">M21-M22-M23</f>
         <v>31266</v>
       </c>
       <c r="N24" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="51"/>
         <v>29384</v>
       </c>
       <c r="O24" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="51"/>
         <v>32132</v>
       </c>
       <c r="P24" s="4">
-        <f t="shared" si="29"/>
+        <f t="shared" si="51"/>
         <v>29674</v>
       </c>
-      <c r="Q24" s="4"/>
-      <c r="R24" s="4"/>
-      <c r="S24" s="4"/>
+      <c r="Q24" s="4">
+        <f t="shared" si="51"/>
+        <v>34821.449999999983</v>
+      </c>
+      <c r="R24" s="4">
+        <f t="shared" si="51"/>
+        <v>35414.86</v>
+      </c>
+      <c r="S24" s="4">
+        <f t="shared" si="51"/>
+        <v>41428.650000000016</v>
+      </c>
+      <c r="T24" s="4">
+        <f t="shared" si="51"/>
+        <v>37533.210000000021</v>
+      </c>
+      <c r="U24" s="4">
+        <f t="shared" si="51"/>
+        <v>42184.449000000015</v>
+      </c>
+      <c r="V24" s="4">
+        <f t="shared" si="51"/>
+        <v>43035.149999999994</v>
+      </c>
+      <c r="W24" s="4">
+        <f t="shared" si="51"/>
+        <v>50151.554999999993</v>
+      </c>
       <c r="AN24" s="4">
-        <f t="shared" ref="AN24:AR24" si="30">AN21-AN22-AN23</f>
+        <f t="shared" ref="AN24:AQ24" si="52">AN21-AN22-AN23</f>
         <v>15470</v>
       </c>
       <c r="AO24" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="52"/>
         <v>21945</v>
       </c>
       <c r="AP24" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="52"/>
         <v>30103</v>
       </c>
       <c r="AQ24" s="4">
-        <f t="shared" si="30"/>
+        <f t="shared" si="52"/>
         <v>40683</v>
       </c>
       <c r="AR24" s="4">
-        <f t="shared" ref="AR24:AT24" si="31">AR21-AR22-AR23</f>
+        <f t="shared" ref="AR24:AS24" si="53">AR21-AR22-AR23</f>
         <v>59704</v>
       </c>
       <c r="AS24" s="4">
-        <f t="shared" si="31"/>
+        <f t="shared" si="53"/>
         <v>74755</v>
       </c>
       <c r="AT24" s="4">
-        <f t="shared" ref="AT24:AU24" si="32">AT21-AT22-AT23</f>
+        <f t="shared" ref="AT24:BD24" si="54">AT21-AT22-AT23</f>
         <v>94241</v>
       </c>
       <c r="AU24" s="4">
-        <f t="shared" si="32"/>
+        <f t="shared" si="54"/>
         <v>122367</v>
       </c>
-    </row>
-    <row r="25" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV24" s="4">
+        <f t="shared" si="54"/>
+        <v>141338.96000000005</v>
+      </c>
+      <c r="AW24" s="4">
+        <f t="shared" si="54"/>
+        <v>172904.36399999997</v>
+      </c>
+      <c r="AX24" s="4">
+        <f t="shared" si="54"/>
+        <v>195147.48419999992</v>
+      </c>
+      <c r="AY24" s="4">
+        <f t="shared" si="54"/>
+        <v>221681.56221000006</v>
+      </c>
+      <c r="AZ24" s="4">
+        <f t="shared" si="54"/>
+        <v>253584.72958049999</v>
+      </c>
+      <c r="BA24" s="4">
+        <f t="shared" si="54"/>
+        <v>292239.09384952503</v>
+      </c>
+      <c r="BB24" s="4">
+        <f t="shared" si="54"/>
+        <v>322436.88563428115</v>
+      </c>
+      <c r="BC24" s="4">
+        <f t="shared" si="54"/>
+        <v>357261.73442673136</v>
+      </c>
+      <c r="BD24" s="4">
+        <f t="shared" si="54"/>
+        <v>397568.42656095099</v>
+      </c>
+    </row>
+    <row r="25" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
@@ -2366,9 +3068,34 @@
       <c r="P25" s="4">
         <v>14842</v>
       </c>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
+      <c r="Q25" s="4">
+        <f>+M25*1.1</f>
+        <v>15258.1</v>
+      </c>
+      <c r="R25" s="4">
+        <f t="shared" ref="R25:W25" si="55">+N25*1.1</f>
+        <v>15818.000000000002</v>
+      </c>
+      <c r="S25" s="4">
+        <f t="shared" si="55"/>
+        <v>16844.300000000003</v>
+      </c>
+      <c r="T25" s="4">
+        <f t="shared" si="55"/>
+        <v>16326.2</v>
+      </c>
+      <c r="U25" s="4">
+        <f t="shared" si="55"/>
+        <v>16783.910000000003</v>
+      </c>
+      <c r="V25" s="4">
+        <f t="shared" si="55"/>
+        <v>17399.800000000003</v>
+      </c>
+      <c r="W25" s="4">
+        <f t="shared" si="55"/>
+        <v>18528.730000000003</v>
+      </c>
       <c r="AN25" s="2">
         <v>9275</v>
       </c>
@@ -2385,19 +3112,55 @@
         <v>28837</v>
       </c>
       <c r="AS25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>35932</v>
       </c>
       <c r="AT25" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="28"/>
         <v>42738</v>
       </c>
       <c r="AU25" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>56052</v>
       </c>
-    </row>
-    <row r="26" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV25" s="17">
+        <f>SUM(P25:S25)</f>
+        <v>62762.400000000001</v>
+      </c>
+      <c r="AW25" s="17">
+        <f>SUM(T25:W25)</f>
+        <v>69038.640000000014</v>
+      </c>
+      <c r="AX25" s="2">
+        <f>+AW25*1.03</f>
+        <v>71109.799200000023</v>
+      </c>
+      <c r="AY25" s="2">
+        <f t="shared" ref="AY25:BD25" si="56">+AX25*1.03</f>
+        <v>73243.093176000024</v>
+      </c>
+      <c r="AZ25" s="2">
+        <f t="shared" si="56"/>
+        <v>75440.385971280033</v>
+      </c>
+      <c r="BA25" s="2">
+        <f t="shared" si="56"/>
+        <v>77703.597550418432</v>
+      </c>
+      <c r="BB25" s="2">
+        <f t="shared" si="56"/>
+        <v>80034.705476930991</v>
+      </c>
+      <c r="BC25" s="2">
+        <f t="shared" si="56"/>
+        <v>82435.746641238919</v>
+      </c>
+      <c r="BD25" s="2">
+        <f t="shared" si="56"/>
+        <v>84908.819040476083</v>
+      </c>
+    </row>
+    <row r="26" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
@@ -2443,9 +3206,34 @@
       <c r="P26" s="4">
         <v>8320</v>
       </c>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="4"/>
+      <c r="Q26" s="4">
+        <f>+M26*1.05</f>
+        <v>7900.2000000000007</v>
+      </c>
+      <c r="R26" s="4">
+        <f t="shared" ref="R26:R27" si="57">+N26*1.05</f>
+        <v>8410.5</v>
+      </c>
+      <c r="S26" s="4">
+        <f t="shared" ref="S26:S27" si="58">+O26*1.05</f>
+        <v>11350.5</v>
+      </c>
+      <c r="T26" s="4">
+        <f t="shared" ref="T26:T27" si="59">+P26*1.05</f>
+        <v>8736</v>
+      </c>
+      <c r="U26" s="4">
+        <f t="shared" ref="U26:U27" si="60">+Q26*1.05</f>
+        <v>8295.2100000000009</v>
+      </c>
+      <c r="V26" s="4">
+        <f t="shared" ref="V26:V27" si="61">+R26*1.05</f>
+        <v>8831.0249999999996</v>
+      </c>
+      <c r="W26" s="4">
+        <f t="shared" ref="W26:W27" si="62">+S26*1.05</f>
+        <v>11918.025</v>
+      </c>
       <c r="AN26" s="2">
         <v>4332</v>
       </c>
@@ -2462,19 +3250,55 @@
         <v>13814</v>
       </c>
       <c r="AS26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>18879</v>
       </c>
       <c r="AT26" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="28"/>
         <v>22010</v>
       </c>
       <c r="AU26" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>32551</v>
       </c>
-    </row>
-    <row r="27" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV26" s="17">
+        <f>SUM(P26:S26)</f>
+        <v>35981.199999999997</v>
+      </c>
+      <c r="AW26" s="17">
+        <f>SUM(T26:W26)</f>
+        <v>37780.26</v>
+      </c>
+      <c r="AX26" s="2">
+        <f t="shared" ref="AX26:BD26" si="63">+AW26*1.03</f>
+        <v>38913.667800000003</v>
+      </c>
+      <c r="AY26" s="2">
+        <f t="shared" si="63"/>
+        <v>40081.077834000003</v>
+      </c>
+      <c r="AZ26" s="2">
+        <f t="shared" si="63"/>
+        <v>41283.510169020003</v>
+      </c>
+      <c r="BA26" s="2">
+        <f t="shared" si="63"/>
+        <v>42522.015474090607</v>
+      </c>
+      <c r="BB26" s="2">
+        <f t="shared" si="63"/>
+        <v>43797.675938313325</v>
+      </c>
+      <c r="BC26" s="2">
+        <f t="shared" si="63"/>
+        <v>45111.606216462729</v>
+      </c>
+      <c r="BD26" s="2">
+        <f t="shared" si="63"/>
+        <v>46464.95440295661</v>
+      </c>
+    </row>
+    <row r="27" spans="2:56" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
@@ -2520,6 +3344,34 @@
       <c r="P27" s="4">
         <v>2594</v>
       </c>
+      <c r="Q27" s="4">
+        <f t="shared" ref="Q27" si="64">+M27*1.05</f>
+        <v>2265.9</v>
+      </c>
+      <c r="R27" s="4">
+        <f t="shared" si="57"/>
+        <v>2260.65</v>
+      </c>
+      <c r="S27" s="4">
+        <f t="shared" si="58"/>
+        <v>2651.25</v>
+      </c>
+      <c r="T27" s="4">
+        <f t="shared" si="59"/>
+        <v>2723.7000000000003</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="60"/>
+        <v>2379.1950000000002</v>
+      </c>
+      <c r="V27" s="4">
+        <f t="shared" si="61"/>
+        <v>2373.6825000000003</v>
+      </c>
+      <c r="W27" s="4">
+        <f t="shared" si="62"/>
+        <v>2783.8125</v>
+      </c>
       <c r="AN27" s="2">
         <v>1552</v>
       </c>
@@ -2536,24 +3388,60 @@
         <v>4336</v>
       </c>
       <c r="AS27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>5203</v>
       </c>
       <c r="AT27" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="28"/>
         <v>6668</v>
       </c>
       <c r="AU27" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="27"/>
         <v>8823</v>
       </c>
-    </row>
-    <row r="28" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV27" s="17">
+        <f>SUM(P27:S27)</f>
+        <v>9771.7999999999993</v>
+      </c>
+      <c r="AW27" s="17">
+        <f>SUM(T27:W27)</f>
+        <v>10260.390000000001</v>
+      </c>
+      <c r="AX27" s="2">
+        <f t="shared" ref="AX27:BD27" si="65">+AW27*1.03</f>
+        <v>10568.201700000001</v>
+      </c>
+      <c r="AY27" s="2">
+        <f t="shared" si="65"/>
+        <v>10885.247751000003</v>
+      </c>
+      <c r="AZ27" s="2">
+        <f t="shared" si="65"/>
+        <v>11211.805183530003</v>
+      </c>
+      <c r="BA27" s="2">
+        <f t="shared" si="65"/>
+        <v>11548.159339035903</v>
+      </c>
+      <c r="BB27" s="2">
+        <f t="shared" si="65"/>
+        <v>11894.604119206981</v>
+      </c>
+      <c r="BC27" s="2">
+        <f t="shared" si="65"/>
+        <v>12251.442242783191</v>
+      </c>
+      <c r="BD27" s="2">
+        <f t="shared" si="65"/>
+        <v>12618.985510066686</v>
+      </c>
+    </row>
+    <row r="28" spans="2:56" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" ref="C28" si="33">SUM(C25:C27)</f>
+        <f t="shared" ref="C28" si="66">SUM(C25:C27)</f>
         <v>13697</v>
       </c>
       <c r="D28" s="4">
@@ -2561,7 +3449,7 @@
         <v>12764</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" ref="E28" si="34">SUM(E25:E27)</f>
+        <f t="shared" ref="E28" si="67">SUM(E25:E27)</f>
         <v>14626</v>
       </c>
       <c r="F28" s="4">
@@ -2569,15 +3457,15 @@
         <v>15300</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" ref="G28" si="35">SUM(G25:G27)</f>
+        <f t="shared" ref="G28" si="68">SUM(G25:G27)</f>
         <v>17324</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" ref="H28" si="36">SUM(H25:H27)</f>
+        <f t="shared" ref="H28" si="69">SUM(H25:H27)</f>
         <v>15605</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" ref="I28" si="37">SUM(I25:I27)</f>
+        <f t="shared" ref="I28" si="70">SUM(I25:I27)</f>
         <v>16313</v>
       </c>
       <c r="J28" s="4">
@@ -2585,7 +3473,7 @@
         <v>18078</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" ref="K28" si="38">SUM(K25:K27)</f>
+        <f t="shared" ref="K28" si="71">SUM(K25:K27)</f>
         <v>21420</v>
       </c>
       <c r="L28" s="4">
@@ -2593,60 +3481,124 @@
         <v>20682</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" ref="M28:P28" si="39">SUM(M25:M27)</f>
+        <f t="shared" ref="M28:P28" si="72">SUM(M25:M27)</f>
         <v>23553</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="72"/>
         <v>24543</v>
       </c>
       <c r="O28" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="72"/>
         <v>28648</v>
       </c>
       <c r="P28" s="4">
-        <f t="shared" si="39"/>
+        <f t="shared" si="72"/>
         <v>25756</v>
       </c>
+      <c r="Q28" s="4">
+        <f t="shared" ref="Q28:W28" si="73">SUM(Q25:Q27)</f>
+        <v>25424.200000000004</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="73"/>
+        <v>26489.15</v>
+      </c>
+      <c r="S28" s="4">
+        <f t="shared" si="73"/>
+        <v>30846.050000000003</v>
+      </c>
+      <c r="T28" s="4">
+        <f t="shared" si="73"/>
+        <v>27785.9</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="73"/>
+        <v>27458.315000000002</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="73"/>
+        <v>28604.507500000003</v>
+      </c>
+      <c r="W28" s="4">
+        <f t="shared" si="73"/>
+        <v>33230.567500000005</v>
+      </c>
       <c r="AN28" s="4">
-        <f t="shared" ref="AN28:AQ28" si="40">SUM(AN25:AN27)</f>
+        <f t="shared" ref="AN28:AP28" si="74">SUM(AN25:AN27)</f>
         <v>15159</v>
       </c>
       <c r="AO28" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="74"/>
         <v>19541</v>
       </c>
       <c r="AP28" s="4">
-        <f t="shared" si="40"/>
+        <f t="shared" si="74"/>
         <v>25750</v>
       </c>
       <c r="AQ28" s="4">
-        <f t="shared" ref="AQ28:AR28" si="41">SUM(AQ25:AQ27)</f>
+        <f t="shared" ref="AQ28" si="75">SUM(AQ25:AQ27)</f>
         <v>36363</v>
       </c>
       <c r="AR28" s="4">
-        <f t="shared" ref="AR28:AT28" si="42">SUM(AR25:AR27)</f>
+        <f t="shared" ref="AR28:AS28" si="76">SUM(AR25:AR27)</f>
         <v>46987</v>
       </c>
       <c r="AS28" s="4">
-        <f t="shared" si="42"/>
+        <f t="shared" si="76"/>
         <v>60014</v>
       </c>
       <c r="AT28" s="4">
-        <f t="shared" ref="AT28:AU28" si="43">SUM(AT25:AT27)</f>
+        <f t="shared" ref="AT28:AU28" si="77">SUM(AT25:AT27)</f>
         <v>71416</v>
       </c>
       <c r="AU28" s="4">
-        <f t="shared" si="43"/>
+        <f t="shared" si="77"/>
         <v>97426</v>
       </c>
-    </row>
-    <row r="29" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV28" s="4">
+        <f t="shared" ref="AV28:AW28" si="78">SUM(AV25:AV27)</f>
+        <v>108515.40000000001</v>
+      </c>
+      <c r="AW28" s="4">
+        <f t="shared" si="78"/>
+        <v>117079.29000000002</v>
+      </c>
+      <c r="AX28" s="4">
+        <f t="shared" ref="AX28:BD28" si="79">SUM(AX25:AX27)</f>
+        <v>120591.66870000004</v>
+      </c>
+      <c r="AY28" s="4">
+        <f t="shared" si="79"/>
+        <v>124209.41876100002</v>
+      </c>
+      <c r="AZ28" s="4">
+        <f t="shared" si="79"/>
+        <v>127935.70132383003</v>
+      </c>
+      <c r="BA28" s="4">
+        <f t="shared" si="79"/>
+        <v>131773.77236354494</v>
+      </c>
+      <c r="BB28" s="4">
+        <f t="shared" si="79"/>
+        <v>135726.98553445129</v>
+      </c>
+      <c r="BC28" s="4">
+        <f t="shared" si="79"/>
+        <v>139798.79510048486</v>
+      </c>
+      <c r="BD28" s="4">
+        <f t="shared" si="79"/>
+        <v>143992.75895349937</v>
+      </c>
+    </row>
+    <row r="29" spans="2:56" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29" si="44">C24-C28</f>
+        <f t="shared" ref="C29" si="80">C24-C28</f>
         <v>3872</v>
       </c>
       <c r="D29" s="4">
@@ -2654,7 +3606,7 @@
         <v>4415</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" ref="E29" si="45">E24-E28</f>
+        <f t="shared" ref="E29" si="81">E24-E28</f>
         <v>3170</v>
       </c>
       <c r="F29" s="4">
@@ -2662,15 +3614,15 @@
         <v>3212</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" ref="G29" si="46">G24-G28</f>
+        <f t="shared" ref="G29" si="82">G24-G28</f>
         <v>3944</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" ref="H29" si="47">H24-H28</f>
+        <f t="shared" ref="H29" si="83">H24-H28</f>
         <v>4059</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" ref="I29" si="48">I24-I28</f>
+        <f t="shared" ref="I29" si="84">I24-I28</f>
         <v>6133</v>
       </c>
       <c r="J29" s="4">
@@ -2678,7 +3630,7 @@
         <v>6256</v>
       </c>
       <c r="K29" s="4">
-        <f t="shared" ref="K29" si="49">K24-K28</f>
+        <f t="shared" ref="K29" si="85">K24-K28</f>
         <v>6377</v>
       </c>
       <c r="L29" s="4">
@@ -2686,55 +3638,119 @@
         <v>8903</v>
       </c>
       <c r="M29" s="4">
-        <f t="shared" ref="M29:P29" si="50">M24-M28</f>
+        <f t="shared" ref="M29:P29" si="86">M24-M28</f>
         <v>7713</v>
       </c>
       <c r="N29" s="4">
-        <f t="shared" si="50"/>
+        <f t="shared" si="86"/>
         <v>4841</v>
       </c>
       <c r="O29" s="4">
-        <f t="shared" si="50"/>
+        <f t="shared" si="86"/>
         <v>3484</v>
       </c>
       <c r="P29" s="4">
-        <f t="shared" si="50"/>
+        <f t="shared" si="86"/>
         <v>3918</v>
       </c>
+      <c r="Q29" s="4">
+        <f t="shared" ref="Q29:W29" si="87">Q24-Q28</f>
+        <v>9397.2499999999782</v>
+      </c>
+      <c r="R29" s="4">
+        <f t="shared" si="87"/>
+        <v>8925.7099999999991</v>
+      </c>
+      <c r="S29" s="4">
+        <f t="shared" si="87"/>
+        <v>10582.600000000013</v>
+      </c>
+      <c r="T29" s="4">
+        <f t="shared" si="87"/>
+        <v>9747.3100000000195</v>
+      </c>
+      <c r="U29" s="4">
+        <f t="shared" si="87"/>
+        <v>14726.134000000013</v>
+      </c>
+      <c r="V29" s="4">
+        <f t="shared" si="87"/>
+        <v>14430.642499999991</v>
+      </c>
+      <c r="W29" s="4">
+        <f t="shared" si="87"/>
+        <v>16920.987499999988</v>
+      </c>
       <c r="AN29" s="4">
-        <f t="shared" ref="AN29:AQ29" si="51">AN24-AN28</f>
+        <f t="shared" ref="AN29:AP29" si="88">AN24-AN28</f>
         <v>311</v>
       </c>
       <c r="AO29" s="4">
-        <f t="shared" si="51"/>
+        <f t="shared" si="88"/>
         <v>2404</v>
       </c>
       <c r="AP29" s="4">
-        <f t="shared" si="51"/>
+        <f t="shared" si="88"/>
         <v>4353</v>
       </c>
       <c r="AQ29" s="4">
-        <f t="shared" ref="AQ29:AR29" si="52">AQ24-AQ28</f>
+        <f t="shared" ref="AQ29" si="89">AQ24-AQ28</f>
         <v>4320</v>
       </c>
       <c r="AR29" s="4">
-        <f t="shared" ref="AR29:AT29" si="53">AR24-AR28</f>
+        <f t="shared" ref="AR29:AS29" si="90">AR24-AR28</f>
         <v>12717</v>
       </c>
       <c r="AS29" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" si="90"/>
         <v>14741</v>
       </c>
       <c r="AT29" s="4">
-        <f t="shared" ref="AT29:AU29" si="54">AT24-AT28</f>
+        <f t="shared" ref="AT29:AU29" si="91">AT24-AT28</f>
         <v>22825</v>
       </c>
       <c r="AU29" s="4">
-        <f t="shared" si="54"/>
+        <f t="shared" si="91"/>
         <v>24941</v>
       </c>
-    </row>
-    <row r="30" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV29" s="4">
+        <f t="shared" ref="AV29:AW29" si="92">AV24-AV28</f>
+        <v>32823.560000000041</v>
+      </c>
+      <c r="AW29" s="4">
+        <f t="shared" si="92"/>
+        <v>55825.07399999995</v>
+      </c>
+      <c r="AX29" s="4">
+        <f t="shared" ref="AX29:BD29" si="93">AX24-AX28</f>
+        <v>74555.815499999881</v>
+      </c>
+      <c r="AY29" s="4">
+        <f t="shared" si="93"/>
+        <v>97472.143449000039</v>
+      </c>
+      <c r="AZ29" s="4">
+        <f t="shared" si="93"/>
+        <v>125649.02825666996</v>
+      </c>
+      <c r="BA29" s="4">
+        <f t="shared" si="93"/>
+        <v>160465.32148598009</v>
+      </c>
+      <c r="BB29" s="4">
+        <f t="shared" si="93"/>
+        <v>186709.90009982986</v>
+      </c>
+      <c r="BC29" s="4">
+        <f t="shared" si="93"/>
+        <v>217462.9393262465</v>
+      </c>
+      <c r="BD29" s="4">
+        <f t="shared" si="93"/>
+        <v>253575.66760745161</v>
+      </c>
+    </row>
+    <row r="30" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
@@ -2818,24 +3834,60 @@
         <v>-1456</v>
       </c>
       <c r="AS30" s="2">
-        <f t="shared" ref="AS30" si="55">SUM(D30:G30)</f>
+        <f t="shared" ref="AS30" si="94">SUM(D30:G30)</f>
         <v>-766</v>
       </c>
       <c r="AT30" s="2">
-        <f t="shared" ref="AT30" si="56">SUM(H30:K30)</f>
+        <f t="shared" ref="AT30" si="95">SUM(H30:K30)</f>
         <v>1353</v>
       </c>
       <c r="AU30" s="2">
-        <f t="shared" ref="AU30" si="57">SUM(L30:O30)</f>
+        <f t="shared" ref="AU30" si="96">SUM(L30:O30)</f>
         <v>13210</v>
       </c>
-    </row>
-    <row r="31" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV30" s="17">
+        <f>SUM(P30:S30)</f>
+        <v>-9183</v>
+      </c>
+      <c r="AW30" s="17">
+        <f>SUM(T30:W30)</f>
+        <v>0</v>
+      </c>
+      <c r="AX30" s="2">
+        <f>+AW45*$BG$44</f>
+        <v>908.50038900000004</v>
+      </c>
+      <c r="AY30" s="2">
+        <f t="shared" ref="AY30:BD30" si="97">+AX45*$BG$44</f>
+        <v>1549.9470740564989</v>
+      </c>
+      <c r="AZ30" s="2">
+        <f t="shared" si="97"/>
+        <v>2391.6348435024797</v>
+      </c>
+      <c r="BA30" s="2">
+        <f t="shared" si="97"/>
+        <v>3479.9804798539453</v>
+      </c>
+      <c r="BB30" s="2">
+        <f t="shared" si="97"/>
+        <v>4873.5155465635353</v>
+      </c>
+      <c r="BC30" s="2">
+        <f t="shared" si="97"/>
+        <v>6501.9745795578792</v>
+      </c>
+      <c r="BD30" s="2">
+        <f t="shared" si="97"/>
+        <v>8405.6763477572167</v>
+      </c>
+    </row>
+    <row r="31" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" ref="C31" si="58">C29+C30</f>
+        <f t="shared" ref="C31" si="98">C29+C30</f>
         <v>3350</v>
       </c>
       <c r="D31" s="4">
@@ -2843,7 +3895,7 @@
         <v>4401</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" ref="E31" si="59">E29+E30</f>
+        <f t="shared" ref="E31" si="99">E29+E30</f>
         <v>2889</v>
       </c>
       <c r="F31" s="4">
@@ -2851,15 +3903,15 @@
         <v>2632</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" ref="G31" si="60">G29+G30</f>
+        <f t="shared" ref="G31" si="100">G29+G30</f>
         <v>4053</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" ref="H31" si="61">H29+H30</f>
+        <f t="shared" ref="H31" si="101">H29+H30</f>
         <v>3383</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" ref="I31" si="62">I29+I30</f>
+        <f t="shared" ref="I31" si="102">I29+I30</f>
         <v>6221</v>
       </c>
       <c r="J31" s="4">
@@ -2867,7 +3919,7 @@
         <v>6809</v>
       </c>
       <c r="K31" s="4">
-        <f t="shared" ref="K31" si="63">K29+K30</f>
+        <f t="shared" ref="K31" si="103">K29+K30</f>
         <v>7765</v>
       </c>
       <c r="L31" s="4">
@@ -2875,58 +3927,119 @@
         <v>10268</v>
       </c>
       <c r="M31" s="4">
-        <f t="shared" ref="M31:P31" si="64">M29+M30</f>
+        <f t="shared" ref="M31:W31" si="104">M29+M30</f>
         <v>8634</v>
       </c>
       <c r="N31" s="4">
-        <f t="shared" si="64"/>
+        <f t="shared" si="104"/>
         <v>4315</v>
       </c>
       <c r="O31" s="4">
-        <f t="shared" si="64"/>
+        <f t="shared" si="104"/>
         <v>14934</v>
       </c>
       <c r="P31" s="4">
-        <f t="shared" si="64"/>
+        <f t="shared" si="104"/>
         <v>-5265</v>
       </c>
-      <c r="Q31" s="4"/>
-      <c r="R31" s="4"/>
-      <c r="S31" s="4"/>
+      <c r="Q31" s="4">
+        <f t="shared" si="104"/>
+        <v>9397.2499999999782</v>
+      </c>
+      <c r="R31" s="4">
+        <f t="shared" si="104"/>
+        <v>8925.7099999999991</v>
+      </c>
+      <c r="S31" s="4">
+        <f t="shared" si="104"/>
+        <v>10582.600000000013</v>
+      </c>
+      <c r="T31" s="4">
+        <f t="shared" si="104"/>
+        <v>9747.3100000000195</v>
+      </c>
+      <c r="U31" s="4">
+        <f t="shared" si="104"/>
+        <v>14726.134000000013</v>
+      </c>
+      <c r="V31" s="4">
+        <f t="shared" si="104"/>
+        <v>14430.642499999991</v>
+      </c>
+      <c r="W31" s="4">
+        <f t="shared" si="104"/>
+        <v>16920.987499999988</v>
+      </c>
       <c r="AN31" s="4">
-        <f t="shared" ref="AN31:AQ31" si="65">AN29+AN30</f>
+        <f t="shared" ref="AN31:AP31" si="105">AN29+AN30</f>
         <v>-111</v>
       </c>
       <c r="AO31" s="4">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>1568</v>
       </c>
       <c r="AP31" s="4">
-        <f t="shared" si="65"/>
+        <f t="shared" si="105"/>
         <v>3892</v>
       </c>
       <c r="AQ31" s="4">
-        <f t="shared" ref="AQ31:AR31" si="66">AQ29+AQ30</f>
+        <f t="shared" ref="AQ31" si="106">AQ29+AQ30</f>
         <v>3806</v>
       </c>
       <c r="AR31" s="4">
-        <f t="shared" ref="AR31:AT31" si="67">AR29+AR30</f>
+        <f t="shared" ref="AR31:AS31" si="107">AR29+AR30</f>
         <v>11261</v>
       </c>
       <c r="AS31" s="4">
-        <f t="shared" si="67"/>
+        <f t="shared" si="107"/>
         <v>13975</v>
       </c>
       <c r="AT31" s="4">
-        <f t="shared" ref="AT31:AU31" si="68">AT29+AT30</f>
+        <f t="shared" ref="AT31:BD31" si="108">AT29+AT30</f>
         <v>24178</v>
       </c>
       <c r="AU31" s="4">
-        <f t="shared" si="68"/>
+        <f t="shared" si="108"/>
         <v>38151</v>
       </c>
-    </row>
-    <row r="32" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV31" s="4">
+        <f t="shared" si="108"/>
+        <v>23640.560000000041</v>
+      </c>
+      <c r="AW31" s="4">
+        <f t="shared" si="108"/>
+        <v>55825.07399999995</v>
+      </c>
+      <c r="AX31" s="4">
+        <f t="shared" si="108"/>
+        <v>75464.315888999874</v>
+      </c>
+      <c r="AY31" s="4">
+        <f t="shared" si="108"/>
+        <v>99022.09052305654</v>
+      </c>
+      <c r="AZ31" s="4">
+        <f t="shared" si="108"/>
+        <v>128040.66310017245</v>
+      </c>
+      <c r="BA31" s="4">
+        <f t="shared" si="108"/>
+        <v>163945.30196583405</v>
+      </c>
+      <c r="BB31" s="4">
+        <f t="shared" si="108"/>
+        <v>191583.41564639341</v>
+      </c>
+      <c r="BC31" s="4">
+        <f t="shared" si="108"/>
+        <v>223964.91390580439</v>
+      </c>
+      <c r="BD31" s="4">
+        <f t="shared" si="108"/>
+        <v>261981.34395520884</v>
+      </c>
+    </row>
+    <row r="32" spans="2:56" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
@@ -2986,9 +4099,34 @@
         <f>-1422+1</f>
         <v>-1421</v>
       </c>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
+      <c r="Q32" s="4">
+        <f>+Q31*0.15</f>
+        <v>1409.5874999999967</v>
+      </c>
+      <c r="R32" s="4">
+        <f t="shared" ref="R32:W32" si="109">+R31*0.15</f>
+        <v>1338.8564999999999</v>
+      </c>
+      <c r="S32" s="4">
+        <f t="shared" si="109"/>
+        <v>1587.3900000000019</v>
+      </c>
+      <c r="T32" s="4">
+        <f t="shared" si="109"/>
+        <v>1462.0965000000028</v>
+      </c>
+      <c r="U32" s="4">
+        <f t="shared" si="109"/>
+        <v>2208.9201000000016</v>
+      </c>
+      <c r="V32" s="4">
+        <f t="shared" si="109"/>
+        <v>2164.5963749999987</v>
+      </c>
+      <c r="W32" s="4">
+        <f t="shared" si="109"/>
+        <v>2538.1481249999983</v>
+      </c>
       <c r="AN32" s="2">
         <f>167-37</f>
         <v>130</v>
@@ -3010,24 +4148,60 @@
         <v>1188</v>
       </c>
       <c r="AS32" s="2">
-        <f t="shared" ref="AS32" si="69">SUM(D32:G32)</f>
+        <f t="shared" ref="AS32" si="110">SUM(D32:G32)</f>
         <v>2387</v>
       </c>
       <c r="AT32" s="2">
-        <f t="shared" ref="AT32" si="70">SUM(H32:K32)</f>
+        <f t="shared" ref="AT32" si="111">SUM(H32:K32)</f>
         <v>2847</v>
       </c>
       <c r="AU32" s="2">
-        <f t="shared" ref="AU32" si="71">SUM(L32:O32)</f>
+        <f t="shared" ref="AU32" si="112">SUM(L32:O32)</f>
         <v>4787</v>
       </c>
-    </row>
-    <row r="33" spans="2:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV32" s="17">
+        <f>SUM(P32:S32)</f>
+        <v>2914.8339999999985</v>
+      </c>
+      <c r="AW32" s="17">
+        <f>SUM(T32:W32)</f>
+        <v>8373.7611000000015</v>
+      </c>
+      <c r="AX32" s="2">
+        <f>+AX31*0.15</f>
+        <v>11319.64738334998</v>
+      </c>
+      <c r="AY32" s="2">
+        <f t="shared" ref="AY32:BD32" si="113">+AY31*0.15</f>
+        <v>14853.313578458481</v>
+      </c>
+      <c r="AZ32" s="2">
+        <f t="shared" si="113"/>
+        <v>19206.099465025865</v>
+      </c>
+      <c r="BA32" s="2">
+        <f t="shared" si="113"/>
+        <v>24591.795294875108</v>
+      </c>
+      <c r="BB32" s="2">
+        <f t="shared" si="113"/>
+        <v>28737.512346959011</v>
+      </c>
+      <c r="BC32" s="2">
+        <f t="shared" si="113"/>
+        <v>33594.737085870656</v>
+      </c>
+      <c r="BD32" s="2">
+        <f t="shared" si="113"/>
+        <v>39297.201593281323</v>
+      </c>
+    </row>
+    <row r="33" spans="2:118" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C33" s="4">
-        <f t="shared" ref="C33" si="72">C31-C32</f>
+        <f t="shared" ref="C33" si="114">C31-C32</f>
         <v>3027</v>
       </c>
       <c r="D33" s="4">
@@ -3035,7 +4209,7 @@
         <v>3561</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" ref="E33" si="73">E31-E32</f>
+        <f t="shared" ref="E33" si="115">E31-E32</f>
         <v>2625</v>
       </c>
       <c r="F33" s="4">
@@ -3043,15 +4217,15 @@
         <v>2134</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" ref="G33" si="74">G31-G32</f>
+        <f t="shared" ref="G33" si="116">G31-G32</f>
         <v>3268</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" ref="H33" si="75">H31-H32</f>
+        <f t="shared" ref="H33" si="117">H31-H32</f>
         <v>2535</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" ref="I33" si="76">I31-I32</f>
+        <f t="shared" ref="I33" si="118">I31-I32</f>
         <v>5243</v>
       </c>
       <c r="J33" s="4">
@@ -3059,7 +4233,7 @@
         <v>6331</v>
       </c>
       <c r="K33" s="4">
-        <f t="shared" ref="K33" si="77">K31-K32</f>
+        <f t="shared" ref="K33" si="119">K31-K32</f>
         <v>7222</v>
       </c>
       <c r="L33" s="4">
@@ -3067,63 +4241,372 @@
         <v>8107</v>
       </c>
       <c r="M33" s="4">
-        <f t="shared" ref="M33:P33" si="78">M31-M32</f>
+        <f t="shared" ref="M33:W33" si="120">M31-M32</f>
         <v>7778</v>
       </c>
       <c r="N33" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="120"/>
         <v>3156</v>
       </c>
       <c r="O33" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="120"/>
         <v>14323</v>
       </c>
       <c r="P33" s="4">
-        <f t="shared" si="78"/>
+        <f t="shared" si="120"/>
         <v>-3844</v>
       </c>
-      <c r="Q33" s="4"/>
-      <c r="R33" s="4"/>
-      <c r="S33" s="4"/>
+      <c r="Q33" s="4">
+        <f t="shared" si="120"/>
+        <v>7987.6624999999813</v>
+      </c>
+      <c r="R33" s="4">
+        <f t="shared" si="120"/>
+        <v>7586.8534999999993</v>
+      </c>
+      <c r="S33" s="4">
+        <f t="shared" si="120"/>
+        <v>8995.2100000000119</v>
+      </c>
+      <c r="T33" s="4">
+        <f t="shared" si="120"/>
+        <v>8285.2135000000162</v>
+      </c>
+      <c r="U33" s="4">
+        <f t="shared" si="120"/>
+        <v>12517.213900000012</v>
+      </c>
+      <c r="V33" s="4">
+        <f t="shared" si="120"/>
+        <v>12266.046124999992</v>
+      </c>
+      <c r="W33" s="4">
+        <f t="shared" si="120"/>
+        <v>14382.83937499999</v>
+      </c>
       <c r="AN33" s="4">
-        <f t="shared" ref="AN33:AQ33" si="79">AN31-AN32</f>
+        <f t="shared" ref="AN33:AP33" si="121">AN31-AN32</f>
         <v>-241</v>
       </c>
       <c r="AO33" s="4">
-        <f t="shared" si="79"/>
+        <f t="shared" si="121"/>
         <v>596</v>
       </c>
       <c r="AP33" s="4">
-        <f t="shared" si="79"/>
+        <f t="shared" si="121"/>
         <v>2371</v>
       </c>
       <c r="AQ33" s="4">
-        <f t="shared" ref="AQ33:AR33" si="80">AQ31-AQ32</f>
+        <f t="shared" ref="AQ33" si="122">AQ31-AQ32</f>
         <v>3033</v>
       </c>
       <c r="AR33" s="4">
-        <f t="shared" ref="AR33:AT33" si="81">AR31-AR32</f>
+        <f t="shared" ref="AR33:AS33" si="123">AR31-AR32</f>
         <v>10073</v>
       </c>
       <c r="AS33" s="4">
-        <f t="shared" si="81"/>
+        <f t="shared" si="123"/>
         <v>11588</v>
       </c>
       <c r="AT33" s="4">
-        <f t="shared" ref="AT33:AU33" si="82">AT31-AT32</f>
+        <f t="shared" ref="AT33:AW33" si="124">AT31-AT32</f>
         <v>21331</v>
       </c>
       <c r="AU33" s="4">
-        <f t="shared" si="82"/>
+        <f t="shared" si="124"/>
         <v>33364</v>
       </c>
-    </row>
-    <row r="34" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV33" s="4">
+        <f t="shared" si="124"/>
+        <v>20725.726000000042</v>
+      </c>
+      <c r="AW33" s="4">
+        <f t="shared" si="124"/>
+        <v>47451.312899999946</v>
+      </c>
+      <c r="AX33" s="4">
+        <f t="shared" ref="AX33:BD33" si="125">AX31-AX32</f>
+        <v>64144.668505649897</v>
+      </c>
+      <c r="AY33" s="4">
+        <f t="shared" si="125"/>
+        <v>84168.776944598067</v>
+      </c>
+      <c r="AZ33" s="4">
+        <f t="shared" si="125"/>
+        <v>108834.56363514658</v>
+      </c>
+      <c r="BA33" s="4">
+        <f t="shared" si="125"/>
+        <v>139353.50667095894</v>
+      </c>
+      <c r="BB33" s="4">
+        <f t="shared" si="125"/>
+        <v>162845.9032994344</v>
+      </c>
+      <c r="BC33" s="4">
+        <f t="shared" si="125"/>
+        <v>190370.17681993375</v>
+      </c>
+      <c r="BD33" s="4">
+        <f t="shared" si="125"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BE33" s="2">
+        <f>+BD33*(1+$BG$45)</f>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BF33" s="2">
+        <f t="shared" ref="BF33:DN33" si="126">+BE33*(1+$BG$45)</f>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BG33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BH33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BI33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BJ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BK33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BL33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BM33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BN33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BO33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BP33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BQ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BR33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BS33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BT33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BU33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BV33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BW33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BX33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BY33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="BZ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CA33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CB33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CC33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CD33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CE33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CF33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CG33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CH33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CI33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CJ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CK33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CL33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CM33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CN33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CO33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CP33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CQ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CR33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CS33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CT33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CU33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CV33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CW33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CX33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CY33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="CZ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DA33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DB33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DC33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DD33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DE33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DF33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DG33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DH33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DI33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DJ33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DK33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DL33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DM33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+      <c r="DN33" s="2">
+        <f t="shared" si="126"/>
+        <v>222684.14236192752</v>
+      </c>
+    </row>
+    <row r="34" spans="2:118" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" ref="C34" si="83">C33/C35</f>
+        <f t="shared" ref="C34" si="127">C33/C35</f>
         <v>6.0419161676646711</v>
       </c>
       <c r="D34" s="7">
@@ -3131,7 +4614,7 @@
         <v>7.0936254980079685</v>
       </c>
       <c r="E34" s="7">
-        <f t="shared" ref="E34" si="84">E33/E35</f>
+        <f t="shared" ref="E34" si="128">E33/E35</f>
         <v>5.2186878727634198</v>
       </c>
       <c r="F34" s="7">
@@ -3139,15 +4622,15 @@
         <v>4.2341269841269842</v>
       </c>
       <c r="G34" s="7">
-        <f t="shared" ref="G34" si="85">G33/G35</f>
+        <f t="shared" ref="G34" si="129">G33/G35</f>
         <v>6.4712871287128717</v>
       </c>
       <c r="H34" s="7">
-        <f t="shared" ref="H34" si="86">H33/H35</f>
+        <f t="shared" ref="H34" si="130">H33/H35</f>
         <v>5.0098814229249014</v>
       </c>
       <c r="I34" s="7">
-        <f t="shared" ref="I34" si="87">I33/I35</f>
+        <f t="shared" ref="I34" si="131">I33/I35</f>
         <v>10.300589390962672</v>
       </c>
       <c r="J34" s="7">
@@ -3155,7 +4638,7 @@
         <v>12.365234375</v>
       </c>
       <c r="K34" s="7">
-        <f t="shared" ref="K34" si="88">K33/K35</f>
+        <f t="shared" ref="K34" si="132">K33/K35</f>
         <v>14.077972709551657</v>
       </c>
       <c r="L34" s="7">
@@ -3178,29 +4661,56 @@
         <f>P33/P35</f>
         <v>-7.5520628683693518</v>
       </c>
-      <c r="Q34" s="7"/>
+      <c r="Q34" s="7">
+        <f t="shared" ref="Q34:W34" si="133">Q33/Q35</f>
+        <v>15.692853634577567</v>
+      </c>
+      <c r="R34" s="7">
+        <f t="shared" si="133"/>
+        <v>14.905409626719056</v>
+      </c>
+      <c r="S34" s="7">
+        <f t="shared" si="133"/>
+        <v>17.672318271119867</v>
+      </c>
+      <c r="T34" s="7">
+        <f t="shared" si="133"/>
+        <v>16.277433202357596</v>
+      </c>
+      <c r="U34" s="7">
+        <f t="shared" si="133"/>
+        <v>24.591775834970552</v>
+      </c>
+      <c r="V34" s="7">
+        <f t="shared" si="133"/>
+        <v>24.098322445972478</v>
+      </c>
+      <c r="W34" s="7">
+        <f t="shared" si="133"/>
+        <v>28.257051817288783</v>
+      </c>
       <c r="AN34" s="7">
-        <f t="shared" ref="AN34" si="89">AN33/AN35</f>
+        <f t="shared" ref="AN34" si="134">AN33/AN35</f>
         <v>-0.52164502164502169</v>
       </c>
       <c r="AO34" s="7">
-        <f t="shared" ref="AO34" si="90">AO33/AO35</f>
+        <f t="shared" ref="AO34" si="135">AO33/AO35</f>
         <v>1.249475890985325</v>
       </c>
       <c r="AP34" s="7">
-        <f t="shared" ref="AP34" si="91">AP33/AP35</f>
+        <f t="shared" ref="AP34" si="136">AP33/AP35</f>
         <v>4.8987603305785123</v>
       </c>
       <c r="AQ34" s="7">
-        <f t="shared" ref="AQ34" si="92">AQ33/AQ35</f>
+        <f t="shared" ref="AQ34" si="137">AQ33/AQ35</f>
         <v>6.1521298174442194</v>
       </c>
       <c r="AR34" s="7">
-        <f t="shared" ref="AR34:AS34" si="93">AR33/AR35</f>
+        <f t="shared" ref="AR34:AS34" si="138">AR33/AR35</f>
         <v>20.146000000000001</v>
       </c>
       <c r="AS34" s="7">
-        <f t="shared" si="93"/>
+        <f t="shared" si="138"/>
         <v>23.014895729890764</v>
       </c>
       <c r="AT34" s="7">
@@ -3211,8 +4721,44 @@
         <f>AU33/AU35</f>
         <v>64.847424684159378</v>
       </c>
-    </row>
-    <row r="35" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV34" s="7">
+        <f t="shared" ref="AV34:AW34" si="139">AV33/AV35</f>
+        <v>40.718518664047238</v>
+      </c>
+      <c r="AW34" s="7">
+        <f t="shared" si="139"/>
+        <v>93.224583300589288</v>
+      </c>
+      <c r="AX34" s="7">
+        <f t="shared" ref="AX34" si="140">AX33/AX35</f>
+        <v>126.02095973605088</v>
+      </c>
+      <c r="AY34" s="7">
+        <f t="shared" ref="AY34" si="141">AY33/AY35</f>
+        <v>165.36105490097853</v>
+      </c>
+      <c r="AZ34" s="7">
+        <f t="shared" ref="AZ34" si="142">AZ33/AZ35</f>
+        <v>213.8203607763194</v>
+      </c>
+      <c r="BA34" s="7">
+        <f t="shared" ref="BA34" si="143">BA33/BA35</f>
+        <v>273.77899149500774</v>
+      </c>
+      <c r="BB34" s="7">
+        <f t="shared" ref="BB34" si="144">BB33/BB35</f>
+        <v>319.93301237609904</v>
+      </c>
+      <c r="BC34" s="7">
+        <f t="shared" ref="BC34" si="145">BC33/BC35</f>
+        <v>374.00820593307219</v>
+      </c>
+      <c r="BD34" s="7">
+        <f t="shared" ref="BD34" si="146">BD33/BD35</f>
+        <v>437.49340346154719</v>
+      </c>
+    </row>
+    <row r="35" spans="2:118" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>2</v>
       </c>
@@ -3256,6 +4802,34 @@
         <v>516</v>
       </c>
       <c r="P35" s="3">
+        <v>509</v>
+      </c>
+      <c r="Q35" s="3">
+        <f>+P35</f>
+        <v>509</v>
+      </c>
+      <c r="R35" s="3">
+        <f t="shared" ref="R35:W35" si="147">+Q35</f>
+        <v>509</v>
+      </c>
+      <c r="S35" s="3">
+        <f t="shared" si="147"/>
+        <v>509</v>
+      </c>
+      <c r="T35" s="3">
+        <f t="shared" si="147"/>
+        <v>509</v>
+      </c>
+      <c r="U35" s="3">
+        <f t="shared" si="147"/>
+        <v>509</v>
+      </c>
+      <c r="V35" s="3">
+        <f t="shared" si="147"/>
+        <v>509</v>
+      </c>
+      <c r="W35" s="3">
+        <f t="shared" si="147"/>
         <v>509</v>
       </c>
       <c r="AN35">
@@ -3285,8 +4859,44 @@
         <f>AVERAGE(L35:O35)</f>
         <v>514.5</v>
       </c>
-    </row>
-    <row r="37" spans="2:47" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV35">
+        <f>AVERAGE(P35:S35)</f>
+        <v>509</v>
+      </c>
+      <c r="AW35">
+        <f>AVERAGE(T35:W35)</f>
+        <v>509</v>
+      </c>
+      <c r="AX35">
+        <f>+AW35</f>
+        <v>509</v>
+      </c>
+      <c r="AY35">
+        <f t="shared" ref="AY35:BD35" si="148">+AX35</f>
+        <v>509</v>
+      </c>
+      <c r="AZ35">
+        <f t="shared" si="148"/>
+        <v>509</v>
+      </c>
+      <c r="BA35">
+        <f t="shared" si="148"/>
+        <v>509</v>
+      </c>
+      <c r="BB35">
+        <f t="shared" si="148"/>
+        <v>509</v>
+      </c>
+      <c r="BC35">
+        <f t="shared" si="148"/>
+        <v>509</v>
+      </c>
+      <c r="BD35">
+        <f t="shared" si="148"/>
+        <v>509</v>
+      </c>
+    </row>
+    <row r="37" spans="2:118" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
@@ -3303,78 +4913,139 @@
         <v>0.26385259631490787</v>
       </c>
       <c r="I37" s="10">
-        <f t="shared" ref="I37:K37" si="94">I21/E21-1</f>
+        <f t="shared" ref="I37:K37" si="149">I21/E21-1</f>
         <v>0.40230900258658764</v>
       </c>
       <c r="J37" s="10">
-        <f t="shared" si="94"/>
+        <f t="shared" si="149"/>
         <v>0.37387290836084075</v>
       </c>
       <c r="K37" s="10">
-        <f t="shared" si="94"/>
+        <f t="shared" si="149"/>
         <v>0.43594816839553041</v>
       </c>
       <c r="L37" s="10">
-        <f t="shared" ref="L37" si="95">L21/H21-1</f>
+        <f t="shared" ref="L37" si="150">L21/H21-1</f>
         <v>0.43823888034777081</v>
       </c>
       <c r="M37" s="10">
-        <f t="shared" ref="M37" si="96">M21/I21-1</f>
+        <f t="shared" ref="M37" si="151">M21/I21-1</f>
         <v>0.27181932697498645</v>
       </c>
       <c r="N37" s="10">
-        <f t="shared" ref="N37" si="97">N21/J21-1</f>
+        <f t="shared" ref="N37" si="152">N21/J21-1</f>
         <v>0.15255083467679031</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" ref="O37" si="98">O21/K21-1</f>
+        <f t="shared" ref="O37" si="153">O21/K21-1</f>
         <v>9.4436701047349692E-2</v>
       </c>
       <c r="P37" s="10">
         <f>P21/L21-1</f>
         <v>7.3038574245747334E-2</v>
       </c>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
+      <c r="Q37" s="10">
+        <f t="shared" ref="Q37:W37" si="154">Q21/M21-1</f>
+        <v>0.17094004244782446</v>
+      </c>
+      <c r="R37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.17543767822979461</v>
+      </c>
+      <c r="S37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.16993639565685692</v>
+      </c>
+      <c r="T37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.17874428910034013</v>
+      </c>
+      <c r="U37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.18011515755241891</v>
+      </c>
+      <c r="V37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.18516405814548054</v>
+      </c>
+      <c r="W37" s="10">
+        <f t="shared" si="154"/>
+        <v>0.17904092538533334</v>
+      </c>
       <c r="AM37" s="15">
-        <f t="shared" ref="AM37:AR37" si="99">AM21/AL21-1</f>
+        <f t="shared" ref="AM37:AQ37" si="155">AM21/AL21-1</f>
         <v>0.21866662301736706</v>
       </c>
       <c r="AN37" s="15">
-        <f t="shared" si="99"/>
+        <f t="shared" si="155"/>
         <v>0.1952398861011122</v>
       </c>
       <c r="AO37" s="15">
-        <f t="shared" si="99"/>
+        <f t="shared" si="155"/>
         <v>0.20247673843664304</v>
       </c>
       <c r="AP37" s="15">
-        <f t="shared" si="99"/>
+        <f t="shared" si="155"/>
         <v>0.27083528026465808</v>
       </c>
       <c r="AQ37" s="15">
-        <f t="shared" si="99"/>
+        <f t="shared" si="155"/>
         <v>0.30796326119408479</v>
       </c>
       <c r="AR37" s="15">
-        <f t="shared" ref="AR37:AS37" si="100">AR21/AQ21-1</f>
+        <f t="shared" ref="AR37" si="156">AR21/AQ21-1</f>
         <v>0.3093396152159491</v>
       </c>
       <c r="AS37" s="15">
-        <f t="shared" ref="AS37:AT37" si="101">AS21/AR21-1</f>
+        <f t="shared" ref="AS37" si="157">AS21/AR21-1</f>
         <v>0.20454125820676983</v>
       </c>
       <c r="AT37" s="15">
-        <f t="shared" ref="AT37:AU37" si="102">AT21/AS21-1</f>
+        <f t="shared" ref="AT37" si="158">AT21/AS21-1</f>
         <v>0.37623430604373276</v>
       </c>
       <c r="AU37" s="15">
         <f>AU21/AT21-1</f>
         <v>0.21695366571345676</v>
       </c>
-    </row>
-    <row r="38" spans="2:47" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV37" s="15">
+        <f t="shared" ref="AV37:BD37" si="159">AV21/AU21-1</f>
+        <v>0.14909433785561355</v>
+      </c>
+      <c r="AW37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.18071772119870366</v>
+      </c>
+      <c r="AX37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.10462481251387579</v>
+      </c>
+      <c r="AY37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.11300732331655872</v>
+      </c>
+      <c r="AZ37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.12232893274764023</v>
+      </c>
+      <c r="BA37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.13254012099457801</v>
+      </c>
+      <c r="BB37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.10215394818293033</v>
+      </c>
+      <c r="BC37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.10678402542829613</v>
+      </c>
+      <c r="BD37" s="15">
+        <f t="shared" si="159"/>
+        <v>0.11156651067274548</v>
+      </c>
+    </row>
+    <row r="38" spans="2:118" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B38" s="17" t="s">
         <v>56</v>
       </c>
@@ -3382,34 +5053,125 @@
       <c r="D38" s="18"/>
       <c r="E38" s="18"/>
       <c r="F38" s="18"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="19"/>
-      <c r="I38" s="19"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="N38" s="19"/>
-      <c r="O38" s="19"/>
-      <c r="P38" s="19"/>
-      <c r="Q38" s="18"/>
-      <c r="R38" s="18"/>
-      <c r="S38" s="18"/>
+      <c r="G38" s="19">
+        <f t="shared" ref="G38" si="160">+G12/C12-1</f>
+        <v>0.14652704535181549</v>
+      </c>
+      <c r="H38" s="19">
+        <f t="shared" ref="H38" si="161">+H12/D12-1</f>
+        <v>0.24252491694352152</v>
+      </c>
+      <c r="I38" s="19">
+        <f t="shared" ref="I38" si="162">+I12/E12-1</f>
+        <v>0.47798924419540789</v>
+      </c>
+      <c r="J38" s="19">
+        <f t="shared" ref="J38" si="163">+J12/F12-1</f>
+        <v>0.37989097862381915</v>
+      </c>
+      <c r="K38" s="19">
+        <f t="shared" ref="K38:O38" si="164">+K12/G12-1</f>
+        <v>0.45543947258908823</v>
+      </c>
+      <c r="L38" s="19">
+        <f t="shared" si="164"/>
+        <v>0.44333187820582776</v>
+      </c>
+      <c r="M38" s="19">
+        <f t="shared" si="164"/>
+        <v>0.15820550810528156</v>
+      </c>
+      <c r="N38" s="19">
+        <f t="shared" si="164"/>
+        <v>3.2926577042399208E-2</v>
+      </c>
+      <c r="O38" s="19">
+        <f t="shared" si="164"/>
+        <v>-5.6583046154309313E-3</v>
+      </c>
+      <c r="P38" s="19">
+        <f>+P12/L12-1</f>
+        <v>-3.3496531256497986E-2</v>
+      </c>
+      <c r="Q38" s="19">
+        <f t="shared" ref="Q38:W38" si="165">+Q12/M12-1</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="R38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="S38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="T38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="U38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="V38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="W38" s="19">
+        <f t="shared" si="165"/>
+        <v>0.10000000000000009</v>
+      </c>
       <c r="AR38" s="20"/>
       <c r="AS38" s="20">
-        <f t="shared" ref="AS38" si="103">AS12/AR12-1</f>
+        <f t="shared" ref="AS38" si="166">AS12/AR12-1</f>
         <v>0.14847097660728359</v>
       </c>
       <c r="AT38" s="20">
-        <f t="shared" ref="AT38" si="104">AT12/AS12-1</f>
+        <f t="shared" ref="AT38" si="167">AT12/AS12-1</f>
         <v>0.39719073679440986</v>
       </c>
       <c r="AU38" s="20">
         <f>AU12/AT12-1</f>
         <v>0.12529072860769497</v>
       </c>
-    </row>
-    <row r="39" spans="2:47" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV38" s="20">
+        <f t="shared" ref="AV38:BD38" si="168">AV12/AU12-1</f>
+        <v>6.819948215692917E-2</v>
+      </c>
+      <c r="AW38" s="20">
+        <f t="shared" si="168"/>
+        <v>9.9999999999999867E-2</v>
+      </c>
+      <c r="AX38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="AY38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="AZ38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BA38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BB38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BC38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BD38" s="20">
+        <f t="shared" si="168"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:118" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B39" s="17" t="s">
         <v>57</v>
       </c>
@@ -3417,34 +5179,125 @@
       <c r="D39" s="18"/>
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
-      <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
-      <c r="L39" s="19"/>
-      <c r="M39" s="19"/>
-      <c r="N39" s="19"/>
-      <c r="O39" s="19"/>
-      <c r="P39" s="19"/>
-      <c r="Q39" s="18"/>
-      <c r="R39" s="18"/>
-      <c r="S39" s="18"/>
+      <c r="G39" s="19">
+        <f t="shared" ref="G39:O39" si="169">+G14/C14-1</f>
+        <v>0.30359411193304942</v>
+      </c>
+      <c r="H39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.29961403823714217</v>
+      </c>
+      <c r="I39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.52106671125229886</v>
+      </c>
+      <c r="J39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.54677565849227983</v>
+      </c>
+      <c r="K39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.56637624670411557</v>
+      </c>
+      <c r="L39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.63747496374058987</v>
+      </c>
+      <c r="M39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.37867546029128873</v>
+      </c>
+      <c r="N39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.18672930123311793</v>
+      </c>
+      <c r="O39" s="19">
+        <f t="shared" si="169"/>
+        <v>0.10952537783144867</v>
+      </c>
+      <c r="P39" s="19">
+        <f>+P14/L14-1</f>
+        <v>6.8581551309629285E-2</v>
+      </c>
+      <c r="Q39" s="19">
+        <f t="shared" ref="Q39:W39" si="170">+Q14/M14-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="R39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="S39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="T39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="U39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="V39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="W39" s="19">
+        <f t="shared" si="170"/>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="AR39" s="20"/>
       <c r="AS39" s="20">
-        <f t="shared" ref="AS39" si="105">AS14/AR14-1</f>
+        <f t="shared" ref="AS39" si="171">AS14/AR14-1</f>
         <v>0.25771435255585451</v>
       </c>
       <c r="AT39" s="20">
-        <f t="shared" ref="AT39:AU39" si="106">AT14/AS14-1</f>
+        <f t="shared" ref="AT39" si="172">AT14/AS14-1</f>
         <v>0.4961961273041795</v>
       </c>
       <c r="AU39" s="20">
         <f>AU14/AT14-1</f>
         <v>0.28505538495965776</v>
       </c>
-    </row>
-    <row r="40" spans="2:47" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV39" s="20">
+        <f t="shared" ref="AV39:BD39" si="173">AV14/AU14-1</f>
+        <v>0.16985662596985462</v>
+      </c>
+      <c r="AW39" s="20">
+        <f t="shared" si="173"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AX39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="AY39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="AZ39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BA39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BB39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BC39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BD39" s="20">
+        <f t="shared" si="173"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:118" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B40" s="17" t="s">
         <v>58</v>
       </c>
@@ -3452,34 +5305,125 @@
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
       <c r="F40" s="18"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
-      <c r="L40" s="19"/>
-      <c r="M40" s="19"/>
-      <c r="N40" s="19"/>
-      <c r="O40" s="19"/>
-      <c r="P40" s="19"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
+      <c r="G40" s="19">
+        <f t="shared" ref="G40:O41" si="174">+G15/C15-1</f>
+        <v>0.3223036120232381</v>
+      </c>
+      <c r="H40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.27959465684016571</v>
+      </c>
+      <c r="I40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.28699743370402042</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.32580189630825096</v>
+      </c>
+      <c r="K40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.34880611270296091</v>
+      </c>
+      <c r="L40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.36429085673146155</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.31555333998005985</v>
+      </c>
+      <c r="N40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.23980523432744971</v>
+      </c>
+      <c r="O40" s="19">
+        <f t="shared" si="174"/>
+        <v>0.15040362554878905</v>
+      </c>
+      <c r="P40" s="19">
+        <f>+P15/L15-1</f>
+        <v>0.10949868073878632</v>
+      </c>
+      <c r="Q40" s="19">
+        <f t="shared" ref="Q40:W41" si="175">+Q15/M15-1</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="R40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="S40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="T40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="U40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="V40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="W40" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="AR40" s="20"/>
       <c r="AS40" s="20">
-        <f t="shared" ref="AS40" si="107">AS15/AR15-1</f>
+        <f t="shared" ref="AS40" si="176">AS15/AR15-1</f>
         <v>0.35596809486835612</v>
       </c>
       <c r="AT40" s="20">
-        <f t="shared" ref="AT40:AU40" si="108">AT15/AS15-1</f>
+        <f t="shared" ref="AT40" si="177">AT15/AS15-1</f>
         <v>0.31218115564810001</v>
       </c>
       <c r="AU40" s="20">
         <f>AU15/AT15-1</f>
         <v>0.26028484151227826</v>
       </c>
-    </row>
-    <row r="41" spans="2:47" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AV40" s="20">
+        <f t="shared" ref="AV40:BD41" si="178">AV15/AU15-1</f>
+        <v>0.17840594308738345</v>
+      </c>
+      <c r="AW40" s="20">
+        <f t="shared" si="178"/>
+        <v>0.20000000000000018</v>
+      </c>
+      <c r="AX40" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AY40" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AZ40" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="BA40" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="BB40" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BC40" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BD40" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:118" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B41" s="17" t="s">
         <v>59</v>
       </c>
@@ -3487,132 +5431,287 @@
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="18"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
-      <c r="L41" s="19"/>
-      <c r="M41" s="19"/>
-      <c r="N41" s="19"/>
-      <c r="O41" s="19"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
+      <c r="G41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.41145218417945695</v>
+      </c>
+      <c r="H41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.43814432989690721</v>
+      </c>
+      <c r="I41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.40606262491672229</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.50529838259899607</v>
+      </c>
+      <c r="K41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.53701380175658731</v>
+      </c>
+      <c r="L41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.63364055299539168</v>
+      </c>
+      <c r="M41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.76522151149016815</v>
+      </c>
+      <c r="N41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.41015190811411628</v>
+      </c>
+      <c r="O41" s="19">
+        <f t="shared" si="174"/>
+        <v>0.32190476190476192</v>
+      </c>
+      <c r="P41" s="19">
+        <f t="shared" ref="P40:P41" si="179">+P16/L16-1</f>
+        <v>0.23444601159692846</v>
+      </c>
+      <c r="Q41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="R41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="S41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="T41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="U41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="V41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="W41" s="19">
+        <f t="shared" si="175"/>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="AR41" s="20"/>
       <c r="AS41" s="20">
-        <f t="shared" ref="AS41" si="109">AS16/AR16-1</f>
+        <f t="shared" ref="AS41" si="180">AS16/AR16-1</f>
         <v>0.39354966363276622</v>
       </c>
       <c r="AT41" s="20">
-        <f t="shared" ref="AT41:AU41" si="110">AT16/AS16-1</f>
+        <f t="shared" ref="AT41:AU41" si="181">AT16/AS16-1</f>
         <v>0.4819679114013915</v>
       </c>
       <c r="AU41" s="20">
-        <f t="shared" si="110"/>
+        <f t="shared" si="181"/>
         <v>0.49269461077844312</v>
       </c>
-    </row>
-    <row r="42" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.2070539152759947</v>
+      </c>
+      <c r="AW41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="AX41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AY41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="AZ41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="BA41" s="20">
+        <f t="shared" si="178"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="BB41" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BC41" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+      <c r="BD41" s="20">
+        <f t="shared" si="178"/>
+        <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:118" x14ac:dyDescent="0.2">
       <c r="B42" s="2" t="s">
         <v>39</v>
       </c>
       <c r="G42" s="8">
-        <f t="shared" ref="G42:H42" si="111">G10/C10-1</f>
+        <f t="shared" ref="G42:H42" si="182">G10/C10-1</f>
         <v>0.33970390309555865</v>
       </c>
       <c r="H42" s="8">
-        <f t="shared" si="111"/>
+        <f t="shared" si="182"/>
         <v>0.32783264033264037</v>
       </c>
       <c r="I42" s="8">
-        <f t="shared" ref="I42" si="112">I10/E10-1</f>
+        <f t="shared" ref="I42" si="183">I10/E10-1</f>
         <v>0.28958358191146649</v>
       </c>
       <c r="J42" s="8">
-        <f t="shared" ref="J42" si="113">J10/F10-1</f>
+        <f t="shared" ref="J42" si="184">J10/F10-1</f>
         <v>0.28971650917176217</v>
       </c>
       <c r="K42" s="8">
-        <f t="shared" ref="K42" si="114">K10/G10-1</f>
+        <f t="shared" ref="K42" si="185">K10/G10-1</f>
         <v>0.28008840667068524</v>
       </c>
       <c r="L42" s="8">
-        <f t="shared" ref="L42" si="115">L10/H10-1</f>
+        <f t="shared" ref="L42" si="186">L10/H10-1</f>
         <v>0.32136216850963883</v>
       </c>
       <c r="M42" s="8">
-        <f t="shared" ref="M42" si="116">M10/I10-1</f>
+        <f t="shared" ref="M42" si="187">M10/I10-1</f>
         <v>0.37018874907475952</v>
       </c>
       <c r="N42" s="8">
-        <f t="shared" ref="N42" si="117">N10/J10-1</f>
+        <f t="shared" ref="N42" si="188">N10/J10-1</f>
         <v>0.3886733902249806</v>
       </c>
       <c r="O42" s="8">
-        <f t="shared" ref="O42" si="118">O10/K10-1</f>
+        <f t="shared" ref="O42" si="189">O10/K10-1</f>
         <v>0.39538533982106427</v>
       </c>
       <c r="P42" s="8">
         <f>P10/L10-1</f>
         <v>0.36569651188624741</v>
       </c>
+      <c r="Q42" s="8">
+        <f t="shared" ref="Q42:W42" si="190">Q10/M10-1</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="R42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="S42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="T42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="U42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="V42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="W42" s="8">
+        <f t="shared" si="190"/>
+        <v>0.39999999999999991</v>
+      </c>
       <c r="AO42" s="13">
-        <f t="shared" ref="AO42:AR42" si="119">AO10/AN10-1</f>
+        <f t="shared" ref="AO42:AQ42" si="191">AO10/AN10-1</f>
         <v>0.69681309216192933</v>
       </c>
       <c r="AP42" s="13">
-        <f t="shared" si="119"/>
+        <f t="shared" si="191"/>
         <v>0.55063451776649752</v>
       </c>
       <c r="AQ42" s="13">
-        <f t="shared" si="119"/>
+        <f t="shared" si="191"/>
         <v>0.42884033063262139</v>
       </c>
       <c r="AR42" s="13">
-        <f t="shared" ref="AR42" si="120">AR10/AQ10-1</f>
+        <f t="shared" ref="AR42" si="192">AR10/AQ10-1</f>
         <v>0.46944269431238905</v>
       </c>
       <c r="AS42" s="13">
-        <f t="shared" ref="AS42:AT42" si="121">AS10/AR10-1</f>
+        <f t="shared" ref="AS42" si="193">AS10/AR10-1</f>
         <v>0.36526992788930035</v>
       </c>
       <c r="AT42" s="13">
-        <f t="shared" ref="AT42:AU42" si="122">AT10/AS10-1</f>
+        <f t="shared" ref="AT42" si="194">AT10/AS10-1</f>
         <v>0.29532347399074976</v>
       </c>
       <c r="AU42" s="13">
         <f>AU10/AT10-1</f>
         <v>0.37099404893101173</v>
       </c>
-    </row>
-    <row r="43" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="AV42" s="13">
+        <f t="shared" ref="AV42:BD42" si="195">AV10/AU10-1</f>
+        <v>0.39255329410629902</v>
+      </c>
+      <c r="AW42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.39999999999999969</v>
+      </c>
+      <c r="AX42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AY42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="AZ42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.29999999999999982</v>
+      </c>
+      <c r="BA42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="BB42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="BC42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="BD42" s="13">
+        <f t="shared" si="195"/>
+        <v>0.19999999999999996</v>
+      </c>
+    </row>
+    <row r="43" spans="2:118" x14ac:dyDescent="0.2">
       <c r="B43" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C43" s="8">
-        <f t="shared" ref="C43:I43" si="123">C24/C21</f>
+        <f t="shared" ref="C43:H43" si="196">C24/C21</f>
         <v>0.24272273876462705</v>
       </c>
       <c r="D43" s="8">
-        <f t="shared" si="123"/>
+        <f t="shared" si="196"/>
         <v>0.28775544388609714</v>
       </c>
       <c r="E43" s="8">
-        <f t="shared" si="123"/>
+        <f t="shared" si="196"/>
         <v>0.28067629802536115</v>
       </c>
       <c r="F43" s="8">
-        <f t="shared" si="123"/>
+        <f t="shared" si="196"/>
         <v>0.26452894357039769</v>
       </c>
       <c r="G43" s="8">
-        <f t="shared" si="123"/>
+        <f t="shared" si="196"/>
         <v>0.24323798849457323</v>
       </c>
       <c r="H43" s="8">
-        <f t="shared" si="123"/>
+        <f t="shared" si="196"/>
         <v>0.26061602078142393</v>
       </c>
       <c r="I43" s="8">
@@ -3632,53 +5731,609 @@
         <v>0.2726275825208721</v>
       </c>
       <c r="M43" s="8">
-        <f t="shared" ref="M43:P43" si="124">M24/M21</f>
+        <f t="shared" ref="M43:P43" si="197">M24/M21</f>
         <v>0.27649451715599577</v>
       </c>
       <c r="N43" s="8">
-        <f t="shared" si="124"/>
+        <f t="shared" si="197"/>
         <v>0.26516983720174708</v>
       </c>
       <c r="O43" s="8">
-        <f t="shared" si="124"/>
+        <f t="shared" si="197"/>
         <v>0.23383692836142403</v>
       </c>
       <c r="P43" s="8">
-        <f t="shared" si="124"/>
+        <f t="shared" si="197"/>
         <v>0.25483494211809971</v>
       </c>
+      <c r="Q43" s="8">
+        <f t="shared" ref="Q43:W43" si="198">Q24/Q21</f>
+        <v>0.26298222413882938</v>
+      </c>
+      <c r="R43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.27189368964611837</v>
+      </c>
+      <c r="S43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.25769967399275839</v>
+      </c>
+      <c r="T43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.27345066979848864</v>
+      </c>
+      <c r="U43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.26996504455777348</v>
+      </c>
+      <c r="V43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.27877796758063539</v>
+      </c>
+      <c r="W43" s="8">
+        <f t="shared" si="198"/>
+        <v>0.26458706625619222</v>
+      </c>
       <c r="AN43" s="14">
-        <f t="shared" ref="AN43:AP43" si="125">AN24/AN21</f>
+        <f t="shared" ref="AN43:AP43" si="199">AN24/AN21</f>
         <v>0.17384366431428958</v>
       </c>
       <c r="AO43" s="14">
-        <f t="shared" si="125"/>
+        <f t="shared" si="199"/>
         <v>0.20508195802104554</v>
       </c>
       <c r="AP43" s="14">
-        <f t="shared" si="125"/>
+        <f t="shared" si="199"/>
         <v>0.22136674829211617</v>
       </c>
       <c r="AQ43" s="14">
-        <f t="shared" ref="AQ43:AR43" si="126">AQ24/AQ21</f>
+        <f t="shared" ref="AQ43" si="200">AQ24/AQ21</f>
         <v>0.22872836854710848</v>
       </c>
       <c r="AR43" s="14">
-        <f t="shared" ref="AR43:AT43" si="127">AR24/AR21</f>
+        <f t="shared" ref="AR43:AS43" si="201">AR24/AR21</f>
         <v>0.25636467471348767</v>
       </c>
       <c r="AS43" s="14">
-        <f t="shared" si="127"/>
+        <f t="shared" si="201"/>
         <v>0.26648533804835273</v>
       </c>
       <c r="AT43" s="14">
-        <f t="shared" ref="AT43:AU43" si="128">AT24/AT21</f>
+        <f t="shared" ref="AT43" si="202">AT24/AT21</f>
         <v>0.24410719466202496</v>
       </c>
       <c r="AU43" s="14">
         <f>AU24/AU21</f>
         <v>0.26045395915900066</v>
       </c>
+      <c r="AV43" s="14">
+        <f t="shared" ref="AV43:BD43" si="203">AV24/AV21</f>
+        <v>0.26180193817101832</v>
+      </c>
+      <c r="AW43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.27125068226688431</v>
+      </c>
+      <c r="AX43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.27714882839393068</v>
+      </c>
+      <c r="AY43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.28286658126876557</v>
+      </c>
+      <c r="AZ43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.28830688049681286</v>
+      </c>
+      <c r="BA43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.29337062489644677</v>
+      </c>
+      <c r="BB43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.2936843270668249</v>
+      </c>
+      <c r="BC43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.29400835535436326</v>
+      </c>
+      <c r="BD43" s="14">
+        <f t="shared" si="203"/>
+        <v>0.29434021552690437</v>
+      </c>
+      <c r="BF43" t="s">
+        <v>77</v>
+      </c>
+      <c r="BG43" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:118" x14ac:dyDescent="0.2">
+      <c r="BF44" t="s">
+        <v>76</v>
+      </c>
+      <c r="BG44" s="13">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="45" spans="2:118" x14ac:dyDescent="0.2">
+      <c r="B45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P45" s="4">
+        <f>+P46-P59</f>
+        <v>18829</v>
+      </c>
+      <c r="Q45" s="4">
+        <f>+P45+Q33</f>
+        <v>26816.66249999998</v>
+      </c>
+      <c r="R45" s="4">
+        <f>+Q45+R33</f>
+        <v>34403.515999999981</v>
+      </c>
+      <c r="S45" s="4">
+        <f>+R45+S33</f>
+        <v>43398.725999999995</v>
+      </c>
+      <c r="T45" s="4">
+        <f>+S45+T33</f>
+        <v>51683.939500000008</v>
+      </c>
+      <c r="U45" s="4">
+        <f>+T45+U33</f>
+        <v>64201.153400000017</v>
+      </c>
+      <c r="V45" s="4">
+        <f>+U45+V33</f>
+        <v>76467.199525000004</v>
+      </c>
+      <c r="W45" s="4">
+        <f>+V45+W33</f>
+        <v>90850.0389</v>
+      </c>
+      <c r="X45" s="4"/>
+      <c r="AV45" s="2">
+        <f>+S45</f>
+        <v>43398.725999999995</v>
+      </c>
+      <c r="AW45" s="2">
+        <f>+W45</f>
+        <v>90850.0389</v>
+      </c>
+      <c r="AX45" s="2">
+        <f>+AW45+AX33</f>
+        <v>154994.70740564988</v>
+      </c>
+      <c r="AY45" s="2">
+        <f t="shared" ref="AY45:BD45" si="204">+AX45+AY33</f>
+        <v>239163.48435024795</v>
+      </c>
+      <c r="AZ45" s="2">
+        <f t="shared" si="204"/>
+        <v>347998.04798539454</v>
+      </c>
+      <c r="BA45" s="2">
+        <f t="shared" si="204"/>
+        <v>487351.55465635349</v>
+      </c>
+      <c r="BB45" s="2">
+        <f t="shared" si="204"/>
+        <v>650197.45795578789</v>
+      </c>
+      <c r="BC45" s="2">
+        <f t="shared" si="204"/>
+        <v>840567.6347757217</v>
+      </c>
+      <c r="BD45" s="2">
+        <f t="shared" si="204"/>
+        <v>1063251.7771376492</v>
+      </c>
+      <c r="BF45" t="s">
+        <v>78</v>
+      </c>
+      <c r="BG45" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:118" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4">
+        <f>36393+29992</f>
+        <v>66385</v>
+      </c>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="BF46" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="BG46" s="2">
+        <f>NPV(BG43,AW33:DN33)+Main!K5-Main!K6</f>
+        <v>2550544.6921945531</v>
+      </c>
+    </row>
+    <row r="47" spans="2:118" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4">
+        <v>34987</v>
+      </c>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="BG47" s="1">
+        <f>+BG46/Main!K3</f>
+        <v>250.54466524504451</v>
+      </c>
+    </row>
+    <row r="48" spans="2:118" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4">
+        <v>32504</v>
+      </c>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+    </row>
+    <row r="49" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4"/>
+      <c r="M49" s="4"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4">
+        <v>168468</v>
+      </c>
+      <c r="Q49" s="4"/>
+      <c r="R49" s="4"/>
+      <c r="S49" s="4"/>
+    </row>
+    <row r="50" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4">
+        <v>56161</v>
+      </c>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+    </row>
+    <row r="51" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4">
+        <v>20229</v>
+      </c>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+    </row>
+    <row r="52" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="4"/>
+      <c r="L52" s="4"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="4"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="4">
+        <v>32033</v>
+      </c>
+      <c r="Q52" s="4"/>
+      <c r="R52" s="4"/>
+      <c r="S52" s="4"/>
+    </row>
+    <row r="53" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="4"/>
+      <c r="L53" s="4"/>
+      <c r="M53" s="4"/>
+      <c r="N53" s="4"/>
+      <c r="O53" s="4"/>
+      <c r="P53" s="4">
+        <f>SUM(P46:P52)</f>
+        <v>410767</v>
+      </c>
+      <c r="Q53" s="4"/>
+      <c r="R53" s="4"/>
+      <c r="S53" s="4"/>
+    </row>
+    <row r="55" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+      <c r="O55" s="4"/>
+      <c r="P55" s="4">
+        <v>68547</v>
+      </c>
+      <c r="Q55" s="4"/>
+      <c r="R55" s="4"/>
+      <c r="S55" s="4"/>
+    </row>
+    <row r="56" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4">
+        <v>58141</v>
+      </c>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+    </row>
+    <row r="57" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4">
+        <v>12820</v>
+      </c>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+    </row>
+    <row r="58" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="4"/>
+      <c r="L58" s="4"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="4"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="4">
+        <v>65731</v>
+      </c>
+      <c r="Q58" s="4"/>
+      <c r="R58" s="4"/>
+      <c r="S58" s="4"/>
+    </row>
+    <row r="59" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="4"/>
+      <c r="L59" s="4"/>
+      <c r="M59" s="4"/>
+      <c r="N59" s="4"/>
+      <c r="O59" s="4"/>
+      <c r="P59" s="4">
+        <v>47556</v>
+      </c>
+      <c r="Q59" s="4"/>
+      <c r="R59" s="4"/>
+      <c r="S59" s="4"/>
+    </row>
+    <row r="60" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="L60" s="4"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="4"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4">
+        <v>23971</v>
+      </c>
+      <c r="Q60" s="4"/>
+      <c r="R60" s="4"/>
+      <c r="S60" s="4"/>
+    </row>
+    <row r="61" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="L61" s="4"/>
+      <c r="M61" s="4"/>
+      <c r="N61" s="4"/>
+      <c r="O61" s="4"/>
+      <c r="P61" s="4">
+        <v>134001</v>
+      </c>
+      <c r="Q61" s="4"/>
+      <c r="R61" s="4"/>
+      <c r="S61" s="4"/>
+    </row>
+    <row r="62" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="4"/>
+      <c r="L62" s="4"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="4"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="4">
+        <f>SUM(P55:P61)</f>
+        <v>410767</v>
+      </c>
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="4"/>
     </row>
     <row r="66" spans="2:19" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">

</xml_diff>

<commit_message>
long time since update
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D9214A-2BA4-4E7C-8D00-70EAC56632DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8768B91-9F6B-463B-A22F-CE35B404C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18975" yWindow="1875" windowWidth="32715" windowHeight="15915" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -457,12 +457,6 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -975,9 +969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E919ED4-9952-4C3B-8FDF-EC99BCC4C526}">
   <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
-    </sheetView>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1049,6 +1041,9 @@
         <v>1015174.44</v>
       </c>
       <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
       <c r="J9" t="s">
@@ -1064,11 +1059,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5282D4FF-6525-4291-9B79-B00D62C08099}">
   <dimension ref="A1:DS101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="O40" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="N13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S64" sqref="S64"/>
+      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2725,7 +2720,7 @@
         <v>125730.72</v>
       </c>
       <c r="U21" s="6">
-        <f t="shared" ref="S21:W21" si="29">SUM(U10:U17)</f>
+        <f t="shared" ref="U21:W21" si="29">SUM(U10:U17)</f>
         <v>131075.60999999999</v>
       </c>
       <c r="V21" s="6">
@@ -4377,7 +4372,7 @@
         <v>0</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" ref="S32:W32" si="99">+T31*0.15</f>
+        <f t="shared" ref="T32:W32" si="99">+T31*0.15</f>
         <v>1438.7136599999994</v>
       </c>
       <c r="U32" s="4">
@@ -5079,7 +5074,7 @@
         <v>10308</v>
       </c>
       <c r="T35" s="4">
-        <f t="shared" ref="S35:W35" si="137">+S35</f>
+        <f t="shared" ref="T35:W35" si="137">+S35</f>
         <v>10308</v>
       </c>
       <c r="U35" s="4">
@@ -6073,7 +6068,7 @@
         <v>0.20236220472440936</v>
       </c>
       <c r="T44" s="8">
-        <f t="shared" ref="S44:W44" si="204">T10/P10-1</f>
+        <f t="shared" ref="T44:W44" si="204">T10/P10-1</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="U44" s="8">

</xml_diff>

<commit_message>
update MSFT AMZN GOOG NVDA
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93765436-BF10-48DF-960E-30475572B74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6834718-ED16-4A6A-966F-8F48972AA228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="-27930" yWindow="75" windowWidth="27825" windowHeight="19425" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -38,17 +38,28 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={25D31764-16FB-4D93-B4DD-0EA3D148D991}</author>
     <author>tc={89E45B5F-0C20-4B81-874E-AD8DF93707A2}</author>
     <author>tc={9EC27BD9-44A2-48E9-9E13-C02A116B6B0B}</author>
     <author>tc={1C7E52D4-5BCB-4AA9-9278-E6CDC311AA1D}</author>
     <author>tc={D82076A3-F6B1-40A8-A09D-2B367ECEDED9}</author>
+    <author>tc={4F53D287-EDAA-4481-ACF6-A09E2F7614C4}</author>
     <author>tc={BC0611F9-311A-4928-9AD6-94F49AE6B822}</author>
     <author>tc={1123E429-DC3C-402F-A940-60A8A504E208}</author>
     <author>tc={F0CECC32-58CA-41B9-9B42-426709AD1A9F}</author>
+    <author>tc={EEC432E6-C1EF-4C03-8D2E-1AD7704A7DFC}</author>
     <author>tc={7DD33F83-8D06-4AB5-AE42-CC8AE1143AEE}</author>
   </authors>
   <commentList>
-    <comment ref="R20" authorId="0" shapeId="0" xr:uid="{89E45B5F-0C20-4B81-874E-AD8DF93707A2}">
+    <comment ref="U9" authorId="0" shapeId="0" xr:uid="{25D31764-16FB-4D93-B4DD-0EA3D148D991}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    I estimated 23.7B prior to results</t>
+      </text>
+    </comment>
+    <comment ref="R20" authorId="1" shapeId="0" xr:uid="{89E45B5F-0C20-4B81-874E-AD8DF93707A2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +67,7 @@
     Q222 guidance: 125-130B</t>
       </text>
     </comment>
-    <comment ref="S20" authorId="1" shapeId="0" xr:uid="{9EC27BD9-44A2-48E9-9E13-C02A116B6B0B}">
+    <comment ref="S20" authorId="2" shapeId="0" xr:uid="{9EC27BD9-44A2-48E9-9E13-C02A116B6B0B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -64,7 +75,7 @@
     Q3 guidance: 140-148B</t>
       </text>
     </comment>
-    <comment ref="T20" authorId="2" shapeId="0" xr:uid="{1C7E52D4-5BCB-4AA9-9278-E6CDC311AA1D}">
+    <comment ref="T20" authorId="3" shapeId="0" xr:uid="{1C7E52D4-5BCB-4AA9-9278-E6CDC311AA1D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +83,7 @@
     Q422 guidance: 121-126B</t>
       </text>
     </comment>
-    <comment ref="U20" authorId="3" shapeId="0" xr:uid="{D82076A3-F6B1-40A8-A09D-2B367ECEDED9}">
+    <comment ref="U20" authorId="4" shapeId="0" xr:uid="{D82076A3-F6B1-40A8-A09D-2B367ECEDED9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -80,7 +91,16 @@
     Q123 guidance: 127-133B</t>
       </text>
     </comment>
-    <comment ref="R28" authorId="4" shapeId="0" xr:uid="{BC0611F9-311A-4928-9AD6-94F49AE6B822}">
+    <comment ref="V20" authorId="5" shapeId="0" xr:uid="{4F53D287-EDAA-4481-ACF6-A09E2F7614C4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Q223 guidance: 138B-143B
+I estimated 135B prior to guidance</t>
+      </text>
+    </comment>
+    <comment ref="R28" authorId="6" shapeId="0" xr:uid="{BC0611F9-311A-4928-9AD6-94F49AE6B822}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -88,7 +108,7 @@
     Q222 guidance: 0.0-3.5B</t>
       </text>
     </comment>
-    <comment ref="S28" authorId="5" shapeId="0" xr:uid="{1123E429-DC3C-402F-A940-60A8A504E208}">
+    <comment ref="S28" authorId="7" shapeId="0" xr:uid="{1123E429-DC3C-402F-A940-60A8A504E208}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -96,7 +116,7 @@
     Q3 guidance: 0-4B</t>
       </text>
     </comment>
-    <comment ref="T28" authorId="6" shapeId="0" xr:uid="{F0CECC32-58CA-41B9-9B42-426709AD1A9F}">
+    <comment ref="T28" authorId="8" shapeId="0" xr:uid="{F0CECC32-58CA-41B9-9B42-426709AD1A9F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -104,7 +124,16 @@
     Q4 guidance 0-4B</t>
       </text>
     </comment>
-    <comment ref="R36" authorId="7" shapeId="0" xr:uid="{7DD33F83-8D06-4AB5-AE42-CC8AE1143AEE}">
+    <comment ref="U28" authorId="9" shapeId="0" xr:uid="{EEC432E6-C1EF-4C03-8D2E-1AD7704A7DFC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Q223 guidance: 5.5-8.5B
+I estimated 5.6B prior to guidance</t>
+      </text>
+    </comment>
+    <comment ref="R36" authorId="10" shapeId="0" xr:uid="{7DD33F83-8D06-4AB5-AE42-CC8AE1143AEE}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -450,7 +479,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -469,6 +498,12 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -551,16 +586,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>15648</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>35355</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>39120</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>15648</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>35355</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>48645</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -575,8 +610,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12550548" y="39120"/>
-          <a:ext cx="0" cy="17317811"/>
+          <a:off x="13206131" y="0"/>
+          <a:ext cx="0" cy="17417284"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -955,6 +990,9 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="U9" dT="2023-08-16T02:08:15.29" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{25D31764-16FB-4D93-B4DD-0EA3D148D991}">
+    <text>I estimated 23.7B prior to results</text>
+  </threadedComment>
   <threadedComment ref="R20" dT="2022-07-29T15:08:40.16" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{89E45B5F-0C20-4B81-874E-AD8DF93707A2}">
     <text>Q222 guidance: 125-130B</text>
   </threadedComment>
@@ -967,6 +1005,10 @@
   <threadedComment ref="U20" dT="2023-04-30T02:01:08.68" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{D82076A3-F6B1-40A8-A09D-2B367ECEDED9}">
     <text>Q123 guidance: 127-133B</text>
   </threadedComment>
+  <threadedComment ref="V20" dT="2023-08-16T02:05:55.59" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{4F53D287-EDAA-4481-ACF6-A09E2F7614C4}">
+    <text>Q223 guidance: 138B-143B
+I estimated 135B prior to guidance</text>
+  </threadedComment>
   <threadedComment ref="R28" dT="2022-07-29T15:10:25.65" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{BC0611F9-311A-4928-9AD6-94F49AE6B822}">
     <text>Q222 guidance: 0.0-3.5B</text>
   </threadedComment>
@@ -975,6 +1017,10 @@
   </threadedComment>
   <threadedComment ref="T28" dT="2023-02-09T23:51:52.21" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{F0CECC32-58CA-41B9-9B42-426709AD1A9F}">
     <text>Q4 guidance 0-4B</text>
+  </threadedComment>
+  <threadedComment ref="U28" dT="2023-08-16T02:06:13.82" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{EEC432E6-C1EF-4C03-8D2E-1AD7704A7DFC}">
+    <text>Q223 guidance: 5.5-8.5B
+I estimated 5.6B prior to guidance</text>
   </threadedComment>
   <threadedComment ref="R36" dT="2022-12-19T01:32:23.85" personId="{9B8D1A3E-D1D5-4929-A5A0-67791399E886}" id="{7DD33F83-8D06-4AB5-AE42-CC8AE1143AEE}">
     <text>+19% net of FX</text>
@@ -1076,11 +1122,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5282D4FF-6525-4291-9B79-B00D62C08099}">
   <dimension ref="A1:DS100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="295" zoomScaleNormal="295" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="L75" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="J54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="Q89" sqref="Q89:T91"/>
+      <selection pane="bottomRight" activeCell="L75" sqref="L75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1396,6 +1442,9 @@
       </c>
       <c r="T3" s="2">
         <v>76881</v>
+      </c>
+      <c r="U3" s="2">
+        <v>82546</v>
       </c>
       <c r="AS3" s="2">
         <v>50834</v>
@@ -1545,6 +1594,9 @@
       <c r="T6" s="2">
         <v>29123</v>
       </c>
+      <c r="U6" s="2">
+        <v>29697</v>
+      </c>
       <c r="AS6" s="2">
         <v>33510</v>
       </c>
@@ -1694,8 +1746,7 @@
         <v>21354</v>
       </c>
       <c r="U9" s="4">
-        <f>+Q9*1.2</f>
-        <v>23686.799999999999</v>
+        <v>22140</v>
       </c>
       <c r="V9" s="4">
         <f>+R9*1.2</f>
@@ -1738,35 +1789,35 @@
       </c>
       <c r="BB9" s="2">
         <f>SUM(T9:W9)</f>
-        <v>95340</v>
+        <v>93793.200000000012</v>
       </c>
       <c r="BC9" s="2">
         <f>+BB9*1.3</f>
-        <v>123942</v>
+        <v>121931.16000000002</v>
       </c>
       <c r="BD9" s="2">
         <f t="shared" ref="BD9:BF9" si="3">+BC9*1.3</f>
-        <v>161124.6</v>
+        <v>158510.50800000003</v>
       </c>
       <c r="BE9" s="2">
         <f t="shared" si="3"/>
-        <v>209461.98</v>
+        <v>206063.66040000005</v>
       </c>
       <c r="BF9" s="2">
         <f t="shared" si="3"/>
-        <v>272300.57400000002</v>
+        <v>267882.75852000009</v>
       </c>
       <c r="BG9" s="2">
         <f>+BF9*1.2</f>
-        <v>326760.6888</v>
+        <v>321459.31022400007</v>
       </c>
       <c r="BH9" s="2">
         <f t="shared" ref="BH9:BI9" si="4">+BG9*1.2</f>
-        <v>392112.82656000002</v>
+        <v>385751.17226880009</v>
       </c>
       <c r="BI9" s="2">
         <f t="shared" si="4"/>
-        <v>470535.39187200001</v>
+        <v>462901.40672256012</v>
       </c>
     </row>
     <row r="11" spans="1:71" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2563,6 +2614,9 @@
       <c r="T18" s="2">
         <v>56981</v>
       </c>
+      <c r="U18" s="2">
+        <v>59032</v>
+      </c>
       <c r="AV18" s="2">
         <v>118573</v>
       </c>
@@ -2640,6 +2694,9 @@
       <c r="T19" s="2">
         <v>70377</v>
       </c>
+      <c r="U19" s="2">
+        <v>75351</v>
+      </c>
       <c r="AV19" s="2">
         <v>59293</v>
       </c>
@@ -2736,8 +2793,8 @@
         <v>127358</v>
       </c>
       <c r="U20" s="6">
-        <f>SUM(U9:U16)</f>
-        <v>129101.70999999999</v>
+        <f>+U18+U19</f>
+        <v>134383</v>
       </c>
       <c r="V20" s="6">
         <f t="shared" ref="V20:W20" si="29">SUM(V9:V16)</f>
@@ -2842,35 +2899,35 @@
       </c>
       <c r="BB20" s="5">
         <f>SUM(BB9:BB16)</f>
-        <v>550196.52</v>
+        <v>548649.72</v>
       </c>
       <c r="BC20" s="5">
         <f t="shared" ref="BC20:BI20" si="33">SUM(BC9:BC16)</f>
-        <v>605589.68800000008</v>
+        <v>603578.84800000011</v>
       </c>
       <c r="BD20" s="5">
         <f t="shared" si="33"/>
-        <v>671307.84860000014</v>
+        <v>668693.75659999996</v>
       </c>
       <c r="BE20" s="5">
         <f t="shared" si="33"/>
-        <v>750052.88485000003</v>
+        <v>746654.5652500001</v>
       </c>
       <c r="BF20" s="5">
         <f t="shared" si="33"/>
-        <v>845309.3672945</v>
+        <v>840891.55181450013</v>
       </c>
       <c r="BG20" s="5">
         <f t="shared" si="33"/>
-        <v>928419.92175922508</v>
+        <v>923118.54318322521</v>
       </c>
       <c r="BH20" s="5">
         <f t="shared" si="33"/>
-        <v>1023855.0211671864</v>
+        <v>1017493.3668759866</v>
       </c>
       <c r="BI20" s="5">
         <f t="shared" si="33"/>
-        <v>1133864.6962095457</v>
+        <v>1126230.7110601058</v>
       </c>
     </row>
     <row r="21" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2932,11 +2989,10 @@
         <v>67791</v>
       </c>
       <c r="U21" s="4">
-        <f t="shared" ref="U21:W21" si="34">SUM(U11:U13)*0.68+U9*0.5</f>
-        <v>69846.67240000001</v>
+        <v>69373</v>
       </c>
       <c r="V21" s="4">
-        <f t="shared" si="34"/>
+        <f t="shared" ref="U21:W21" si="34">SUM(V11:V13)*0.68+V9*0.5</f>
         <v>73056.081999999995</v>
       </c>
       <c r="W21" s="4">
@@ -2985,35 +3041,35 @@
       </c>
       <c r="BB21" s="2">
         <f>SUM(T21:W21)</f>
-        <v>297540.66240000003</v>
+        <v>297066.99</v>
       </c>
       <c r="BC21" s="4">
         <f t="shared" ref="BC21:BI21" si="35">SUM(BC11:BC13)*0.8+BC9*0.7</f>
-        <v>396951.8112</v>
+        <v>395544.22320000001</v>
       </c>
       <c r="BD21" s="4">
         <f t="shared" si="35"/>
-        <v>438489.25176000013</v>
+        <v>436659.38736000011</v>
       </c>
       <c r="BE21" s="4">
         <f t="shared" si="35"/>
-        <v>488610.51934800006</v>
+        <v>486231.69562800007</v>
       </c>
       <c r="BF21" s="4">
         <f t="shared" si="35"/>
-        <v>549696.8918154001</v>
+        <v>546604.42097940017</v>
       </c>
       <c r="BG21" s="4">
         <f t="shared" si="35"/>
-        <v>605773.29667617008</v>
+        <v>602062.33167297021</v>
       </c>
       <c r="BH21" s="4">
         <f t="shared" si="35"/>
-        <v>670371.83383397863</v>
+        <v>665918.67583013873</v>
       </c>
       <c r="BI21" s="4">
         <f t="shared" si="35"/>
-        <v>745062.27231447748</v>
+        <v>739718.48270986951</v>
       </c>
     </row>
     <row r="22" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3075,11 +3131,10 @@
         <v>20905</v>
       </c>
       <c r="U22" s="4">
-        <f t="shared" ref="U22:W22" si="36">(U13+U11)*0.25</f>
-        <v>20144.482500000002</v>
+        <v>21305</v>
       </c>
       <c r="V22" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="U22:W22" si="36">(V13+V11)*0.25</f>
         <v>21154.912499999999</v>
       </c>
       <c r="W22" s="4">
@@ -3128,7 +3183,7 @@
       </c>
       <c r="BB22" s="2">
         <f>SUM(T22:W22)</f>
-        <v>88178.42</v>
+        <v>89338.9375</v>
       </c>
       <c r="BC22" s="4">
         <f t="shared" ref="BC22:BI22" si="37">(BC13+BC11)*0.1</f>
@@ -3237,7 +3292,7 @@
       </c>
       <c r="U23" s="4">
         <f t="shared" si="44"/>
-        <v>39110.555099999983</v>
+        <v>43705</v>
       </c>
       <c r="V23" s="4">
         <f t="shared" si="44"/>
@@ -3297,35 +3352,35 @@
       </c>
       <c r="BB23" s="4">
         <f t="shared" si="47"/>
-        <v>164477.4376</v>
+        <v>162243.79249999998</v>
       </c>
       <c r="BC23" s="4">
         <f t="shared" si="47"/>
-        <v>171886.86040000009</v>
+        <v>171283.60840000011</v>
       </c>
       <c r="BD23" s="4">
         <f t="shared" si="47"/>
-        <v>194230.02962000002</v>
+        <v>193445.80201999986</v>
       </c>
       <c r="BE23" s="4">
         <f t="shared" si="47"/>
-        <v>220924.36992099998</v>
+        <v>219904.87404100003</v>
       </c>
       <c r="BF23" s="4">
         <f t="shared" si="47"/>
-        <v>253068.58011904988</v>
+        <v>251743.23547504994</v>
       </c>
       <c r="BG23" s="4">
         <f t="shared" si="47"/>
-        <v>277975.53495500248</v>
+        <v>276385.12138220249</v>
       </c>
       <c r="BH23" s="4">
         <f t="shared" si="47"/>
-        <v>306578.54269875266</v>
+        <v>304670.04641139269</v>
       </c>
       <c r="BI23" s="4">
         <f t="shared" si="47"/>
-        <v>339552.54702889035</v>
+        <v>337262.35148405842</v>
       </c>
     </row>
     <row r="24" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3387,11 +3442,10 @@
         <v>20450</v>
       </c>
       <c r="U24" s="4">
-        <f t="shared" ref="U24:W24" si="48">+Q24*1.1</f>
-        <v>19879.2</v>
+        <v>21931</v>
       </c>
       <c r="V24" s="4">
-        <f t="shared" si="48"/>
+        <f t="shared" ref="U24:W24" si="48">+R24*1.1</f>
         <v>21433.5</v>
       </c>
       <c r="W24" s="4">
@@ -3440,35 +3494,35 @@
       </c>
       <c r="BB24" s="2">
         <f>SUM(T24:W24)</f>
-        <v>84658.1</v>
+        <v>86709.9</v>
       </c>
       <c r="BC24" s="2">
         <f>+BB24*1.03</f>
-        <v>87197.843000000008</v>
+        <v>89311.197</v>
       </c>
       <c r="BD24" s="2">
         <f t="shared" ref="BD24:BI24" si="49">+BC24*1.03</f>
-        <v>89813.778290000017</v>
+        <v>91990.532910000009</v>
       </c>
       <c r="BE24" s="2">
         <f t="shared" si="49"/>
-        <v>92508.191638700024</v>
+        <v>94750.248897300015</v>
       </c>
       <c r="BF24" s="2">
         <f t="shared" si="49"/>
-        <v>95283.43738786102</v>
+        <v>97592.756364219022</v>
       </c>
       <c r="BG24" s="2">
         <f t="shared" si="49"/>
-        <v>98141.940509496853</v>
+        <v>100520.53905514559</v>
       </c>
       <c r="BH24" s="2">
         <f t="shared" si="49"/>
-        <v>101086.19872478176</v>
+        <v>103536.15522679997</v>
       </c>
       <c r="BI24" s="2">
         <f t="shared" si="49"/>
-        <v>104118.78468652522</v>
+        <v>106642.23988360396</v>
       </c>
     </row>
     <row r="25" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3530,15 +3584,14 @@
         <v>10172</v>
       </c>
       <c r="U25" s="4">
-        <f t="shared" ref="U25:U26" si="50">+Q25*1.05</f>
-        <v>10590.300000000001</v>
+        <v>10745</v>
       </c>
       <c r="V25" s="4">
-        <f t="shared" ref="V25:V26" si="51">+R25*1.05</f>
+        <f t="shared" ref="V25:V26" si="50">+R25*1.05</f>
         <v>11564.7</v>
       </c>
       <c r="W25" s="4">
-        <f t="shared" ref="W25:W26" si="52">+S25*1.05</f>
+        <f t="shared" ref="W25:W26" si="51">+S25*1.05</f>
         <v>13458.900000000001</v>
       </c>
       <c r="AF25" s="2">
@@ -3583,35 +3636,35 @@
       </c>
       <c r="BB25" s="2">
         <f>SUM(T25:W25)</f>
-        <v>45785.900000000009</v>
+        <v>45940.600000000006</v>
       </c>
       <c r="BC25" s="2">
-        <f t="shared" ref="BC25:BI25" si="53">+BB25*1.03</f>
-        <v>47159.477000000014</v>
+        <f t="shared" ref="BC25:BI25" si="52">+BB25*1.03</f>
+        <v>47318.818000000007</v>
       </c>
       <c r="BD25" s="2">
-        <f t="shared" si="53"/>
-        <v>48574.261310000016</v>
+        <f t="shared" si="52"/>
+        <v>48738.382540000006</v>
       </c>
       <c r="BE25" s="2">
-        <f t="shared" si="53"/>
-        <v>50031.489149300018</v>
+        <f t="shared" si="52"/>
+        <v>50200.534016200007</v>
       </c>
       <c r="BF25" s="2">
-        <f t="shared" si="53"/>
-        <v>51532.433823779022</v>
+        <f t="shared" si="52"/>
+        <v>51706.550036686007</v>
       </c>
       <c r="BG25" s="2">
-        <f t="shared" si="53"/>
-        <v>53078.406838492396</v>
+        <f t="shared" si="52"/>
+        <v>53257.746537786588</v>
       </c>
       <c r="BH25" s="2">
-        <f t="shared" si="53"/>
-        <v>54670.759043647166</v>
+        <f t="shared" si="52"/>
+        <v>54855.478933920189</v>
       </c>
       <c r="BI25" s="2">
-        <f t="shared" si="53"/>
-        <v>56310.881814956585</v>
+        <f t="shared" si="52"/>
+        <v>56501.143301937795</v>
       </c>
     </row>
     <row r="26" spans="2:123" x14ac:dyDescent="0.2">
@@ -3673,15 +3726,14 @@
         <v>3043</v>
       </c>
       <c r="U26" s="4">
+        <v>3202</v>
+      </c>
+      <c r="V26" s="4">
         <f t="shared" si="50"/>
-        <v>3048.15</v>
-      </c>
-      <c r="V26" s="4">
+        <v>3214.05</v>
+      </c>
+      <c r="W26" s="4">
         <f t="shared" si="51"/>
-        <v>3214.05</v>
-      </c>
-      <c r="W26" s="4">
-        <f t="shared" si="52"/>
         <v>3499.65</v>
       </c>
       <c r="AF26" s="2">
@@ -3726,35 +3778,35 @@
       </c>
       <c r="BB26" s="2">
         <f>SUM(T26:W26)</f>
-        <v>12804.85</v>
+        <v>12958.699999999999</v>
       </c>
       <c r="BC26" s="2">
-        <f t="shared" ref="BC26:BI26" si="54">+BB26*1.03</f>
-        <v>13188.995500000001</v>
+        <f t="shared" ref="BC26:BI26" si="53">+BB26*1.03</f>
+        <v>13347.460999999999</v>
       </c>
       <c r="BD26" s="2">
-        <f t="shared" si="54"/>
-        <v>13584.665365000001</v>
+        <f t="shared" si="53"/>
+        <v>13747.884829999999</v>
       </c>
       <c r="BE26" s="2">
-        <f t="shared" si="54"/>
-        <v>13992.205325950001</v>
+        <f t="shared" si="53"/>
+        <v>14160.321374899999</v>
       </c>
       <c r="BF26" s="2">
-        <f t="shared" si="54"/>
-        <v>14411.971485728502</v>
+        <f t="shared" si="53"/>
+        <v>14585.131016146999</v>
       </c>
       <c r="BG26" s="2">
-        <f t="shared" si="54"/>
-        <v>14844.330630300357</v>
+        <f t="shared" si="53"/>
+        <v>15022.684946631409</v>
       </c>
       <c r="BH26" s="2">
-        <f t="shared" si="54"/>
-        <v>15289.660549209368</v>
+        <f t="shared" si="53"/>
+        <v>15473.365495030352</v>
       </c>
       <c r="BI26" s="2">
-        <f t="shared" si="54"/>
-        <v>15748.350365685648</v>
+        <f t="shared" si="53"/>
+        <v>15937.566459881262</v>
       </c>
     </row>
     <row r="27" spans="2:123" x14ac:dyDescent="0.2">
@@ -3762,7 +3814,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" ref="C27" si="55">SUM(C24:C26)</f>
+        <f t="shared" ref="C27" si="54">SUM(C24:C26)</f>
         <v>13697</v>
       </c>
       <c r="D27" s="4">
@@ -3770,7 +3822,7 @@
         <v>12764</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27" si="56">SUM(E24:E26)</f>
+        <f t="shared" ref="E27" si="55">SUM(E24:E26)</f>
         <v>14626</v>
       </c>
       <c r="F27" s="4">
@@ -3778,15 +3830,15 @@
         <v>15300</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" ref="G27" si="57">SUM(G24:G26)</f>
+        <f t="shared" ref="G27" si="56">SUM(G24:G26)</f>
         <v>17324</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" ref="H27" si="58">SUM(H24:H26)</f>
+        <f t="shared" ref="H27" si="57">SUM(H24:H26)</f>
         <v>15605</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" ref="I27" si="59">SUM(I24:I26)</f>
+        <f t="shared" ref="I27" si="58">SUM(I24:I26)</f>
         <v>16313</v>
       </c>
       <c r="J27" s="4">
@@ -3794,7 +3846,7 @@
         <v>18078</v>
       </c>
       <c r="K27" s="4">
-        <f t="shared" ref="K27" si="60">SUM(K24:K26)</f>
+        <f t="shared" ref="K27" si="59">SUM(K24:K26)</f>
         <v>21420</v>
       </c>
       <c r="L27" s="4">
@@ -3802,23 +3854,23 @@
         <v>20682</v>
       </c>
       <c r="M27" s="4">
-        <f t="shared" ref="M27:P27" si="61">SUM(M24:M26)</f>
+        <f t="shared" ref="M27:P27" si="60">SUM(M24:M26)</f>
         <v>23553</v>
       </c>
       <c r="N27" s="4">
-        <f t="shared" si="61"/>
+        <f t="shared" si="60"/>
         <v>24543</v>
       </c>
       <c r="O27" s="4">
-        <f t="shared" si="61"/>
+        <f t="shared" si="60"/>
         <v>28648</v>
       </c>
       <c r="P27" s="4">
-        <f t="shared" si="61"/>
+        <f t="shared" si="60"/>
         <v>25756</v>
       </c>
       <c r="Q27" s="4">
-        <f t="shared" ref="Q27:W27" si="62">SUM(Q24:Q26)</f>
+        <f t="shared" ref="Q27:W27" si="61">SUM(Q24:Q26)</f>
         <v>31061</v>
       </c>
       <c r="R27" s="4">
@@ -3826,23 +3878,23 @@
         <v>33560</v>
       </c>
       <c r="S27" s="4">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>36965</v>
       </c>
       <c r="T27" s="4">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>33665</v>
       </c>
       <c r="U27" s="4">
-        <f t="shared" si="62"/>
-        <v>33517.65</v>
+        <f t="shared" si="61"/>
+        <v>35878</v>
       </c>
       <c r="V27" s="4">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>36212.25</v>
       </c>
       <c r="W27" s="4">
-        <f t="shared" si="62"/>
+        <f t="shared" si="61"/>
         <v>39853.950000000004</v>
       </c>
       <c r="AF27" s="2">
@@ -3858,72 +3910,72 @@
         <v>418.89800000000002</v>
       </c>
       <c r="AS27" s="4">
-        <f t="shared" ref="AS27:AU27" si="63">SUM(AS24:AS26)</f>
+        <f t="shared" ref="AS27:AU27" si="62">SUM(AS24:AS26)</f>
         <v>15159</v>
       </c>
       <c r="AT27" s="4">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>19541</v>
       </c>
       <c r="AU27" s="4">
-        <f t="shared" si="63"/>
+        <f t="shared" si="62"/>
         <v>25750</v>
       </c>
       <c r="AV27" s="4">
-        <f t="shared" ref="AV27" si="64">SUM(AV24:AV26)</f>
+        <f t="shared" ref="AV27" si="63">SUM(AV24:AV26)</f>
         <v>36363</v>
       </c>
       <c r="AW27" s="4">
-        <f t="shared" ref="AW27:AX27" si="65">SUM(AW24:AW26)</f>
+        <f t="shared" ref="AW27:AX27" si="64">SUM(AW24:AW26)</f>
         <v>46987</v>
       </c>
       <c r="AX27" s="4">
+        <f t="shared" si="64"/>
+        <v>60014</v>
+      </c>
+      <c r="AY27" s="4">
+        <f t="shared" ref="AY27:AZ27" si="65">SUM(AY24:AY26)</f>
+        <v>71416</v>
+      </c>
+      <c r="AZ27" s="4">
         <f t="shared" si="65"/>
-        <v>60014</v>
-      </c>
-      <c r="AY27" s="4">
-        <f t="shared" ref="AY27:AZ27" si="66">SUM(AY24:AY26)</f>
-        <v>71416</v>
-      </c>
-      <c r="AZ27" s="4">
+        <v>97426</v>
+      </c>
+      <c r="BA27" s="4">
+        <f t="shared" ref="BA27:BB27" si="66">SUM(BA24:BA26)</f>
+        <v>127342</v>
+      </c>
+      <c r="BB27" s="4">
         <f t="shared" si="66"/>
-        <v>97426</v>
-      </c>
-      <c r="BA27" s="4">
-        <f t="shared" ref="BA27:BB27" si="67">SUM(BA24:BA26)</f>
-        <v>127342</v>
-      </c>
-      <c r="BB27" s="4">
+        <v>145609.20000000001</v>
+      </c>
+      <c r="BC27" s="4">
+        <f t="shared" ref="BC27:BI27" si="67">SUM(BC24:BC26)</f>
+        <v>149977.47600000002</v>
+      </c>
+      <c r="BD27" s="4">
         <f t="shared" si="67"/>
-        <v>143248.85</v>
-      </c>
-      <c r="BC27" s="4">
-        <f t="shared" ref="BC27:BI27" si="68">SUM(BC24:BC26)</f>
-        <v>147546.3155</v>
-      </c>
-      <c r="BD27" s="4">
-        <f t="shared" si="68"/>
-        <v>151972.70496500001</v>
+        <v>154476.80028000002</v>
       </c>
       <c r="BE27" s="4">
-        <f t="shared" si="68"/>
-        <v>156531.88611395005</v>
+        <f t="shared" si="67"/>
+        <v>159111.10428840003</v>
       </c>
       <c r="BF27" s="4">
-        <f t="shared" si="68"/>
-        <v>161227.84269736856</v>
+        <f t="shared" si="67"/>
+        <v>163884.43741705202</v>
       </c>
       <c r="BG27" s="4">
-        <f t="shared" si="68"/>
-        <v>166064.6779782896</v>
+        <f t="shared" si="67"/>
+        <v>168800.9705395636</v>
       </c>
       <c r="BH27" s="4">
-        <f t="shared" si="68"/>
-        <v>171046.61831763829</v>
+        <f t="shared" si="67"/>
+        <v>173864.99965575052</v>
       </c>
       <c r="BI27" s="4">
-        <f t="shared" si="68"/>
-        <v>176178.01686716746</v>
+        <f t="shared" si="67"/>
+        <v>179080.94964542301</v>
       </c>
     </row>
     <row r="28" spans="2:123" x14ac:dyDescent="0.2">
@@ -3931,7 +3983,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4">
-        <f t="shared" ref="C28" si="69">C23-C27</f>
+        <f t="shared" ref="C28" si="68">C23-C27</f>
         <v>3872</v>
       </c>
       <c r="D28" s="4">
@@ -3939,7 +3991,7 @@
         <v>4415</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" ref="E28" si="70">E23-E27</f>
+        <f t="shared" ref="E28" si="69">E23-E27</f>
         <v>3170</v>
       </c>
       <c r="F28" s="4">
@@ -3947,15 +3999,15 @@
         <v>3212</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" ref="G28" si="71">G23-G27</f>
+        <f t="shared" ref="G28" si="70">G23-G27</f>
         <v>3944</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" ref="H28" si="72">H23-H27</f>
+        <f t="shared" ref="H28" si="71">H23-H27</f>
         <v>4059</v>
       </c>
       <c r="I28" s="4">
-        <f t="shared" ref="I28" si="73">I23-I27</f>
+        <f t="shared" ref="I28" si="72">I23-I27</f>
         <v>6133</v>
       </c>
       <c r="J28" s="4">
@@ -3963,7 +4015,7 @@
         <v>6256</v>
       </c>
       <c r="K28" s="4">
-        <f t="shared" ref="K28" si="74">K23-K27</f>
+        <f t="shared" ref="K28" si="73">K23-K27</f>
         <v>6377</v>
       </c>
       <c r="L28" s="4">
@@ -3971,23 +4023,23 @@
         <v>8903</v>
       </c>
       <c r="M28" s="4">
-        <f t="shared" ref="M28:P28" si="75">M23-M27</f>
+        <f t="shared" ref="M28:P28" si="74">M23-M27</f>
         <v>7713</v>
       </c>
       <c r="N28" s="4">
-        <f t="shared" si="75"/>
+        <f t="shared" si="74"/>
         <v>4841</v>
       </c>
       <c r="O28" s="4">
-        <f t="shared" si="75"/>
+        <f t="shared" si="74"/>
         <v>3484</v>
       </c>
       <c r="P28" s="4">
-        <f t="shared" si="75"/>
+        <f t="shared" si="74"/>
         <v>3918</v>
       </c>
       <c r="Q28" s="4">
-        <f t="shared" ref="Q28:W28" si="76">Q23-Q27</f>
+        <f t="shared" ref="Q28:W28" si="75">Q23-Q27</f>
         <v>3407</v>
       </c>
       <c r="R28" s="4">
@@ -3995,7 +4047,7 @@
         <v>2690</v>
       </c>
       <c r="S28" s="4">
-        <f t="shared" si="76"/>
+        <f t="shared" si="75"/>
         <v>3496</v>
       </c>
       <c r="T28" s="4">
@@ -4003,15 +4055,15 @@
         <v>4997</v>
       </c>
       <c r="U28" s="4">
-        <f t="shared" si="76"/>
-        <v>5592.9050999999818</v>
+        <f t="shared" si="75"/>
+        <v>7827</v>
       </c>
       <c r="V28" s="4">
-        <f t="shared" si="76"/>
+        <f t="shared" si="75"/>
         <v>4917.0454999999856</v>
       </c>
       <c r="W28" s="4">
-        <f t="shared" si="76"/>
+        <f t="shared" si="75"/>
         <v>5721.6370000000024</v>
       </c>
       <c r="AF28" s="2">
@@ -4027,72 +4079,72 @@
         <v>361.23799999999972</v>
       </c>
       <c r="AS28" s="4">
-        <f t="shared" ref="AS28:AU28" si="77">AS23-AS27</f>
+        <f t="shared" ref="AS28:AU28" si="76">AS23-AS27</f>
         <v>311</v>
       </c>
       <c r="AT28" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="76"/>
         <v>2404</v>
       </c>
       <c r="AU28" s="4">
-        <f t="shared" si="77"/>
+        <f t="shared" si="76"/>
         <v>4353</v>
       </c>
       <c r="AV28" s="4">
-        <f t="shared" ref="AV28" si="78">AV23-AV27</f>
+        <f t="shared" ref="AV28" si="77">AV23-AV27</f>
         <v>4320</v>
       </c>
       <c r="AW28" s="4">
-        <f t="shared" ref="AW28:AX28" si="79">AW23-AW27</f>
+        <f t="shared" ref="AW28:AX28" si="78">AW23-AW27</f>
         <v>12717</v>
       </c>
       <c r="AX28" s="4">
+        <f t="shared" si="78"/>
+        <v>14741</v>
+      </c>
+      <c r="AY28" s="4">
+        <f t="shared" ref="AY28:AZ28" si="79">AY23-AY27</f>
+        <v>22825</v>
+      </c>
+      <c r="AZ28" s="4">
         <f t="shared" si="79"/>
-        <v>14741</v>
-      </c>
-      <c r="AY28" s="4">
-        <f t="shared" ref="AY28:AZ28" si="80">AY23-AY27</f>
-        <v>22825</v>
-      </c>
-      <c r="AZ28" s="4">
+        <v>24941</v>
+      </c>
+      <c r="BA28" s="4">
+        <f t="shared" ref="BA28:BB28" si="80">BA23-BA27</f>
+        <v>13511</v>
+      </c>
+      <c r="BB28" s="4">
         <f t="shared" si="80"/>
-        <v>24941</v>
-      </c>
-      <c r="BA28" s="4">
-        <f t="shared" ref="BA28:BB28" si="81">BA23-BA27</f>
-        <v>13511</v>
-      </c>
-      <c r="BB28" s="4">
+        <v>16634.59249999997</v>
+      </c>
+      <c r="BC28" s="4">
+        <f t="shared" ref="BC28:BI28" si="81">BC23-BC27</f>
+        <v>21306.13240000009</v>
+      </c>
+      <c r="BD28" s="4">
         <f t="shared" si="81"/>
-        <v>21228.587599999999</v>
-      </c>
-      <c r="BC28" s="4">
-        <f t="shared" ref="BC28:BI28" si="82">BC23-BC27</f>
-        <v>24340.544900000095</v>
-      </c>
-      <c r="BD28" s="4">
-        <f t="shared" si="82"/>
-        <v>42257.324655000004</v>
+        <v>38969.001739999832</v>
       </c>
       <c r="BE28" s="4">
-        <f t="shared" si="82"/>
-        <v>64392.483807049925</v>
+        <f t="shared" si="81"/>
+        <v>60793.769752599997</v>
       </c>
       <c r="BF28" s="4">
-        <f t="shared" si="82"/>
-        <v>91840.737421681319</v>
+        <f t="shared" si="81"/>
+        <v>87858.798057997919</v>
       </c>
       <c r="BG28" s="4">
-        <f t="shared" si="82"/>
-        <v>111910.85697671288</v>
+        <f t="shared" si="81"/>
+        <v>107584.15084263889</v>
       </c>
       <c r="BH28" s="4">
-        <f t="shared" si="82"/>
-        <v>135531.92438111437</v>
+        <f t="shared" si="81"/>
+        <v>130805.04675564216</v>
       </c>
       <c r="BI28" s="4">
-        <f t="shared" si="82"/>
-        <v>163374.53016172288</v>
+        <f t="shared" si="81"/>
+        <v>158181.40183863541</v>
       </c>
     </row>
     <row r="29" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4171,6 +4223,10 @@
         <f>-223+611-823-443</f>
         <v>-878</v>
       </c>
+      <c r="U29" s="2">
+        <f>-146+661-840+61</f>
+        <v>-264</v>
+      </c>
       <c r="AF29" s="2">
         <f>29.103-139.232</f>
         <v>-110.12899999999999</v>
@@ -4204,15 +4260,15 @@
         <v>-1456</v>
       </c>
       <c r="AX29" s="2">
-        <f t="shared" ref="AX29" si="83">SUM(D29:G29)</f>
+        <f t="shared" ref="AX29" si="82">SUM(D29:G29)</f>
         <v>-766</v>
       </c>
       <c r="AY29" s="2">
-        <f t="shared" ref="AY29" si="84">SUM(H29:K29)</f>
+        <f t="shared" ref="AY29" si="83">SUM(H29:K29)</f>
         <v>1353</v>
       </c>
       <c r="AZ29" s="2">
-        <f t="shared" ref="AZ29" si="85">SUM(L29:O29)</f>
+        <f t="shared" ref="AZ29" si="84">SUM(L29:O29)</f>
         <v>13210</v>
       </c>
       <c r="BA29" s="2">
@@ -4221,35 +4277,35 @@
       </c>
       <c r="BB29" s="2">
         <f>SUM(T29:W29)</f>
-        <v>-878</v>
+        <v>-1142</v>
       </c>
       <c r="BC29" s="2">
         <f>+BB46*$BL$45</f>
-        <v>111.17849459999974</v>
+        <v>99.208801249999894</v>
       </c>
       <c r="BD29" s="2">
-        <f t="shared" ref="BD29:BI29" si="86">+BC46*$BL$45</f>
-        <v>319.0181434541006</v>
+        <f t="shared" ref="BD29:BI29" si="85">+BC46*$BL$45</f>
+        <v>281.15420146062564</v>
       </c>
       <c r="BE29" s="2">
-        <f t="shared" si="86"/>
-        <v>680.91705724096039</v>
+        <f t="shared" si="85"/>
+        <v>614.78052696303951</v>
       </c>
       <c r="BF29" s="2">
-        <f t="shared" si="86"/>
-        <v>1234.0409645874331</v>
+        <f t="shared" si="85"/>
+        <v>1136.7532043393253</v>
       </c>
       <c r="BG29" s="2">
-        <f t="shared" si="86"/>
-        <v>2025.1765808707173</v>
+        <f t="shared" si="85"/>
+        <v>1893.2153900691919</v>
       </c>
       <c r="BH29" s="2">
-        <f t="shared" si="86"/>
-        <v>2993.6328661101779</v>
+        <f t="shared" si="85"/>
+        <v>2823.7730030472108</v>
       </c>
       <c r="BI29" s="2">
-        <f t="shared" si="86"/>
-        <v>4171.1001027115863</v>
+        <f t="shared" si="85"/>
+        <v>3959.6179709960702</v>
       </c>
     </row>
     <row r="30" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4257,7 +4313,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" ref="C30" si="87">C28+C29</f>
+        <f t="shared" ref="C30" si="86">C28+C29</f>
         <v>3350</v>
       </c>
       <c r="D30" s="4">
@@ -4265,7 +4321,7 @@
         <v>4401</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" ref="E30" si="88">E28+E29</f>
+        <f t="shared" ref="E30" si="87">E28+E29</f>
         <v>2889</v>
       </c>
       <c r="F30" s="4">
@@ -4273,15 +4329,15 @@
         <v>2632</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30" si="89">G28+G29</f>
+        <f t="shared" ref="G30" si="88">G28+G29</f>
         <v>4053</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" ref="H30" si="90">H28+H29</f>
+        <f t="shared" ref="H30" si="89">H28+H29</f>
         <v>3383</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" ref="I30" si="91">I28+I29</f>
+        <f t="shared" ref="I30" si="90">I28+I29</f>
         <v>6221</v>
       </c>
       <c r="J30" s="4">
@@ -4289,7 +4345,7 @@
         <v>6809</v>
       </c>
       <c r="K30" s="4">
-        <f t="shared" ref="K30" si="92">K28+K29</f>
+        <f t="shared" ref="K30" si="91">K28+K29</f>
         <v>7765</v>
       </c>
       <c r="L30" s="4">
@@ -4297,47 +4353,47 @@
         <v>10268</v>
       </c>
       <c r="M30" s="4">
-        <f t="shared" ref="M30:W30" si="93">M28+M29</f>
+        <f t="shared" ref="M30:W30" si="92">M28+M29</f>
         <v>8634</v>
       </c>
       <c r="N30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>4315</v>
       </c>
       <c r="O30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>14934</v>
       </c>
       <c r="P30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>-5265</v>
       </c>
       <c r="Q30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>2982</v>
       </c>
       <c r="R30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>2944</v>
       </c>
       <c r="S30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>3247</v>
       </c>
       <c r="T30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>4119</v>
       </c>
       <c r="U30" s="4">
-        <f t="shared" si="93"/>
-        <v>5592.9050999999818</v>
+        <f t="shared" si="92"/>
+        <v>7563</v>
       </c>
       <c r="V30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>4917.0454999999856</v>
       </c>
       <c r="W30" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="92"/>
         <v>5721.6370000000024</v>
       </c>
       <c r="AF30" s="2">
@@ -4353,72 +4409,72 @@
         <v>253.21399999999971</v>
       </c>
       <c r="AS30" s="4">
-        <f t="shared" ref="AS30:AU30" si="94">AS28+AS29</f>
+        <f t="shared" ref="AS30:AU30" si="93">AS28+AS29</f>
         <v>-111</v>
       </c>
       <c r="AT30" s="4">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>1568</v>
       </c>
       <c r="AU30" s="4">
-        <f t="shared" si="94"/>
+        <f t="shared" si="93"/>
         <v>3892</v>
       </c>
       <c r="AV30" s="4">
-        <f t="shared" ref="AV30" si="95">AV28+AV29</f>
+        <f t="shared" ref="AV30" si="94">AV28+AV29</f>
         <v>3806</v>
       </c>
       <c r="AW30" s="4">
-        <f t="shared" ref="AW30:AX30" si="96">AW28+AW29</f>
+        <f t="shared" ref="AW30:AX30" si="95">AW28+AW29</f>
         <v>11261</v>
       </c>
       <c r="AX30" s="4">
+        <f t="shared" si="95"/>
+        <v>13975</v>
+      </c>
+      <c r="AY30" s="4">
+        <f t="shared" ref="AY30:BI30" si="96">AY28+AY29</f>
+        <v>24178</v>
+      </c>
+      <c r="AZ30" s="4">
         <f t="shared" si="96"/>
-        <v>13975</v>
-      </c>
-      <c r="AY30" s="4">
-        <f t="shared" ref="AY30:BI30" si="97">AY28+AY29</f>
-        <v>24178</v>
-      </c>
-      <c r="AZ30" s="4">
-        <f t="shared" si="97"/>
         <v>38151</v>
       </c>
       <c r="BA30" s="4">
-        <f t="shared" si="97"/>
+        <f t="shared" si="96"/>
         <v>3908</v>
       </c>
       <c r="BB30" s="4">
-        <f t="shared" si="97"/>
-        <v>20350.587599999999</v>
+        <f t="shared" si="96"/>
+        <v>15492.59249999997</v>
       </c>
       <c r="BC30" s="4">
-        <f t="shared" si="97"/>
-        <v>24451.723394600096</v>
+        <f t="shared" si="96"/>
+        <v>21405.341201250088</v>
       </c>
       <c r="BD30" s="4">
-        <f t="shared" si="97"/>
-        <v>42576.342798454105</v>
+        <f t="shared" si="96"/>
+        <v>39250.155941460456</v>
       </c>
       <c r="BE30" s="4">
-        <f t="shared" si="97"/>
-        <v>65073.400864290888</v>
+        <f t="shared" si="96"/>
+        <v>61408.550279563038</v>
       </c>
       <c r="BF30" s="4">
-        <f t="shared" si="97"/>
-        <v>93074.77838626875</v>
+        <f t="shared" si="96"/>
+        <v>88995.551262337249</v>
       </c>
       <c r="BG30" s="4">
-        <f t="shared" si="97"/>
-        <v>113936.03355758359</v>
+        <f t="shared" si="96"/>
+        <v>109477.36623270808</v>
       </c>
       <c r="BH30" s="4">
-        <f t="shared" si="97"/>
-        <v>138525.55724722455</v>
+        <f t="shared" si="96"/>
+        <v>133628.81975868938</v>
       </c>
       <c r="BI30" s="4">
-        <f t="shared" si="97"/>
-        <v>167545.63026443447</v>
+        <f t="shared" si="96"/>
+        <v>162141.01980963149</v>
       </c>
     </row>
     <row r="31" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4496,15 +4552,15 @@
         <v>947</v>
       </c>
       <c r="U31" s="4">
-        <f t="shared" ref="U31:W31" si="98">+U30*0.15</f>
-        <v>838.93576499999722</v>
+        <f>804+9</f>
+        <v>813</v>
       </c>
       <c r="V31" s="4">
-        <f t="shared" si="98"/>
+        <f t="shared" ref="U31:W31" si="97">+V30*0.15</f>
         <v>737.55682499999784</v>
       </c>
       <c r="W31" s="4">
-        <f t="shared" si="98"/>
+        <f t="shared" si="97"/>
         <v>858.24555000000032</v>
       </c>
       <c r="AF31" s="2">
@@ -4537,15 +4593,15 @@
         <v>1188</v>
       </c>
       <c r="AX31" s="2">
-        <f t="shared" ref="AX31" si="99">SUM(D31:G31)</f>
+        <f t="shared" ref="AX31" si="98">SUM(D31:G31)</f>
         <v>2387</v>
       </c>
       <c r="AY31" s="2">
-        <f t="shared" ref="AY31" si="100">SUM(H31:K31)</f>
+        <f t="shared" ref="AY31" si="99">SUM(H31:K31)</f>
         <v>2847</v>
       </c>
       <c r="AZ31" s="2">
-        <f t="shared" ref="AZ31" si="101">SUM(L31:O31)</f>
+        <f t="shared" ref="AZ31" si="100">SUM(L31:O31)</f>
         <v>4787</v>
       </c>
       <c r="BA31" s="2">
@@ -4554,35 +4610,35 @@
       </c>
       <c r="BB31" s="2">
         <f>SUM(T31:W31)</f>
-        <v>3381.7381399999958</v>
+        <v>3355.8023749999984</v>
       </c>
       <c r="BC31" s="2">
         <f>+BC30*0.15</f>
-        <v>3667.7585091900141</v>
+        <v>3210.8011801875132</v>
       </c>
       <c r="BD31" s="2">
-        <f t="shared" ref="BD31:BI31" si="102">+BD30*0.15</f>
-        <v>6386.4514197681156</v>
+        <f t="shared" ref="BD31:BI31" si="101">+BD30*0.15</f>
+        <v>5887.5233912190679</v>
       </c>
       <c r="BE31" s="2">
-        <f t="shared" si="102"/>
-        <v>9761.0101296436333</v>
+        <f t="shared" si="101"/>
+        <v>9211.2825419344554</v>
       </c>
       <c r="BF31" s="2">
-        <f t="shared" si="102"/>
-        <v>13961.216757940312</v>
+        <f t="shared" si="101"/>
+        <v>13349.332689350587</v>
       </c>
       <c r="BG31" s="2">
-        <f t="shared" si="102"/>
-        <v>17090.405033637537</v>
+        <f t="shared" si="101"/>
+        <v>16421.604934906212</v>
       </c>
       <c r="BH31" s="2">
-        <f t="shared" si="102"/>
-        <v>20778.833587083682</v>
+        <f t="shared" si="101"/>
+        <v>20044.322963803406</v>
       </c>
       <c r="BI31" s="2">
-        <f t="shared" si="102"/>
-        <v>25131.84453966517</v>
+        <f t="shared" si="101"/>
+        <v>24321.152971444721</v>
       </c>
     </row>
     <row r="32" spans="2:123" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -4590,7 +4646,7 @@
         <v>33</v>
       </c>
       <c r="C32" s="4">
-        <f t="shared" ref="C32" si="103">C30-C31</f>
+        <f t="shared" ref="C32" si="102">C30-C31</f>
         <v>3027</v>
       </c>
       <c r="D32" s="4">
@@ -4598,7 +4654,7 @@
         <v>3561</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" ref="E32" si="104">E30-E31</f>
+        <f t="shared" ref="E32" si="103">E30-E31</f>
         <v>2625</v>
       </c>
       <c r="F32" s="4">
@@ -4606,15 +4662,15 @@
         <v>2134</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" ref="G32" si="105">G30-G31</f>
+        <f t="shared" ref="G32" si="104">G30-G31</f>
         <v>3268</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" ref="H32" si="106">H30-H31</f>
+        <f t="shared" ref="H32" si="105">H30-H31</f>
         <v>2535</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" ref="I32" si="107">I30-I31</f>
+        <f t="shared" ref="I32" si="106">I30-I31</f>
         <v>5243</v>
       </c>
       <c r="J32" s="4">
@@ -4622,7 +4678,7 @@
         <v>6331</v>
       </c>
       <c r="K32" s="4">
-        <f t="shared" ref="K32" si="108">K30-K31</f>
+        <f t="shared" ref="K32" si="107">K30-K31</f>
         <v>7222</v>
       </c>
       <c r="L32" s="4">
@@ -4630,47 +4686,47 @@
         <v>8107</v>
       </c>
       <c r="M32" s="4">
-        <f t="shared" ref="M32:W32" si="109">M30-M31</f>
+        <f t="shared" ref="M32:W32" si="108">M30-M31</f>
         <v>7778</v>
       </c>
       <c r="N32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>3156</v>
       </c>
       <c r="O32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>14323</v>
       </c>
       <c r="P32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>-3844</v>
       </c>
       <c r="Q32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>2982</v>
       </c>
       <c r="R32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>2872</v>
       </c>
       <c r="S32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>3247</v>
       </c>
       <c r="T32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>3172</v>
       </c>
       <c r="U32" s="4">
-        <f t="shared" si="109"/>
-        <v>4753.9693349999843</v>
+        <f t="shared" si="108"/>
+        <v>6750</v>
       </c>
       <c r="V32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>4179.4886749999878</v>
       </c>
       <c r="W32" s="4">
-        <f t="shared" si="109"/>
+        <f t="shared" si="108"/>
         <v>4863.3914500000019</v>
       </c>
       <c r="AF32" s="2">
@@ -4686,320 +4742,320 @@
         <v>253.21399999999971</v>
       </c>
       <c r="AS32" s="4">
-        <f t="shared" ref="AS32:AU32" si="110">AS30-AS31</f>
+        <f t="shared" ref="AS32:AU32" si="109">AS30-AS31</f>
         <v>-241</v>
       </c>
       <c r="AT32" s="4">
-        <f t="shared" si="110"/>
+        <f t="shared" si="109"/>
         <v>596</v>
       </c>
       <c r="AU32" s="4">
-        <f t="shared" si="110"/>
+        <f t="shared" si="109"/>
         <v>2371</v>
       </c>
       <c r="AV32" s="4">
-        <f t="shared" ref="AV32" si="111">AV30-AV31</f>
+        <f t="shared" ref="AV32" si="110">AV30-AV31</f>
         <v>3033</v>
       </c>
       <c r="AW32" s="4">
-        <f t="shared" ref="AW32:AX32" si="112">AW30-AW31</f>
+        <f t="shared" ref="AW32:AX32" si="111">AW30-AW31</f>
         <v>10073</v>
       </c>
       <c r="AX32" s="4">
+        <f t="shared" si="111"/>
+        <v>11588</v>
+      </c>
+      <c r="AY32" s="4">
+        <f t="shared" ref="AY32:BB32" si="112">AY30-AY31</f>
+        <v>21331</v>
+      </c>
+      <c r="AZ32" s="4">
         <f t="shared" si="112"/>
-        <v>11588</v>
-      </c>
-      <c r="AY32" s="4">
-        <f t="shared" ref="AY32:BB32" si="113">AY30-AY31</f>
-        <v>21331</v>
-      </c>
-      <c r="AZ32" s="4">
+        <v>33364</v>
+      </c>
+      <c r="BA32" s="4">
+        <f t="shared" si="112"/>
+        <v>5257</v>
+      </c>
+      <c r="BB32" s="4">
+        <f t="shared" si="112"/>
+        <v>12136.79012499997</v>
+      </c>
+      <c r="BC32" s="4">
+        <f t="shared" ref="BC32:BI32" si="113">BC30-BC31</f>
+        <v>18194.540021062574</v>
+      </c>
+      <c r="BD32" s="4">
         <f t="shared" si="113"/>
-        <v>33364</v>
-      </c>
-      <c r="BA32" s="4">
+        <v>33362.632550241389</v>
+      </c>
+      <c r="BE32" s="4">
         <f t="shared" si="113"/>
-        <v>5257</v>
-      </c>
-      <c r="BB32" s="4">
+        <v>52197.267737628586</v>
+      </c>
+      <c r="BF32" s="4">
         <f t="shared" si="113"/>
-        <v>16968.849460000005</v>
-      </c>
-      <c r="BC32" s="4">
-        <f t="shared" ref="BC32:BI32" si="114">BC30-BC31</f>
-        <v>20783.964885410081</v>
-      </c>
-      <c r="BD32" s="4">
-        <f t="shared" si="114"/>
-        <v>36189.891378685992</v>
-      </c>
-      <c r="BE32" s="4">
-        <f t="shared" si="114"/>
-        <v>55312.390734647255</v>
-      </c>
-      <c r="BF32" s="4">
-        <f t="shared" si="114"/>
-        <v>79113.561628328433</v>
+        <v>75646.218572986661</v>
       </c>
       <c r="BG32" s="4">
-        <f t="shared" si="114"/>
-        <v>96845.628523946056</v>
+        <f t="shared" si="113"/>
+        <v>93055.761297801873</v>
       </c>
       <c r="BH32" s="4">
-        <f t="shared" si="114"/>
-        <v>117746.72366014088</v>
+        <f t="shared" si="113"/>
+        <v>113584.49679488597</v>
       </c>
       <c r="BI32" s="4">
-        <f t="shared" si="114"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="113"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BJ32" s="2">
         <f>+BI32*(1+$BL$46)</f>
-        <v>142413.78572476929</v>
+        <v>137819.86683818678</v>
       </c>
       <c r="BK32" s="2">
-        <f t="shared" ref="BK32:DS32" si="115">+BJ32*(1+$BL$46)</f>
-        <v>142413.78572476929</v>
+        <f t="shared" ref="BK32:DS32" si="114">+BJ32*(1+$BL$46)</f>
+        <v>137819.86683818678</v>
       </c>
       <c r="BL32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BM32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BN32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BO32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BP32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BQ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BR32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BS32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BT32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BU32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BV32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BW32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BX32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BY32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="BZ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CA32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CB32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CC32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CD32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CE32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CF32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CG32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CH32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CI32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CJ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CK32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CL32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CM32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CN32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CO32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CP32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CQ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CR32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CS32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CT32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CU32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CV32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CW32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CX32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CY32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="CZ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DA32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DB32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DC32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DD32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DE32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DF32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DG32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DH32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DI32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DJ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DK32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DL32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DM32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DN32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DO32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DP32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DQ32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DR32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
       <c r="DS32" s="2">
-        <f t="shared" si="115"/>
-        <v>142413.78572476929</v>
+        <f t="shared" si="114"/>
+        <v>137819.86683818678</v>
       </c>
     </row>
     <row r="33" spans="2:64" x14ac:dyDescent="0.2">
@@ -5007,7 +5063,7 @@
         <v>34</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" ref="C33" si="116">C32/C34</f>
+        <f t="shared" ref="C33" si="115">C32/C34</f>
         <v>6.0419161676646711</v>
       </c>
       <c r="D33" s="7">
@@ -5015,7 +5071,7 @@
         <v>7.0936254980079685</v>
       </c>
       <c r="E33" s="7">
-        <f t="shared" ref="E33" si="117">E32/E34</f>
+        <f t="shared" ref="E33" si="116">E32/E34</f>
         <v>5.2186878727634198</v>
       </c>
       <c r="F33" s="7">
@@ -5023,15 +5079,15 @@
         <v>4.2341269841269842</v>
       </c>
       <c r="G33" s="7">
-        <f t="shared" ref="G33" si="118">G32/G34</f>
+        <f t="shared" ref="G33" si="117">G32/G34</f>
         <v>6.4712871287128717</v>
       </c>
       <c r="H33" s="7">
-        <f t="shared" ref="H33" si="119">H32/H34</f>
+        <f t="shared" ref="H33" si="118">H32/H34</f>
         <v>5.0098814229249014</v>
       </c>
       <c r="I33" s="7">
-        <f t="shared" ref="I33" si="120">I32/I34</f>
+        <f t="shared" ref="I33" si="119">I32/I34</f>
         <v>10.300589390962672</v>
       </c>
       <c r="J33" s="7">
@@ -5039,7 +5095,7 @@
         <v>12.365234375</v>
       </c>
       <c r="K33" s="7">
-        <f t="shared" ref="K33" si="121">K32/K34</f>
+        <f t="shared" ref="K33" si="120">K32/K34</f>
         <v>14.077972709551657</v>
       </c>
       <c r="L33" s="7">
@@ -5063,32 +5119,32 @@
         <v>-7.5520628683693518</v>
       </c>
       <c r="Q33" s="7">
-        <f t="shared" ref="Q33:W33" si="122">Q32/Q34</f>
+        <f t="shared" ref="Q33:W33" si="121">Q32/Q34</f>
         <v>0.29307125307125309</v>
       </c>
       <c r="R33" s="7">
-        <f t="shared" si="122"/>
+        <f t="shared" si="121"/>
         <v>0.27799825767108705</v>
       </c>
       <c r="S33" s="7">
-        <f t="shared" si="122"/>
+        <f t="shared" si="121"/>
         <v>0.31499805975941014</v>
       </c>
       <c r="T33" s="7">
-        <f t="shared" si="122"/>
+        <f t="shared" si="121"/>
         <v>0.3065622885860636</v>
       </c>
       <c r="U33" s="7">
-        <f t="shared" si="122"/>
-        <v>0.45945388373441426</v>
+        <f t="shared" si="121"/>
+        <v>0.64599483204134367</v>
       </c>
       <c r="V33" s="7">
-        <f t="shared" si="122"/>
-        <v>0.40393241277664904</v>
+        <f t="shared" si="121"/>
+        <v>0.39998934587041707</v>
       </c>
       <c r="W33" s="7">
-        <f t="shared" si="122"/>
-        <v>0.47002913404851665</v>
+        <f t="shared" si="121"/>
+        <v>0.46544085079911973</v>
       </c>
       <c r="AF33" s="1">
         <f>AF32/AF34</f>
@@ -5103,27 +5159,27 @@
         <v>0.60382208741105259</v>
       </c>
       <c r="AS33" s="7">
-        <f t="shared" ref="AS33" si="123">AS32/AS34</f>
+        <f t="shared" ref="AS33" si="122">AS32/AS34</f>
         <v>-0.52164502164502169</v>
       </c>
       <c r="AT33" s="7">
-        <f t="shared" ref="AT33" si="124">AT32/AT34</f>
+        <f t="shared" ref="AT33" si="123">AT32/AT34</f>
         <v>1.249475890985325</v>
       </c>
       <c r="AU33" s="7">
-        <f t="shared" ref="AU33" si="125">AU32/AU34</f>
+        <f t="shared" ref="AU33" si="124">AU32/AU34</f>
         <v>4.8987603305785123</v>
       </c>
       <c r="AV33" s="7">
-        <f t="shared" ref="AV33" si="126">AV32/AV34</f>
+        <f t="shared" ref="AV33" si="125">AV32/AV34</f>
         <v>6.1521298174442194</v>
       </c>
       <c r="AW33" s="7">
-        <f t="shared" ref="AW33:AX33" si="127">AW32/AW34</f>
+        <f t="shared" ref="AW33:AX33" si="126">AW32/AW34</f>
         <v>20.146000000000001</v>
       </c>
       <c r="AX33" s="7">
-        <f t="shared" si="127"/>
+        <f t="shared" si="126"/>
         <v>23.014895729890764</v>
       </c>
       <c r="AY33" s="7">
@@ -5135,40 +5191,40 @@
         <v>6.1676679914964412</v>
       </c>
       <c r="BA33" s="7">
-        <f t="shared" ref="BA33:BB33" si="128">BA32/BA34</f>
+        <f t="shared" ref="BA33:BB33" si="127">BA32/BA34</f>
         <v>0.51665847665847664</v>
       </c>
       <c r="BB33" s="7">
-        <f t="shared" si="128"/>
-        <v>1.6399777191456466</v>
+        <f t="shared" si="127"/>
+        <v>1.1643680265745642</v>
       </c>
       <c r="BC33" s="7">
-        <f t="shared" ref="BC33" si="129">BC32/BC34</f>
-        <v>2.0086947796859072</v>
+        <f t="shared" ref="BC33" si="128">BC32/BC34</f>
+        <v>1.7455307738343717</v>
       </c>
       <c r="BD33" s="7">
-        <f t="shared" ref="BD33" si="130">BD32/BD34</f>
-        <v>3.4976216660564408</v>
+        <f t="shared" ref="BD33" si="129">BD32/BD34</f>
+        <v>3.2007130570577433</v>
       </c>
       <c r="BE33" s="7">
-        <f t="shared" ref="BE33" si="131">BE32/BE34</f>
-        <v>5.3457418318978691</v>
+        <f t="shared" ref="BE33" si="130">BE32/BE34</f>
+        <v>5.0076526826525241</v>
       </c>
       <c r="BF33" s="7">
-        <f t="shared" ref="BF33" si="132">BF32/BF34</f>
-        <v>7.6460386226276631</v>
+        <f t="shared" ref="BF33" si="131">BF32/BF34</f>
+        <v>7.2572762098130825</v>
       </c>
       <c r="BG33" s="7">
-        <f t="shared" ref="BG33" si="133">BG32/BG34</f>
-        <v>9.3597785371553162</v>
+        <f t="shared" ref="BG33" si="132">BG32/BG34</f>
+        <v>8.9274966467886863</v>
       </c>
       <c r="BH33" s="7">
-        <f t="shared" ref="BH33" si="134">BH32/BH34</f>
-        <v>11.379793530505546</v>
+        <f t="shared" ref="BH33" si="133">BH32/BH34</f>
+        <v>10.89696328439449</v>
       </c>
       <c r="BI33" s="7">
-        <f t="shared" ref="BI33" si="135">BI32/BI34</f>
-        <v>13.763775560526653</v>
+        <f t="shared" ref="BI33" si="134">BI32/BI34</f>
+        <v>13.222033562448964</v>
       </c>
     </row>
     <row r="34" spans="2:64" x14ac:dyDescent="0.2">
@@ -5230,16 +5286,15 @@
         <v>10347</v>
       </c>
       <c r="U34" s="4">
-        <f t="shared" ref="U34:W34" si="136">+T34</f>
-        <v>10347</v>
+        <v>10449</v>
       </c>
       <c r="V34" s="4">
-        <f t="shared" si="136"/>
-        <v>10347</v>
+        <f t="shared" ref="U34:W34" si="135">+U34</f>
+        <v>10449</v>
       </c>
       <c r="W34" s="4">
-        <f t="shared" si="136"/>
-        <v>10347</v>
+        <f t="shared" si="135"/>
+        <v>10449</v>
       </c>
       <c r="AD34" s="2">
         <v>161.096869</v>
@@ -5286,35 +5341,35 @@
       </c>
       <c r="BB34" s="2">
         <f>AVERAGE(T34:W34)</f>
-        <v>10347</v>
+        <v>10423.5</v>
       </c>
       <c r="BC34" s="2">
         <f>+BB34</f>
-        <v>10347</v>
+        <v>10423.5</v>
       </c>
       <c r="BD34" s="2">
-        <f t="shared" ref="BD34:BI34" si="137">+BC34</f>
-        <v>10347</v>
+        <f t="shared" ref="BD34:BI34" si="136">+BC34</f>
+        <v>10423.5</v>
       </c>
       <c r="BE34" s="2">
-        <f t="shared" si="137"/>
-        <v>10347</v>
+        <f t="shared" si="136"/>
+        <v>10423.5</v>
       </c>
       <c r="BF34" s="2">
-        <f t="shared" si="137"/>
-        <v>10347</v>
+        <f t="shared" si="136"/>
+        <v>10423.5</v>
       </c>
       <c r="BG34" s="2">
-        <f t="shared" si="137"/>
-        <v>10347</v>
+        <f t="shared" si="136"/>
+        <v>10423.5</v>
       </c>
       <c r="BH34" s="2">
-        <f t="shared" si="137"/>
-        <v>10347</v>
+        <f t="shared" si="136"/>
+        <v>10423.5</v>
       </c>
       <c r="BI34" s="2">
-        <f t="shared" si="137"/>
-        <v>10347</v>
+        <f t="shared" si="136"/>
+        <v>10423.5</v>
       </c>
     </row>
     <row r="36" spans="2:64" s="11" customFormat="1" x14ac:dyDescent="0.2">
@@ -5334,31 +5389,31 @@
         <v>0.26385259631490787</v>
       </c>
       <c r="I36" s="10">
-        <f t="shared" ref="I36:K36" si="138">I20/E20-1</f>
+        <f t="shared" ref="I36:K36" si="137">I20/E20-1</f>
         <v>0.40230900258658764</v>
       </c>
       <c r="J36" s="10">
-        <f t="shared" si="138"/>
+        <f t="shared" si="137"/>
         <v>0.37387290836084075</v>
       </c>
       <c r="K36" s="10">
-        <f t="shared" si="138"/>
+        <f t="shared" si="137"/>
         <v>0.43594816839553041</v>
       </c>
       <c r="L36" s="10">
-        <f t="shared" ref="L36" si="139">L20/H20-1</f>
+        <f t="shared" ref="L36" si="138">L20/H20-1</f>
         <v>0.43823888034777081</v>
       </c>
       <c r="M36" s="10">
-        <f t="shared" ref="M36" si="140">M20/I20-1</f>
+        <f t="shared" ref="M36" si="139">M20/I20-1</f>
         <v>0.27181932697498645</v>
       </c>
       <c r="N36" s="10">
-        <f t="shared" ref="N36" si="141">N20/J20-1</f>
+        <f t="shared" ref="N36" si="140">N20/J20-1</f>
         <v>0.15255083467679031</v>
       </c>
       <c r="O36" s="10">
-        <f t="shared" ref="O36" si="142">O20/K20-1</f>
+        <f t="shared" ref="O36" si="141">O20/K20-1</f>
         <v>9.4436701047349692E-2</v>
       </c>
       <c r="P36" s="10">
@@ -5366,7 +5421,7 @@
         <v>7.3038574245747334E-2</v>
       </c>
       <c r="Q36" s="10">
-        <f t="shared" ref="Q36:W36" si="143">Q20/M20-1</f>
+        <f t="shared" ref="Q36:W36" si="142">Q20/M20-1</f>
         <v>7.2108241952600016E-2</v>
       </c>
       <c r="R36" s="10">
@@ -5374,7 +5429,7 @@
         <v>0.14699671515720314</v>
       </c>
       <c r="S36" s="10">
-        <f t="shared" si="143"/>
+        <f t="shared" si="142"/>
         <v>8.5814921549791867E-2</v>
       </c>
       <c r="T36" s="10">
@@ -5382,107 +5437,107 @@
         <v>9.3727456975026602E-2</v>
       </c>
       <c r="U36" s="10">
+        <f t="shared" si="142"/>
+        <v>0.10845967302901816</v>
+      </c>
+      <c r="V36" s="10">
+        <f t="shared" si="142"/>
+        <v>6.4824745674699535E-2</v>
+      </c>
+      <c r="W36" s="10">
+        <f t="shared" si="142"/>
+        <v>6.1610412589474972E-2</v>
+      </c>
+      <c r="AC36" s="15">
+        <f t="shared" ref="AC36:AD36" si="143">AC20/AB20-1</f>
+        <v>3.1263372285789677</v>
+      </c>
+      <c r="AD36" s="15">
         <f t="shared" si="143"/>
-        <v>6.4896893610703277E-2</v>
-      </c>
-      <c r="V36" s="10">
-        <f t="shared" si="143"/>
-        <v>6.4824745674699535E-2</v>
-      </c>
-      <c r="W36" s="10">
-        <f t="shared" si="143"/>
-        <v>6.1610412589474972E-2</v>
-      </c>
-      <c r="AC36" s="15">
-        <f t="shared" ref="AC36:AD36" si="144">AC20/AB20-1</f>
-        <v>3.1263372285789677</v>
-      </c>
-      <c r="AD36" s="15">
-        <f t="shared" si="144"/>
         <v>1.6890585567192891</v>
       </c>
       <c r="AE36" s="15">
-        <f t="shared" ref="AE36" si="145">AE20/AD20-1</f>
+        <f t="shared" ref="AE36" si="144">AE20/AD20-1</f>
         <v>0.68430132470321792</v>
       </c>
       <c r="AF36" s="15">
-        <f t="shared" ref="AF36" si="146">AF20/AE20-1</f>
+        <f t="shared" ref="AF36" si="145">AF20/AE20-1</f>
         <v>0.1305040617556299</v>
       </c>
       <c r="AG36" s="15">
-        <f t="shared" ref="AG36" si="147">AG20/AF20-1</f>
+        <f t="shared" ref="AG36" si="146">AG20/AF20-1</f>
         <v>0.25957418461821291</v>
       </c>
       <c r="AH36" s="15">
-        <f t="shared" ref="AH36" si="148">AH20/AG20-1</f>
+        <f t="shared" ref="AH36" si="147">AH20/AG20-1</f>
         <v>0.3383637567455966</v>
       </c>
       <c r="AI36" s="15">
-        <f t="shared" ref="AI36" si="149">AI20/AH20-1</f>
+        <f t="shared" ref="AI36" si="148">AI20/AH20-1</f>
         <v>0.31485481977597884</v>
       </c>
       <c r="AJ36" s="15">
-        <f t="shared" ref="AJ36" si="150">AJ20/AI20-1</f>
+        <f t="shared" ref="AJ36" si="149">AJ20/AI20-1</f>
         <v>0.22670134373645423</v>
       </c>
       <c r="AK36" s="15">
-        <f t="shared" ref="AK36" si="151">AK20/AJ20-1</f>
+        <f t="shared" ref="AK36" si="150">AK20/AJ20-1</f>
         <v>0.26160188457008249</v>
       </c>
       <c r="AL36" s="15">
-        <f t="shared" ref="AL36" si="152">AL20/AK20-1</f>
+        <f t="shared" ref="AL36" si="151">AL20/AK20-1</f>
         <v>0.38502474092054895</v>
       </c>
       <c r="AM36" s="15">
-        <f t="shared" ref="AM36" si="153">AM20/AL20-1</f>
+        <f t="shared" ref="AM36" si="152">AM20/AL20-1</f>
         <v>0.29194472531176263</v>
       </c>
       <c r="AN36" s="15">
-        <f t="shared" ref="AN36" si="154">AN20/AM20-1</f>
+        <f t="shared" ref="AN36" si="153">AN20/AM20-1</f>
         <v>0.27877491391004905</v>
       </c>
       <c r="AO36" s="15">
-        <f t="shared" ref="AO36" si="155">AO20/AN20-1</f>
+        <f t="shared" ref="AO36" si="154">AO20/AN20-1</f>
         <v>0.39556897466236896</v>
       </c>
       <c r="AP36" s="15">
-        <f t="shared" ref="AP36" si="156">AP20/AO20-1</f>
+        <f t="shared" ref="AP36" si="155">AP20/AO20-1</f>
         <v>0.40559583674424049</v>
       </c>
       <c r="AQ36" s="15">
-        <f t="shared" ref="AQ36" si="157">AQ20/AP20-1</f>
+        <f t="shared" ref="AQ36" si="156">AQ20/AP20-1</f>
         <v>0.27073236682821311</v>
       </c>
       <c r="AR36" s="15">
-        <f t="shared" ref="AR36:AV36" si="158">AR20/AQ20-1</f>
+        <f t="shared" ref="AR36:AV36" si="157">AR20/AQ20-1</f>
         <v>0.21866662301736706</v>
       </c>
       <c r="AS36" s="15">
-        <f t="shared" si="158"/>
+        <f t="shared" si="157"/>
         <v>0.1952398861011122</v>
       </c>
       <c r="AT36" s="15">
-        <f t="shared" si="158"/>
+        <f t="shared" si="157"/>
         <v>0.20247673843664304</v>
       </c>
       <c r="AU36" s="15">
-        <f t="shared" si="158"/>
+        <f t="shared" si="157"/>
         <v>0.27083528026465808</v>
       </c>
       <c r="AV36" s="15">
-        <f t="shared" si="158"/>
+        <f t="shared" si="157"/>
         <v>0.30796326119408479</v>
       </c>
       <c r="AW36" s="15">
-        <f t="shared" ref="AW36" si="159">AW20/AV20-1</f>
+        <f t="shared" ref="AW36" si="158">AW20/AV20-1</f>
         <v>0.3093396152159491</v>
       </c>
       <c r="AX36" s="15">
-        <f t="shared" ref="AX36" si="160">AX20/AW20-1</f>
+        <f t="shared" ref="AX36" si="159">AX20/AW20-1</f>
         <v>0.20454125820676983</v>
       </c>
       <c r="AY36" s="15">
-        <f t="shared" ref="AY36" si="161">AY20/AX20-1</f>
+        <f t="shared" ref="AY36" si="160">AY20/AX20-1</f>
         <v>0.37623430604373276</v>
       </c>
       <c r="AZ36" s="15">
@@ -5490,40 +5545,40 @@
         <v>0.21695366571345676</v>
       </c>
       <c r="BA36" s="15">
-        <f t="shared" ref="BA36:BI36" si="162">BA20/AZ20-1</f>
+        <f t="shared" ref="BA36:BI36" si="161">BA20/AZ20-1</f>
         <v>9.399517263985091E-2</v>
       </c>
       <c r="BB36" s="15">
         <f>BB20/BA20-1</f>
-        <v>7.0456649344433631E-2</v>
+        <v>6.744721128908937E-2</v>
       </c>
       <c r="BC36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.10067887743092241</v>
+        <f t="shared" si="161"/>
+        <v>0.10011693435294222</v>
       </c>
       <c r="BD36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.10851928608137085</v>
+        <f t="shared" si="161"/>
+        <v>0.10788136266829529</v>
       </c>
       <c r="BE36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.1173009319259728</v>
+        <f t="shared" si="161"/>
+        <v>0.11658671533946263</v>
       </c>
       <c r="BF36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.12699968811339213</v>
+        <f t="shared" si="161"/>
+        <v>0.12621229541795809</v>
       </c>
       <c r="BG36" s="15">
-        <f t="shared" si="162"/>
-        <v>9.8319689430071078E-2</v>
+        <f t="shared" si="161"/>
+        <v>9.7785488736678694E-2</v>
       </c>
       <c r="BH36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.10279303273364193</v>
+        <f t="shared" si="161"/>
+        <v>0.10223478272608966</v>
       </c>
       <c r="BI36" s="15">
-        <f t="shared" si="162"/>
-        <v>0.10744653565985263</v>
+        <f t="shared" si="161"/>
+        <v>0.10686786540729587</v>
       </c>
     </row>
     <row r="37" spans="2:64" x14ac:dyDescent="0.2">
@@ -5535,39 +5590,39 @@
       <c r="F37" s="8"/>
       <c r="G37" s="8"/>
       <c r="H37" s="8">
-        <f t="shared" ref="H37:H38" si="163">+H18/D18-1</f>
+        <f t="shared" ref="H37:H38" si="162">+H18/D18-1</f>
         <v>0.22045911968030807</v>
       </c>
       <c r="I37" s="8">
-        <f t="shared" ref="I37:I38" si="164">+I18/E18-1</f>
+        <f t="shared" ref="I37:I38" si="163">+I18/E18-1</f>
         <v>0.40127175368139234</v>
       </c>
       <c r="J37" s="8">
-        <f t="shared" ref="J37:J38" si="165">+J18/F18-1</f>
+        <f t="shared" ref="J37:J38" si="164">+J18/F18-1</f>
         <v>0.32844988168957356</v>
       </c>
       <c r="K37" s="8">
-        <f t="shared" ref="K37:K38" si="166">+K18/G18-1</f>
+        <f t="shared" ref="K37:K38" si="165">+K18/G18-1</f>
         <v>0.40588025800324479</v>
       </c>
       <c r="L37" s="8">
-        <f t="shared" ref="L37:P37" si="167">+L18/H18-1</f>
+        <f t="shared" ref="L37:P37" si="166">+L18/H18-1</f>
         <v>0.37403503740350375</v>
       </c>
       <c r="M37" s="8">
-        <f t="shared" si="167"/>
+        <f t="shared" si="166"/>
         <v>0.15444630204601539</v>
       </c>
       <c r="N37" s="8">
-        <f t="shared" si="167"/>
+        <f t="shared" si="166"/>
         <v>3.9830219426232549E-2</v>
       </c>
       <c r="O37" s="8">
-        <f t="shared" si="167"/>
+        <f t="shared" si="166"/>
         <v>5.0664264805224679E-3</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" si="167"/>
+        <f t="shared" si="166"/>
         <v>-1.8020211859247515E-2</v>
       </c>
       <c r="Q37" s="8">
@@ -5586,7 +5641,10 @@
         <f>+T18/P18-1</f>
         <v>9.317155256398868E-3</v>
       </c>
-      <c r="U37" s="8"/>
+      <c r="U37" s="8">
+        <f t="shared" ref="U37:U38" si="167">+U18/Q18-1</f>
+        <v>4.342907644719407E-2</v>
+      </c>
       <c r="V37" s="8"/>
       <c r="W37" s="8"/>
       <c r="AR37" s="13"/>
@@ -5617,19 +5675,19 @@
       <c r="F38" s="8"/>
       <c r="G38" s="8"/>
       <c r="H38" s="8">
+        <f t="shared" si="162"/>
+        <v>0.32238265727662596</v>
+      </c>
+      <c r="I38" s="8">
         <f t="shared" si="163"/>
-        <v>0.32238265727662596</v>
-      </c>
-      <c r="I38" s="8">
+        <v>0.40365906780891536</v>
+      </c>
+      <c r="J38" s="8">
         <f t="shared" si="164"/>
-        <v>0.40365906780891536</v>
-      </c>
-      <c r="J38" s="8">
+        <v>0.43351512146752613</v>
+      </c>
+      <c r="K38" s="8">
         <f t="shared" si="165"/>
-        <v>0.43351512146752613</v>
-      </c>
-      <c r="K38" s="8">
-        <f t="shared" si="166"/>
         <v>0.47713782355332701</v>
       </c>
       <c r="L38" s="8">
@@ -5668,7 +5726,10 @@
         <f t="shared" si="172"/>
         <v>0.17316508026471511</v>
       </c>
-      <c r="U38" s="8"/>
+      <c r="U38" s="8">
+        <f t="shared" si="167"/>
+        <v>0.16535981069920669</v>
+      </c>
       <c r="V38" s="8"/>
       <c r="W38" s="8"/>
       <c r="AR38" s="13"/>
@@ -6240,7 +6301,7 @@
       </c>
       <c r="U43" s="8">
         <f t="shared" ref="U43:W43" si="204">U9/Q9-1</f>
-        <v>0.19999999999999996</v>
+        <v>0.12163736764780375</v>
       </c>
       <c r="V43" s="8">
         <f t="shared" si="204"/>
@@ -6284,7 +6345,7 @@
       </c>
       <c r="BB43" s="13">
         <f t="shared" si="209"/>
-        <v>0.19032161406312431</v>
+        <v>0.1710097882540953</v>
       </c>
       <c r="BC43" s="13">
         <f t="shared" si="209"/>
@@ -6393,7 +6454,7 @@
       </c>
       <c r="U44" s="16">
         <f t="shared" si="212"/>
-        <v>0.30294374179861744</v>
+        <v>0.32522714926739243</v>
       </c>
       <c r="V44" s="16">
         <f t="shared" si="212"/>
@@ -6441,35 +6502,35 @@
       </c>
       <c r="BB44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29894307146835464</v>
+        <v>0.29571470937777933</v>
       </c>
       <c r="BC44" s="14">
         <f t="shared" si="217"/>
-        <v>0.2838338627721152</v>
+        <v>0.28378000482879756</v>
       </c>
       <c r="BD44" s="14">
         <f t="shared" si="217"/>
-        <v>0.28933078918273203</v>
+        <v>0.28928908055547392</v>
       </c>
       <c r="BE44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29454505726643759</v>
+        <v>0.29452022966921787</v>
       </c>
       <c r="BF44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29937983643671434</v>
+        <v>0.29937657826604525</v>
       </c>
       <c r="BG44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29940712003279502</v>
+        <v>0.29940371518172848</v>
       </c>
       <c r="BH44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29943550244961009</v>
+        <v>0.29943197305238678</v>
       </c>
       <c r="BI44" s="14">
         <f t="shared" si="217"/>
-        <v>0.29946478461142489</v>
+        <v>0.29946115673457163</v>
       </c>
       <c r="BK44" t="s">
         <v>77</v>
@@ -6491,7 +6552,7 @@
         <v>75</v>
       </c>
       <c r="K46" s="4">
-        <f t="shared" ref="K46:T46" si="218">+K47-K60</f>
+        <f t="shared" ref="K46:U46" si="218">+K47-K60</f>
         <v>52580</v>
       </c>
       <c r="L46" s="4">
@@ -6531,16 +6592,16 @@
         <v>-2679</v>
       </c>
       <c r="U46" s="4">
-        <f t="shared" ref="U46:W46" si="219">+T46+U32</f>
-        <v>2074.9693349999843</v>
+        <f t="shared" si="218"/>
+        <v>878</v>
       </c>
       <c r="V46" s="4">
-        <f t="shared" si="219"/>
-        <v>6254.4580099999721</v>
+        <f t="shared" ref="U46:W46" si="219">+U46+V32</f>
+        <v>5057.4886749999878</v>
       </c>
       <c r="W46" s="4">
         <f t="shared" si="219"/>
-        <v>11117.849459999974</v>
+        <v>9920.8801249999888</v>
       </c>
       <c r="X46" s="4"/>
       <c r="Y46" s="4"/>
@@ -6553,35 +6614,35 @@
       </c>
       <c r="BB46" s="2">
         <f>+W46</f>
-        <v>11117.849459999974</v>
+        <v>9920.8801249999888</v>
       </c>
       <c r="BC46" s="2">
         <f>+BB46+BC32</f>
-        <v>31901.814345410057</v>
+        <v>28115.420146062563</v>
       </c>
       <c r="BD46" s="2">
         <f t="shared" ref="BD46:BI46" si="220">+BC46+BD32</f>
-        <v>68091.705724096042</v>
+        <v>61478.052696303952</v>
       </c>
       <c r="BE46" s="2">
         <f t="shared" si="220"/>
-        <v>123404.0964587433</v>
+        <v>113675.32043393253</v>
       </c>
       <c r="BF46" s="2">
         <f t="shared" si="220"/>
-        <v>202517.65808707173</v>
+        <v>189321.53900691919</v>
       </c>
       <c r="BG46" s="2">
         <f t="shared" si="220"/>
-        <v>299363.28661101777</v>
+        <v>282377.30030472105</v>
       </c>
       <c r="BH46" s="2">
         <f t="shared" si="220"/>
-        <v>417110.01027115865</v>
+        <v>395961.79709960701</v>
       </c>
       <c r="BI46" s="2">
         <f t="shared" si="220"/>
-        <v>559523.79599592788</v>
+        <v>533781.66393779381</v>
       </c>
       <c r="BK46" t="s">
         <v>78</v>
@@ -6642,12 +6703,16 @@
         <f>49343+15062</f>
         <v>64405</v>
       </c>
+      <c r="U47" s="2">
+        <f>49529+14441</f>
+        <v>63970</v>
+      </c>
       <c r="BK47" s="2" t="s">
         <v>79</v>
       </c>
       <c r="BL47" s="2">
         <f>NPV(BL44,BB32:DS32)+Main!K5-Main!K6</f>
-        <v>1316805.5506389481</v>
+        <v>1265156.9732669257</v>
       </c>
     </row>
     <row r="48" spans="2:64" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -6692,12 +6757,15 @@
       <c r="T48" s="2">
         <v>34170</v>
       </c>
+      <c r="U48" s="2">
+        <v>36587</v>
+      </c>
       <c r="BL48" s="1">
         <f>+BL47/Main!K3</f>
-        <v>127.46157686951391</v>
-      </c>
-    </row>
-    <row r="49" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>122.46219855453738</v>
+      </c>
+    </row>
+    <row r="49" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B49" s="2" t="s">
         <v>64</v>
       </c>
@@ -6739,8 +6807,11 @@
       <c r="T49" s="2">
         <v>37646</v>
       </c>
-    </row>
-    <row r="50" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U49" s="2">
+        <v>39925</v>
+      </c>
+    </row>
+    <row r="50" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2" t="s">
         <v>65</v>
       </c>
@@ -6782,8 +6853,11 @@
       <c r="T50" s="2">
         <v>190754</v>
       </c>
-    </row>
-    <row r="51" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U50" s="2">
+        <v>193784</v>
+      </c>
+    </row>
+    <row r="51" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2" t="s">
         <v>66</v>
       </c>
@@ -6825,8 +6899,11 @@
       <c r="T51" s="2">
         <v>68262</v>
       </c>
-    </row>
-    <row r="52" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U51" s="2">
+        <v>70332</v>
+      </c>
+    </row>
+    <row r="52" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2" t="s">
         <v>67</v>
       </c>
@@ -6869,8 +6946,11 @@
         <f>22749</f>
         <v>22749</v>
       </c>
-    </row>
-    <row r="53" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U52" s="2">
+        <v>22785</v>
+      </c>
+    </row>
+    <row r="53" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B53" s="2" t="s">
         <v>68</v>
       </c>
@@ -6912,8 +6992,11 @@
       <c r="T53" s="2">
         <v>46392</v>
       </c>
-    </row>
-    <row r="54" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U53" s="2">
+        <v>50224</v>
+      </c>
+    </row>
+    <row r="54" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2" t="s">
         <v>62</v>
       </c>
@@ -6926,7 +7009,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4">
-        <f t="shared" ref="K54:T54" si="221">SUM(K47:K53)</f>
+        <f t="shared" ref="K54:U54" si="221">SUM(K47:K53)</f>
         <v>321195</v>
       </c>
       <c r="L54" s="4">
@@ -6965,8 +7048,12 @@
         <f t="shared" si="221"/>
         <v>464378</v>
       </c>
-    </row>
-    <row r="56" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U54" s="4">
+        <f t="shared" si="221"/>
+        <v>477607</v>
+      </c>
+    </row>
+    <row r="56" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="2" t="s">
         <v>71</v>
       </c>
@@ -7008,8 +7095,11 @@
       <c r="T56" s="2">
         <v>66907</v>
       </c>
-    </row>
-    <row r="57" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U56" s="2">
+        <v>69481</v>
+      </c>
+    </row>
+    <row r="57" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="2" t="s">
         <v>72</v>
       </c>
@@ -7051,8 +7141,11 @@
       <c r="T57" s="2">
         <v>66382</v>
       </c>
-    </row>
-    <row r="58" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U57" s="2">
+        <v>64235</v>
+      </c>
+    </row>
+    <row r="58" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2" t="s">
         <v>73</v>
       </c>
@@ -7094,8 +7187,11 @@
       <c r="T58" s="2">
         <v>14281</v>
       </c>
-    </row>
-    <row r="59" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U58" s="2">
+        <v>14522</v>
+      </c>
+    </row>
+    <row r="59" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2" t="s">
         <v>66</v>
       </c>
@@ -7137,8 +7233,11 @@
       <c r="T59" s="2">
         <v>74267</v>
       </c>
-    </row>
-    <row r="60" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U59" s="2">
+        <v>75822</v>
+      </c>
+    </row>
+    <row r="60" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="2" t="s">
         <v>5</v>
       </c>
@@ -7180,8 +7279,11 @@
       <c r="T60" s="2">
         <v>67084</v>
       </c>
-    </row>
-    <row r="61" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U60" s="2">
+        <v>63092</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2" t="s">
         <v>74</v>
       </c>
@@ -7223,8 +7325,11 @@
       <c r="T61" s="2">
         <v>20931</v>
       </c>
-    </row>
-    <row r="62" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U61" s="2">
+        <v>21853</v>
+      </c>
+    </row>
+    <row r="62" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
         <v>70</v>
       </c>
@@ -7266,8 +7371,11 @@
       <c r="T62" s="2">
         <v>154526</v>
       </c>
-    </row>
-    <row r="63" spans="2:20" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="U62" s="2">
+        <v>168602</v>
+      </c>
+    </row>
+    <row r="63" spans="2:21" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
         <v>69</v>
       </c>
@@ -7280,7 +7388,7 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4">
-        <f t="shared" ref="K63:T63" si="222">SUM(K56:K62)</f>
+        <f t="shared" ref="K63:U63" si="222">SUM(K56:K62)</f>
         <v>321195</v>
       </c>
       <c r="L63" s="4">
@@ -7318,6 +7426,10 @@
       <c r="T63" s="4">
         <f t="shared" si="222"/>
         <v>464378</v>
+      </c>
+      <c r="U63" s="4">
+        <f t="shared" si="222"/>
+        <v>477607</v>
       </c>
     </row>
     <row r="65" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7372,6 +7484,10 @@
         <f>+T32</f>
         <v>3172</v>
       </c>
+      <c r="U65" s="4">
+        <f>+U32</f>
+        <v>6750</v>
+      </c>
     </row>
     <row r="66" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
@@ -7415,6 +7531,9 @@
       <c r="T66" s="4">
         <v>3172</v>
       </c>
+      <c r="U66" s="2">
+        <v>6750</v>
+      </c>
     </row>
     <row r="67" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
@@ -7458,6 +7577,9 @@
       <c r="T67" s="2">
         <v>11123</v>
       </c>
+      <c r="U67" s="2">
+        <v>11589</v>
+      </c>
     </row>
     <row r="68" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B68" s="2" t="s">
@@ -7501,6 +7623,9 @@
       <c r="T68" s="2">
         <v>4748</v>
       </c>
+      <c r="U68" s="2">
+        <v>7127</v>
+      </c>
     </row>
     <row r="69" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B69" s="2" t="s">
@@ -7544,6 +7669,9 @@
       <c r="T69" s="2">
         <v>534</v>
       </c>
+      <c r="U69" s="2">
+        <v>47</v>
+      </c>
     </row>
     <row r="70" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="2" t="s">
@@ -7587,6 +7715,9 @@
       <c r="T70" s="2">
         <v>0</v>
       </c>
+      <c r="U70" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="2" t="s">
@@ -7629,6 +7760,9 @@
       </c>
       <c r="T71" s="2">
         <v>-472</v>
+      </c>
+      <c r="U71" s="2">
+        <v>-2744</v>
       </c>
     </row>
     <row r="72" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -7683,6 +7817,10 @@
         <f>371+1521-11264-5763+818</f>
         <v>-14317</v>
       </c>
+      <c r="U72" s="2">
+        <f>-2373-5167+3029-1938+156</f>
+        <v>-6293</v>
+      </c>
     </row>
     <row r="73" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="2" t="s">
@@ -7697,7 +7835,7 @@
       <c r="I73" s="4"/>
       <c r="J73" s="4"/>
       <c r="K73" s="4">
-        <f t="shared" ref="K73:T73" si="224">SUM(K66:K72)</f>
+        <f t="shared" ref="K73:U73" si="224">SUM(K66:K72)</f>
         <v>30430</v>
       </c>
       <c r="L73" s="4">
@@ -7735,6 +7873,10 @@
       <c r="T73" s="4">
         <f t="shared" si="224"/>
         <v>4788</v>
+      </c>
+      <c r="U73" s="4">
+        <f t="shared" si="224"/>
+        <v>16476</v>
       </c>
       <c r="AF73" s="2">
         <v>-119.782</v>
@@ -7807,6 +7949,9 @@
       <c r="T75" s="2">
         <v>-14207</v>
       </c>
+      <c r="U75" s="2">
+        <v>-11455</v>
+      </c>
     </row>
     <row r="76" spans="2:34" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="2" t="s">

</xml_diff>

<commit_message>
updated AMGN and added others
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Shkreli - DL\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0EB20-0A9C-4982-AEA9-9E87622BA892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EBFBE7-C41D-4E66-B1AD-C622F4035187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39705" yWindow="1980" windowWidth="28230" windowHeight="17955" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="20580" yWindow="1840" windowWidth="17170" windowHeight="17900" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="151">
   <si>
     <t>Main</t>
   </si>
@@ -554,6 +554,87 @@
   </si>
   <si>
     <t>Revenue CC</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>EC2</t>
+  </si>
+  <si>
+    <t>Dynamo</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Devices</t>
+  </si>
+  <si>
+    <t>Echo</t>
+  </si>
+  <si>
+    <t>Kindle</t>
+  </si>
+  <si>
+    <t>Fire</t>
+  </si>
+  <si>
+    <t>Prime</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>SageMaker</t>
+  </si>
+  <si>
+    <t>Very weak in GPUs</t>
+  </si>
+  <si>
+    <t>Polly</t>
+  </si>
+  <si>
+    <t>EKS</t>
+  </si>
+  <si>
+    <t>Azure, GCP, Digital Ocean</t>
+  </si>
+  <si>
+    <t>Tranium</t>
+  </si>
+  <si>
+    <t>Inferentia</t>
+  </si>
+  <si>
+    <t>HyperPods</t>
+  </si>
+  <si>
+    <t>Bedrock</t>
+  </si>
+  <si>
+    <t>AI models</t>
+  </si>
+  <si>
+    <t>Advertising</t>
+  </si>
+  <si>
+    <t>Twitch</t>
+  </si>
+  <si>
+    <t>Whole Foods</t>
+  </si>
+  <si>
+    <t>3PS</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Audible</t>
   </si>
 </sst>
 </file>
@@ -1132,32 +1213,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E919ED4-9952-4C3B-8FDF-EC99BCC4C526}">
-  <dimension ref="B2:L9"/>
+  <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="1">
-        <v>167.9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
         <v>2</v>
       </c>
       <c r="K3" s="2">
-        <v>10406.627415000001</v>
+        <v>10708</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>103</v>
       </c>
@@ -1166,10 +1252,10 @@
       </c>
       <c r="K4" s="2">
         <f>K3*K2</f>
-        <v>1747272.7429785002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+        <v>1991688</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>106</v>
       </c>
@@ -1177,13 +1263,13 @@
         <v>4</v>
       </c>
       <c r="K5" s="2">
-        <v>85074</v>
+        <v>89092</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>104</v>
       </c>
@@ -1191,28 +1277,160 @@
         <v>5</v>
       </c>
       <c r="K6" s="2">
-        <v>57634</v>
+        <v>54889</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="2">
         <f>K4-K5+K6</f>
-        <v>1719832.7429785002</v>
+        <v>1957485</v>
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>143</v>
+      </c>
+      <c r="D19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1225,26 +1443,26 @@
   <dimension ref="A1:EG101"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AA3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AC46" sqref="AC46"/>
+      <selection pane="bottomRight" activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="26" width="9.140625" style="3"/>
-    <col min="74" max="75" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="26" width="9.1796875" style="3"/>
+    <col min="74" max="75" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>116</v>
       </c>
@@ -1532,7 +1750,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="3" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1640,7 +1858,7 @@
         <v>279833</v>
       </c>
     </row>
-    <row r="4" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
@@ -1678,7 +1896,7 @@
         <v>13580</v>
       </c>
     </row>
-    <row r="5" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1716,7 +1934,7 @@
         <v>64887</v>
       </c>
     </row>
-    <row r="6" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1824,7 +2042,7 @@
         <v>127787</v>
       </c>
     </row>
-    <row r="7" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
@@ -1862,7 +2080,7 @@
         <v>10631</v>
       </c>
     </row>
-    <row r="8" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
@@ -1900,7 +2118,7 @@
         <v>33107</v>
       </c>
     </row>
-    <row r="9" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
@@ -2056,7 +2274,7 @@
         <v>447916.72498560004</v>
       </c>
     </row>
-    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2133,7 +2351,9 @@
       <c r="AE11" s="4">
         <v>54670</v>
       </c>
-      <c r="AF11" s="4"/>
+      <c r="AF11" s="4">
+        <v>55392</v>
+      </c>
       <c r="AG11" s="4"/>
       <c r="BK11" s="2">
         <f>26939+27165+29061+39822</f>
@@ -2188,7 +2408,7 @@
         <v>326267.1892021501</v>
       </c>
     </row>
-    <row r="12" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2265,7 +2485,9 @@
       <c r="AE12" s="4">
         <v>5202</v>
       </c>
-      <c r="AF12" s="4"/>
+      <c r="AF12" s="4">
+        <v>5206</v>
+      </c>
       <c r="AG12" s="4"/>
       <c r="BK12" s="2">
         <f>4263+4312+4248+4401</f>
@@ -2320,7 +2542,7 @@
         <v>28184.221465804694</v>
       </c>
     </row>
-    <row r="13" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
@@ -2397,7 +2619,9 @@
       <c r="AE13" s="4">
         <v>34596</v>
       </c>
-      <c r="AF13" s="4"/>
+      <c r="AF13" s="4">
+        <v>36201</v>
+      </c>
       <c r="AG13" s="4"/>
       <c r="BK13" s="2">
         <f>9265+9702+10395+13383</f>
@@ -2452,7 +2676,7 @@
         <v>197068.63549427583</v>
       </c>
     </row>
-    <row r="14" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
@@ -2529,7 +2753,9 @@
       <c r="AE14" s="4">
         <v>11824</v>
       </c>
-      <c r="AF14" s="4"/>
+      <c r="AF14" s="4">
+        <v>10866</v>
+      </c>
       <c r="AG14" s="4"/>
       <c r="BK14" s="2">
         <f>3102+3408+3698+3959</f>
@@ -2584,7 +2810,7 @@
         <v>68149.380161362526</v>
       </c>
     </row>
-    <row r="15" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2661,7 +2887,9 @@
       <c r="AE15" s="4">
         <v>10722</v>
       </c>
-      <c r="AF15" s="4"/>
+      <c r="AF15" s="4">
+        <v>12771</v>
+      </c>
       <c r="AG15" s="4"/>
       <c r="BK15" s="2">
         <f>2031+2194+2495+3388</f>
@@ -2716,7 +2944,7 @@
         <v>79499.983233825042</v>
       </c>
     </row>
-    <row r="16" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -2791,7 +3019,9 @@
       <c r="AE16" s="4">
         <v>1262</v>
       </c>
-      <c r="AF16" s="4"/>
+      <c r="AF16" s="4">
+        <v>1260</v>
+      </c>
       <c r="AG16" s="4"/>
       <c r="BL16" s="2">
         <f t="shared" si="5"/>
@@ -2842,11 +3072,11 @@
         <v>6976.4038955296901</v>
       </c>
     </row>
-    <row r="17" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:137" x14ac:dyDescent="0.25">
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
@@ -2953,7 +3183,7 @@
         <v>241787</v>
       </c>
     </row>
-    <row r="19" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3060,7 +3290,7 @@
         <v>228035</v>
       </c>
     </row>
-    <row r="20" spans="2:137" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:137" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -3313,7 +3543,7 @@
         <v>1154062.5384385479</v>
       </c>
     </row>
-    <row r="21" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3467,7 +3697,7 @@
         <v>754757.74441970466</v>
       </c>
     </row>
-    <row r="22" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -3621,7 +3851,7 @@
         <v>52333.582469642599</v>
       </c>
     </row>
-    <row r="23" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
@@ -3806,7 +4036,7 @@
         <v>346971.21154920058</v>
       </c>
     </row>
-    <row r="24" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
@@ -3960,7 +4190,7 @@
         <v>105304.26010540825</v>
       </c>
     </row>
-    <row r="25" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -4114,7 +4344,7 @@
         <v>54569.503408901481</v>
       </c>
     </row>
-    <row r="26" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -4269,7 +4499,7 @@
         <v>14532.189593860268</v>
       </c>
     </row>
-    <row r="27" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -4454,7 +4684,7 @@
         <v>174405.95310816998</v>
       </c>
     </row>
-    <row r="28" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -4639,7 +4869,7 @@
         <v>172565.2584410306</v>
       </c>
     </row>
-    <row r="29" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -4823,7 +5053,7 @@
         <v>4858.3672377839066</v>
       </c>
     </row>
-    <row r="30" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -5008,7 +5238,7 @@
         <v>177423.62567881451</v>
       </c>
     </row>
-    <row r="31" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
@@ -5187,7 +5417,7 @@
         <v>26613.543851822174</v>
       </c>
     </row>
-    <row r="32" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
@@ -5620,7 +5850,7 @@
         <v>150810.08182699233</v>
       </c>
     </row>
-    <row r="33" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
@@ -5805,7 +6035,7 @@
         <v>14.375186524353477</v>
       </c>
     </row>
-    <row r="34" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
@@ -5955,7 +6185,7 @@
         <v>10491</v>
       </c>
     </row>
-    <row r="36" spans="2:78" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:78" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>38</v>
       </c>
@@ -6203,7 +6433,7 @@
         <v>0.10353840131598058</v>
       </c>
     </row>
-    <row r="37" spans="2:78" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:78" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>123</v>
       </c>
@@ -6279,7 +6509,7 @@
       <c r="BV37" s="15"/>
       <c r="BW37" s="15"/>
     </row>
-    <row r="38" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>100</v>
       </c>
@@ -6403,7 +6633,7 @@
       <c r="BV38" s="13"/>
       <c r="BW38" s="13"/>
     </row>
-    <row r="39" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>101</v>
       </c>
@@ -6527,7 +6757,7 @@
       <c r="BV39" s="13"/>
       <c r="BW39" s="13"/>
     </row>
-    <row r="40" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
@@ -6605,7 +6835,7 @@
       </c>
       <c r="AF40" s="8">
         <f>+AF11/AB11-1</f>
-        <v>-1</v>
+        <v>4.5802967941698469E-2</v>
       </c>
       <c r="AG40" s="8">
         <f t="shared" ref="AG40:AL40" si="172">+AG11/AC11-1</f>
@@ -6619,9 +6849,9 @@
         <f t="shared" si="172"/>
         <v>-1</v>
       </c>
-      <c r="AJ40" s="8" t="e">
+      <c r="AJ40" s="8">
         <f t="shared" si="172"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="AK40" s="8" t="e">
         <f t="shared" si="172"/>
@@ -6681,7 +6911,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>57</v>
       </c>
@@ -6759,7 +6989,7 @@
       </c>
       <c r="AF41" s="8">
         <f t="shared" si="178"/>
-        <v>-1</v>
+        <v>0.11966472844240994</v>
       </c>
       <c r="AG41" s="8">
         <f t="shared" si="178"/>
@@ -6773,9 +7003,9 @@
         <f t="shared" si="178"/>
         <v>-1</v>
       </c>
-      <c r="AJ41" s="8" t="e">
+      <c r="AJ41" s="8">
         <f t="shared" si="178"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="AK41" s="8" t="e">
         <f t="shared" si="178"/>
@@ -6835,7 +7065,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>58</v>
       </c>
@@ -6913,7 +7143,7 @@
       </c>
       <c r="AF42" s="8">
         <f t="shared" si="178"/>
-        <v>-1</v>
+        <v>9.824135839902981E-2</v>
       </c>
       <c r="AG42" s="8">
         <f t="shared" si="178"/>
@@ -6927,9 +7157,9 @@
         <f t="shared" si="178"/>
         <v>-1</v>
       </c>
-      <c r="AJ42" s="8" t="e">
+      <c r="AJ42" s="8">
         <f t="shared" si="178"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="AK42" s="8" t="e">
         <f t="shared" si="178"/>
@@ -6989,7 +7219,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>59</v>
       </c>
@@ -7067,7 +7297,7 @@
       </c>
       <c r="AF43" s="8">
         <f t="shared" si="178"/>
-        <v>-1</v>
+        <v>0.19545071609098574</v>
       </c>
       <c r="AG43" s="8">
         <f t="shared" si="178"/>
@@ -7081,9 +7311,9 @@
         <f t="shared" si="178"/>
         <v>-1</v>
       </c>
-      <c r="AJ43" s="8" t="e">
+      <c r="AJ43" s="8">
         <f t="shared" si="178"/>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="AK43" s="8" t="e">
         <f t="shared" si="178"/>
@@ -7143,7 +7373,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
@@ -7312,7 +7542,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:78" ht="13" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>29</v>
       </c>
@@ -7514,7 +7744,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="46" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:78" x14ac:dyDescent="0.25">
       <c r="BY46" t="s">
         <v>76</v>
       </c>
@@ -7522,7 +7752,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>75</v>
       </c>
@@ -7651,7 +7881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>4</v>
       </c>
@@ -7744,10 +7974,10 @@
       </c>
       <c r="BZ48" s="2">
         <f>NPV(BZ45,BP32:EG32)+Main!K5-Main!K6</f>
-        <v>1454245.3940996223</v>
-      </c>
-    </row>
-    <row r="49" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>1461008.3940996223</v>
+      </c>
+    </row>
+    <row r="49" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>63</v>
       </c>
@@ -7819,10 +8049,10 @@
       </c>
       <c r="BZ49" s="1">
         <f>+BZ48/Main!K3</f>
-        <v>139.74223695214539</v>
-      </c>
-    </row>
-    <row r="50" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>136.44082873548956</v>
+      </c>
+    </row>
+    <row r="50" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>64</v>
       </c>
@@ -7893,7 +8123,7 @@
         <v>50106</v>
       </c>
     </row>
-    <row r="51" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>65</v>
       </c>
@@ -7964,7 +8194,7 @@
         <v>220717</v>
       </c>
     </row>
-    <row r="52" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>66</v>
       </c>
@@ -8035,7 +8265,7 @@
         <v>74575</v>
       </c>
     </row>
-    <row r="53" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>67</v>
       </c>
@@ -8107,7 +8337,7 @@
         <v>22879</v>
       </c>
     </row>
-    <row r="54" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>68</v>
       </c>
@@ -8178,7 +8408,7 @@
         <v>63340</v>
       </c>
     </row>
-    <row r="55" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>62</v>
       </c>
@@ -8267,7 +8497,7 @@
         <v>554818</v>
       </c>
     </row>
-    <row r="57" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>71</v>
       </c>
@@ -8338,7 +8568,7 @@
         <v>81817</v>
       </c>
     </row>
-    <row r="58" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>72</v>
       </c>
@@ -8409,7 +8639,7 @@
         <v>60351</v>
       </c>
     </row>
-    <row r="59" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>73</v>
       </c>
@@ -8480,7 +8710,7 @@
         <v>16004</v>
       </c>
     </row>
-    <row r="60" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>66</v>
       </c>
@@ -8551,7 +8781,7 @@
         <v>78084</v>
       </c>
     </row>
-    <row r="61" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
@@ -8622,7 +8852,7 @@
         <v>54889</v>
       </c>
     </row>
-    <row r="62" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>74</v>
       </c>
@@ -8693,7 +8923,7 @@
         <v>27226</v>
       </c>
     </row>
-    <row r="63" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>70</v>
       </c>
@@ -8764,7 +8994,7 @@
         <v>236447</v>
       </c>
     </row>
-    <row r="64" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>69</v>
       </c>
@@ -8853,7 +9083,7 @@
         <v>554818</v>
       </c>
     </row>
-    <row r="66" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>84</v>
       </c>
@@ -8938,11 +9168,11 @@
         <v>10431</v>
       </c>
       <c r="AF66" s="4">
-        <f t="shared" si="233"/>
+        <f>+AF32</f>
         <v>13486</v>
       </c>
     </row>
-    <row r="67" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>85</v>
       </c>
@@ -9013,7 +9243,7 @@
         <v>13485</v>
       </c>
     </row>
-    <row r="68" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>88</v>
       </c>
@@ -9084,7 +9314,7 @@
         <v>12038</v>
       </c>
     </row>
-    <row r="69" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>89</v>
       </c>
@@ -9155,7 +9385,7 @@
         <v>6722</v>
       </c>
     </row>
-    <row r="70" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>45</v>
       </c>
@@ -9226,7 +9456,7 @@
         <v>-95</v>
       </c>
     </row>
-    <row r="71" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>45</v>
       </c>
@@ -9291,7 +9521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>90</v>
       </c>
@@ -9362,7 +9592,7 @@
         <v>-785</v>
       </c>
     </row>
-    <row r="73" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>87</v>
       </c>
@@ -9451,7 +9681,7 @@
         <v>-6084</v>
       </c>
     </row>
-    <row r="74" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>86</v>
       </c>
@@ -9549,7 +9779,7 @@
         <v>392.02199999999999</v>
       </c>
     </row>
-    <row r="75" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -9575,7 +9805,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>91</v>
       </c>
@@ -9646,7 +9876,7 @@
         <v>-17620</v>
       </c>
     </row>
-    <row r="77" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>93</v>
       </c>
@@ -9717,7 +9947,7 @@
         <v>1227</v>
       </c>
     </row>
-    <row r="78" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>94</v>
       </c>
@@ -9788,7 +10018,7 @@
         <v>-571</v>
       </c>
     </row>
-    <row r="79" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>95</v>
       </c>
@@ -9877,7 +10107,7 @@
         <v>-5174</v>
       </c>
     </row>
-    <row r="80" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>92</v>
       </c>
@@ -9966,7 +10196,7 @@
         <v>-22138</v>
       </c>
     </row>
-    <row r="81" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -9992,7 +10222,7 @@
       <c r="Y81" s="4"/>
       <c r="Z81" s="4"/>
     </row>
-    <row r="82" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>97</v>
       </c>
@@ -10063,7 +10293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>5</v>
       </c>
@@ -10152,7 +10382,7 @@
         <v>-4490</v>
       </c>
     </row>
-    <row r="84" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>96</v>
       </c>
@@ -10241,7 +10471,7 @@
         <v>-4490</v>
       </c>
     </row>
-    <row r="85" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>98</v>
       </c>
@@ -10312,7 +10542,7 @@
         <v>-312</v>
       </c>
     </row>
-    <row r="86" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>99</v>
       </c>
@@ -10401,7 +10631,7 @@
         <v>-1659</v>
       </c>
     </row>
-    <row r="88" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>46</v>
       </c>
@@ -10485,7 +10715,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="90" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>81</v>
       </c>
@@ -10558,7 +10788,7 @@
         <v>5065</v>
       </c>
     </row>
-    <row r="91" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>82</v>
       </c>
@@ -10631,7 +10861,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="92" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>83</v>
       </c>
@@ -10704,7 +10934,7 @@
         <v>9334</v>
       </c>
     </row>
-    <row r="94" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>102</v>
       </c>
@@ -10781,7 +11011,7 @@
         <v>8888</v>
       </c>
     </row>
-    <row r="95" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>107</v>
       </c>
@@ -10846,7 +11076,7 @@
         <v>52973</v>
       </c>
     </row>
-    <row r="101" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>105</v>
       </c>

</xml_diff>

<commit_message>
added NVDA quarterly preview
</commit_message>
<xml_diff>
--- a/AMZN.xlsx
+++ b/AMZN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Shkreli - DL\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3D183C-1260-4D04-9DEC-5FEE6ACED470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEA922-7441-4798-80BF-D67F47BA4D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32100" yWindow="1725" windowWidth="30735" windowHeight="17835" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
+    <workbookView xWindow="9050" yWindow="4000" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{319C79D3-530A-422D-B7D4-1569BBD88715}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1227,16 +1227,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E919ED4-9952-4C3B-8FDF-EC99BCC4C526}">
   <dimension ref="B2:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J2" t="s">
         <v>1</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>236.13</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
         <v>2</v>
       </c>
@@ -1255,7 +1255,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>103</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>2482909.54931904</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>106</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>104</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>6</v>
       </c>
@@ -1305,20 +1305,20 @@
       </c>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>124</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>125</v>
       </c>
@@ -1334,12 +1334,12 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>135</v>
       </c>
@@ -1347,27 +1347,27 @@
         <v>142</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>143</v>
       </c>
@@ -1375,72 +1375,72 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>149</v>
       </c>
@@ -1454,27 +1454,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5282D4FF-6525-4291-9B79-B00D62C08099}">
   <dimension ref="A1:EG101"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AA36" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AA71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AG48" sqref="AG48"/>
+      <selection pane="bottomRight" activeCell="AD76" sqref="AD76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="26" width="9.140625" style="3"/>
-    <col min="74" max="75" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="3" max="26" width="9.1796875" style="3"/>
+    <col min="74" max="75" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>116</v>
       </c>
@@ -1762,7 +1762,7 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="3" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
@@ -1873,7 +1873,7 @@
         <v>279833</v>
       </c>
     </row>
-    <row r="4" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>60</v>
       </c>
@@ -1911,7 +1911,7 @@
         <v>13580</v>
       </c>
     </row>
-    <row r="5" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>61</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>64887</v>
       </c>
     </row>
-    <row r="6" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>127787</v>
       </c>
     </row>
-    <row r="7" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>60</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>10631</v>
       </c>
     </row>
-    <row r="8" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>33107</v>
       </c>
     </row>
-    <row r="9" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>447916.72498560004</v>
       </c>
     </row>
-    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>40</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>326267.1892021501</v>
       </c>
     </row>
-    <row r="12" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
@@ -2563,7 +2563,7 @@
         <v>28184.221465804694</v>
       </c>
     </row>
-    <row r="13" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>197068.63549427583</v>
       </c>
     </row>
-    <row r="14" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>68149.380161362526</v>
       </c>
     </row>
-    <row r="15" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>44</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>79499.983233825042</v>
       </c>
     </row>
-    <row r="16" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>45</v>
       </c>
@@ -3101,11 +3101,11 @@
         <v>6976.4038955296901</v>
       </c>
     </row>
-    <row r="17" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:137" x14ac:dyDescent="0.25">
       <c r="BO17" s="2"/>
       <c r="BP17" s="2"/>
     </row>
-    <row r="18" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>20</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>241787</v>
       </c>
     </row>
-    <row r="19" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>21</v>
       </c>
@@ -3317,7 +3317,7 @@
         <v>228035</v>
       </c>
     </row>
-    <row r="20" spans="2:137" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:137" s="5" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>8</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>1154062.5384385479</v>
       </c>
     </row>
-    <row r="21" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>754757.74441970466</v>
       </c>
     </row>
-    <row r="22" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>52333.582469642599</v>
       </c>
     </row>
-    <row r="23" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
@@ -4070,7 +4070,7 @@
         <v>346971.21154920058</v>
       </c>
     </row>
-    <row r="24" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
@@ -4226,7 +4226,7 @@
         <v>105304.26010540825</v>
       </c>
     </row>
-    <row r="25" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
@@ -4382,7 +4382,7 @@
         <v>54569.503408901481</v>
       </c>
     </row>
-    <row r="26" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>14532.189593860268</v>
       </c>
     </row>
-    <row r="27" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
@@ -4727,7 +4727,7 @@
         <v>174405.95310816998</v>
       </c>
     </row>
-    <row r="28" spans="2:137" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:137" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>172565.2584410306</v>
       </c>
     </row>
-    <row r="29" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>31</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>4858.3672377839066</v>
       </c>
     </row>
-    <row r="30" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>177423.62567881451</v>
       </c>
     </row>
-    <row r="31" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
@@ -5473,7 +5473,7 @@
         <v>26613.543851822174</v>
       </c>
     </row>
-    <row r="32" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:137" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>150810.08182699233</v>
       </c>
     </row>
-    <row r="33" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>14.375186524353477</v>
       </c>
     </row>
-    <row r="34" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>2</v>
       </c>
@@ -6249,7 +6249,7 @@
         <v>10491</v>
       </c>
     </row>
-    <row r="36" spans="2:78" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:78" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B36" s="5" t="s">
         <v>38</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>0.10353840131598058</v>
       </c>
     </row>
-    <row r="37" spans="2:78" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:78" s="11" customFormat="1" ht="13" x14ac:dyDescent="0.3">
       <c r="B37" s="5" t="s">
         <v>123</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="BV37" s="15"/>
       <c r="BW37" s="15"/>
     </row>
-    <row r="38" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
         <v>100</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="BV38" s="13"/>
       <c r="BW38" s="13"/>
     </row>
-    <row r="39" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
         <v>101</v>
       </c>
@@ -6831,7 +6831,7 @@
       <c r="BV39" s="13"/>
       <c r="BW39" s="13"/>
     </row>
-    <row r="40" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
         <v>56</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="41" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
         <v>57</v>
       </c>
@@ -7139,7 +7139,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
         <v>58</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>59</v>
       </c>
@@ -7447,7 +7447,7 @@
         <v>5.0000000000000044E-2</v>
       </c>
     </row>
-    <row r="44" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
         <v>39</v>
       </c>
@@ -7616,7 +7616,7 @@
         <v>0.19999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:78" ht="13" x14ac:dyDescent="0.3">
       <c r="B45" s="2" t="s">
         <v>29</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="46" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:78" x14ac:dyDescent="0.25">
       <c r="BY46" t="s">
         <v>76</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="47" spans="2:78" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:78" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
         <v>75</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
         <v>4</v>
       </c>
@@ -8058,7 +8058,7 @@
         <v>1459966.3940996223</v>
       </c>
     </row>
-    <row r="49" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>63</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>138.84592160567925</v>
       </c>
     </row>
-    <row r="50" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
         <v>64</v>
       </c>
@@ -8210,7 +8210,7 @@
         <v>51638</v>
       </c>
     </row>
-    <row r="51" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
         <v>65</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>237917</v>
       </c>
     </row>
-    <row r="52" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
         <v>66</v>
       </c>
@@ -8358,7 +8358,7 @@
         <v>76527</v>
       </c>
     </row>
-    <row r="53" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
         <v>67</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>23081</v>
       </c>
     </row>
-    <row r="54" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
         <v>68</v>
       </c>
@@ -8507,7 +8507,7 @@
         <v>71309</v>
       </c>
     </row>
-    <row r="55" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
         <v>62</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>584626</v>
       </c>
     </row>
-    <row r="57" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
         <v>71</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>84570</v>
       </c>
     </row>
-    <row r="58" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
         <v>72</v>
       </c>
@@ -8748,7 +8748,7 @@
         <v>60602</v>
       </c>
     </row>
-    <row r="59" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
         <v>73</v>
       </c>
@@ -8822,7 +8822,7 @@
         <v>16305</v>
       </c>
     </row>
-    <row r="60" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
         <v>66</v>
       </c>
@@ -8896,7 +8896,7 @@
         <v>79802</v>
       </c>
     </row>
-    <row r="61" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
         <v>5</v>
       </c>
@@ -8970,7 +8970,7 @@
         <v>54890</v>
       </c>
     </row>
-    <row r="62" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
         <v>74</v>
       </c>
@@ -9044,7 +9044,7 @@
         <v>29306</v>
       </c>
     </row>
-    <row r="63" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
         <v>70</v>
       </c>
@@ -9118,7 +9118,7 @@
         <v>259151</v>
       </c>
     </row>
-    <row r="64" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:78" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
         <v>69</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>584626</v>
       </c>
     </row>
-    <row r="66" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
         <v>84</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>12940</v>
       </c>
     </row>
-    <row r="67" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
         <v>85</v>
       </c>
@@ -9378,7 +9378,7 @@
         <v>15328</v>
       </c>
     </row>
-    <row r="68" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
         <v>88</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>13442</v>
       </c>
     </row>
-    <row r="69" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
         <v>89</v>
       </c>
@@ -9526,7 +9526,7 @@
         <v>5333</v>
       </c>
     </row>
-    <row r="70" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
         <v>45</v>
       </c>
@@ -9600,7 +9600,7 @@
         <v>-141</v>
       </c>
     </row>
-    <row r="71" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
         <v>45</v>
       </c>
@@ -9665,7 +9665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
         <v>90</v>
       </c>
@@ -9739,7 +9739,7 @@
         <v>-1317</v>
       </c>
     </row>
-    <row r="73" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
         <v>87</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>-6674</v>
       </c>
     </row>
-    <row r="74" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
         <v>86</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>392.02199999999999</v>
       </c>
     </row>
-    <row r="75" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -9960,7 +9960,7 @@
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
     </row>
-    <row r="76" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>91</v>
       </c>
@@ -10033,8 +10033,11 @@
       <c r="AG76" s="2">
         <v>-22620</v>
       </c>
-    </row>
-    <row r="77" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AH76" s="2">
+        <v>-27834</v>
+      </c>
+    </row>
+    <row r="77" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
         <v>93</v>
       </c>
@@ -10108,7 +10111,7 @@
         <v>1342</v>
       </c>
     </row>
-    <row r="78" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
         <v>94</v>
       </c>
@@ -10182,7 +10185,7 @@
         <v>-622</v>
       </c>
     </row>
-    <row r="79" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
         <v>95</v>
       </c>
@@ -10275,7 +10278,7 @@
         <v>5001</v>
       </c>
     </row>
-    <row r="80" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:48" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
         <v>92</v>
       </c>
@@ -10368,7 +10371,7 @@
         <v>-16899</v>
       </c>
     </row>
-    <row r="81" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -10394,7 +10397,7 @@
       <c r="Y81" s="4"/>
       <c r="Z81" s="4"/>
     </row>
-    <row r="82" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>97</v>
       </c>
@@ -10468,7 +10471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>5</v>
       </c>
@@ -10561,7 +10564,7 @@
         <v>-2758</v>
       </c>
     </row>
-    <row r="84" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
         <v>96</v>
       </c>
@@ -10654,7 +10657,7 @@
         <v>-2758</v>
       </c>
     </row>
-    <row r="85" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
         <v>98</v>
       </c>
@@ -10728,7 +10731,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="86" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
         <v>99</v>
       </c>
@@ -10821,7 +10824,7 @@
         <v>7004</v>
       </c>
     </row>
-    <row r="88" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
         <v>46</v>
       </c>
@@ -10908,7 +10911,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="90" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
         <v>81</v>
       </c>
@@ -10984,7 +10987,7 @@
         <v>5663</v>
       </c>
     </row>
-    <row r="91" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
         <v>82</v>
       </c>
@@ -11060,7 +11063,7 @@
         <v>1301</v>
       </c>
     </row>
-    <row r="92" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
         <v>83</v>
       </c>
@@ -11136,7 +11139,7 @@
         <v>10447</v>
       </c>
     </row>
-    <row r="94" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
         <v>102</v>
       </c>
@@ -11217,7 +11220,7 @@
         <v>4693</v>
       </c>
     </row>
-    <row r="95" spans="2:43" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
         <v>107</v>
       </c>
@@ -11286,7 +11289,7 @@
         <v>47747</v>
       </c>
     </row>
-    <row r="101" spans="2:44" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:44" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>105</v>
       </c>

</xml_diff>